<commit_message>
working dictionary for mort and vacc
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-survey-dict.xlsx
+++ b/inst/extdata/MSF-survey-dict.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Mortality" sheetId="11" r:id="rId1"/>
@@ -17,7 +17,10 @@
     <sheet name="Mortality_settings" sheetId="13" r:id="rId3"/>
     <sheet name="Mortality_OLD" sheetId="7" r:id="rId4"/>
     <sheet name="Nutrition" sheetId="8" r:id="rId5"/>
-    <sheet name="Vaccination" sheetId="10" r:id="rId6"/>
+    <sheet name="Vaccination" sheetId="14" r:id="rId6"/>
+    <sheet name="Vaccination_choices" sheetId="15" r:id="rId7"/>
+    <sheet name="Vaccination_settings" sheetId="16" r:id="rId8"/>
+    <sheet name="Vaccination_OLD" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1497" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2070" uniqueCount="836">
   <si>
     <t>level</t>
   </si>
@@ -1859,13 +1862,695 @@
   </si>
   <si>
     <t>id_string</t>
+  </si>
+  <si>
+    <t>${diagnosis_disease}='yes'</t>
+  </si>
+  <si>
+    <t>Age de l'enfant lorsqu'il a eu la rougeole (en mois)</t>
+  </si>
+  <si>
+    <t>Age of child when they had measles (months)</t>
+  </si>
+  <si>
+    <t>age_diagnosis</t>
+  </si>
+  <si>
+    <t>L'enfant a-t-il déjà eu la rougeole?</t>
+  </si>
+  <si>
+    <t>Did the child previously have measles?</t>
+  </si>
+  <si>
+    <t>diagnosis_disease</t>
+  </si>
+  <si>
+    <t>select_one yndk</t>
+  </si>
+  <si>
+    <t>${consent}='yes' and ${child_number} &gt;0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Antécédents de rougeole</t>
+  </si>
+  <si>
+    <t>Previous diagnosis</t>
+  </si>
+  <si>
+    <t>g9</t>
+  </si>
+  <si>
+    <t>${reason_sia_vacc}='other'</t>
+  </si>
+  <si>
+    <t>Veuillez spécifier la raison</t>
+  </si>
+  <si>
+    <t>Specify other reason</t>
+  </si>
+  <si>
+    <t>reason_sia_other</t>
+  </si>
+  <si>
+    <t>${sia_vacc} = 'no'</t>
+  </si>
+  <si>
+    <t>Raison pour ne pas avoir pris la vaccination d'avs</t>
+  </si>
+  <si>
+    <t>Reason for non SIA vaccination</t>
+  </si>
+  <si>
+    <t>reason_sia_vacc</t>
+  </si>
+  <si>
+    <t>select_one reason_msf</t>
+  </si>
+  <si>
+    <t>${sia_vacc} = 'verbal' or ${sia_vacc} = 'card'</t>
+  </si>
+  <si>
+    <t>Endroit de l'activité de vaccination supplémentaire</t>
+  </si>
+  <si>
+    <t>Place of SIA vaccination</t>
+  </si>
+  <si>
+    <t>place_sia_vacc</t>
+  </si>
+  <si>
+    <t>Âge de l'enfant au moment de la vaccination (en mois)</t>
+  </si>
+  <si>
+    <t>Age of child at the time of vaccination (months)</t>
+  </si>
+  <si>
+    <t>age_sia_vacc</t>
+  </si>
+  <si>
+    <t>AVS - 6 mois à 9 ans</t>
+  </si>
+  <si>
+    <t>Immunisation SIA/NID - 6 months to 9 years</t>
+  </si>
+  <si>
+    <t>sia_vacc</t>
+  </si>
+  <si>
+    <t>select_one vaccination</t>
+  </si>
+  <si>
+    <t>Activités de vaccination supplémentaire</t>
+  </si>
+  <si>
+    <t>Immunisation SIA/NID</t>
+  </si>
+  <si>
+    <t>g8</t>
+  </si>
+  <si>
+    <t>${reason_msf_vacc}='other'</t>
+  </si>
+  <si>
+    <t>reason_msf_other</t>
+  </si>
+  <si>
+    <t>${msf_vacc} = 'no'</t>
+  </si>
+  <si>
+    <t>Raison pour ne pas avoir pris la vaccination de MSF</t>
+  </si>
+  <si>
+    <t>Reason for non MSF vaccination</t>
+  </si>
+  <si>
+    <t>reason_msf_vacc</t>
+  </si>
+  <si>
+    <t>${msf_vacc} = 'verbal' or ${msf_vacc} = 'card'</t>
+  </si>
+  <si>
+    <t>Endroit de la vaccination de MSF</t>
+  </si>
+  <si>
+    <t>Place of MSF vaccination</t>
+  </si>
+  <si>
+    <t>place_msf_vacc</t>
+  </si>
+  <si>
+    <t>select_one place_msf</t>
+  </si>
+  <si>
+    <t>age_msf_vacc</t>
+  </si>
+  <si>
+    <t>Campagne de vaccination de MSF - 6 mois à 9 ans</t>
+  </si>
+  <si>
+    <t>MSF Vaccination Campaign - 6 months to 9 years</t>
+  </si>
+  <si>
+    <t>msf_vacc</t>
+  </si>
+  <si>
+    <t>Vaccination de MSF</t>
+  </si>
+  <si>
+    <t>MSF vaccination</t>
+  </si>
+  <si>
+    <t>g7</t>
+  </si>
+  <si>
+    <t>${reason_route_vacc}='other'</t>
+  </si>
+  <si>
+    <t>reason_route_other</t>
+  </si>
+  <si>
+    <t>${routine_vacc} = 'no'</t>
+  </si>
+  <si>
+    <t>Raison pour ne pas avoir pris la vaccination de routine</t>
+  </si>
+  <si>
+    <t>Reason for non routine vaccination</t>
+  </si>
+  <si>
+    <t>reason_route_vacc</t>
+  </si>
+  <si>
+    <t>select_one reason_routine</t>
+  </si>
+  <si>
+    <t>${routine_vacc} = 'verbal' or ${routine_vacc} = 'card'</t>
+  </si>
+  <si>
+    <t>Endroit de la vaccination de routine</t>
+  </si>
+  <si>
+    <t>Place of routine vaccination</t>
+  </si>
+  <si>
+    <t>place_routine_vacc</t>
+  </si>
+  <si>
+    <t>select_one place_routine</t>
+  </si>
+  <si>
+    <t>age_routine_vacc</t>
+  </si>
+  <si>
+    <t>Vaccination de routine - Vaccin de 9 mois</t>
+  </si>
+  <si>
+    <t>Routine Vaccination - 9 months vaccine</t>
+  </si>
+  <si>
+    <t>routine_vacc</t>
+  </si>
+  <si>
+    <t>Vaccination de routine</t>
+  </si>
+  <si>
+    <t>Routine vaccination</t>
+  </si>
+  <si>
+    <t>g6</t>
+  </si>
+  <si>
+    <t>.&lt;12</t>
+  </si>
+  <si>
+    <t>Si l'enfant a mois d'un an, indiquez l'âge en mois</t>
+  </si>
+  <si>
+    <t>.&lt;=15</t>
+  </si>
+  <si>
+    <t>Saisissez 0 pour un âge compris entre 0 et 11 mois, et le nombre d'années pour un an ou plus</t>
+  </si>
+  <si>
+    <t>Age d'enfant en années</t>
+  </si>
+  <si>
+    <t>Numéro d'enfant</t>
+  </si>
+  <si>
+    <t>Child number</t>
+  </si>
+  <si>
+    <t>child_number</t>
+  </si>
+  <si>
+    <t>Information sur les enfants</t>
+  </si>
+  <si>
+    <t>Child Demographics</t>
+  </si>
+  <si>
+    <t>g5</t>
+  </si>
+  <si>
+    <t>${children_count}</t>
+  </si>
+  <si>
+    <t>Combien d'enfants âgés de 6 mois à 9 ans se trouvent dans le ménage ?</t>
+  </si>
+  <si>
+    <t>How many children between 6 months and 9 years are in the household?</t>
+  </si>
+  <si>
+    <t>children_count</t>
+  </si>
+  <si>
+    <t>Nombre d'enfants</t>
+  </si>
+  <si>
+    <t>Children count</t>
+  </si>
+  <si>
+    <t>Pouvez-vous me faire savoir pourquoi vous ne voulez pas participer ?</t>
+  </si>
+  <si>
+    <t>Quel âge a la personne responsable d'enfants?</t>
+  </si>
+  <si>
+    <t>How old is the caretaker?</t>
+  </si>
+  <si>
+    <t>age_caretaker</t>
+  </si>
+  <si>
+    <t>${caretaker} = 'other'</t>
+  </si>
+  <si>
+    <t>Veuillez spécifier la personne responsable d'enfants</t>
+  </si>
+  <si>
+    <t>Other caretaker, please specify</t>
+  </si>
+  <si>
+    <t>other_caretaker</t>
+  </si>
+  <si>
+    <t>Qui est la personne responsable d'enfants ?</t>
+  </si>
+  <si>
+    <t>Who is the main caretaker?</t>
+  </si>
+  <si>
+    <t>caretaker</t>
+  </si>
+  <si>
+    <t>select_one caretaker</t>
+  </si>
+  <si>
+    <t>Consentement verbal donné par le participant ?</t>
+  </si>
+  <si>
+    <t>Verbal consent given by participant?</t>
+  </si>
+  <si>
+    <t>Si &gt;1 ménage dans le bâtiment/l'endroit clotûré, donnez un numéro à chaque ménage.</t>
+  </si>
+  <si>
+    <t>Combien de ménages se trouvent dans le batîment/l'endroit clotûré?</t>
+  </si>
+  <si>
+    <t>Veuillez spécifier le nom du village</t>
+  </si>
+  <si>
+    <t>Numéro de l'équipe</t>
+  </si>
+  <si>
+    <t>Place routine8</t>
+  </si>
+  <si>
+    <t>place_routine8</t>
+  </si>
+  <si>
+    <t>place_routine</t>
+  </si>
+  <si>
+    <t>Place routine7</t>
+  </si>
+  <si>
+    <t>place_routine7</t>
+  </si>
+  <si>
+    <t>Place routine6</t>
+  </si>
+  <si>
+    <t>place_routine6</t>
+  </si>
+  <si>
+    <t>Place routine5</t>
+  </si>
+  <si>
+    <t>place_routine5</t>
+  </si>
+  <si>
+    <t>Place routine4</t>
+  </si>
+  <si>
+    <t>place_routine4</t>
+  </si>
+  <si>
+    <t>Place routine3</t>
+  </si>
+  <si>
+    <t>place_routine3</t>
+  </si>
+  <si>
+    <t>Place routine2</t>
+  </si>
+  <si>
+    <t>place_routine2</t>
+  </si>
+  <si>
+    <t>Place routine1</t>
+  </si>
+  <si>
+    <t>place_routine1</t>
+  </si>
+  <si>
+    <t>Place MSF9</t>
+  </si>
+  <si>
+    <t>place_msf9</t>
+  </si>
+  <si>
+    <t>place_msf</t>
+  </si>
+  <si>
+    <t>Place MSF8</t>
+  </si>
+  <si>
+    <t>place_msf8</t>
+  </si>
+  <si>
+    <t>Place MSF7</t>
+  </si>
+  <si>
+    <t>place_msf7</t>
+  </si>
+  <si>
+    <t>Place MSF6</t>
+  </si>
+  <si>
+    <t>place_msf6</t>
+  </si>
+  <si>
+    <t>Place MSF5</t>
+  </si>
+  <si>
+    <t>place_msf5</t>
+  </si>
+  <si>
+    <t>Place MSF4</t>
+  </si>
+  <si>
+    <t>place_msf4</t>
+  </si>
+  <si>
+    <t>Place MSF3</t>
+  </si>
+  <si>
+    <t>place_msf3</t>
+  </si>
+  <si>
+    <t>Place MSF2</t>
+  </si>
+  <si>
+    <t>place_msf2</t>
+  </si>
+  <si>
+    <t>Place MSF1</t>
+  </si>
+  <si>
+    <t>place_msf1</t>
+  </si>
+  <si>
+    <t>Soeur</t>
+  </si>
+  <si>
+    <t>sister</t>
+  </si>
+  <si>
+    <t>Frère</t>
+  </si>
+  <si>
+    <t>brother</t>
+  </si>
+  <si>
+    <t>Oncle</t>
+  </si>
+  <si>
+    <t>uncle</t>
+  </si>
+  <si>
+    <t>Tante</t>
+  </si>
+  <si>
+    <t>aunt</t>
+  </si>
+  <si>
+    <t>Grand-père</t>
+  </si>
+  <si>
+    <t>grandfather</t>
+  </si>
+  <si>
+    <t>Grand-mère</t>
+  </si>
+  <si>
+    <t>grandmother</t>
+  </si>
+  <si>
+    <t>Père</t>
+  </si>
+  <si>
+    <t>father</t>
+  </si>
+  <si>
+    <t>Mère</t>
+  </si>
+  <si>
+    <t>mother</t>
+  </si>
+  <si>
+    <t>Pas de réponse</t>
+  </si>
+  <si>
+    <t>no_answer</t>
+  </si>
+  <si>
+    <t>yndk</t>
+  </si>
+  <si>
+    <t>Autre raison</t>
+  </si>
+  <si>
+    <t>other_msf</t>
+  </si>
+  <si>
+    <t>reason_msf</t>
+  </si>
+  <si>
+    <t>Pas assez de vaccin sur le lieu de vaccination</t>
+  </si>
+  <si>
+    <t>no_vaccine</t>
+  </si>
+  <si>
+    <t>Le vaccinateur a décidé de ne pas vacciner l'enfant</t>
+  </si>
+  <si>
+    <t>Vaccinator decided not to vaccinate the child</t>
+  </si>
+  <si>
+    <t>vaccinator_refused</t>
+  </si>
+  <si>
+    <t>Un enfant a été malade lors d'une campagne de vaccination</t>
+  </si>
+  <si>
+    <t>Child was sick during vaccination campaign</t>
+  </si>
+  <si>
+    <t>child_sick</t>
+  </si>
+  <si>
+    <t>La famille était à l'extérieur du village pendant la campagne</t>
+  </si>
+  <si>
+    <t>family_away</t>
+  </si>
+  <si>
+    <t>La campagne a eu lieu dimanche</t>
+  </si>
+  <si>
+    <t>Campaign took place on Sunday</t>
+  </si>
+  <si>
+    <t>timing</t>
+  </si>
+  <si>
+    <t>Il/elle travaillait pendant la campagne</t>
+  </si>
+  <si>
+    <t>S/he was working during the campaign</t>
+  </si>
+  <si>
+    <t>working</t>
+  </si>
+  <si>
+    <t>Lieu de vaccination trop éloigné/trop cher</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>N'était pas au courant de la campagne de vaccination</t>
+  </si>
+  <si>
+    <t>Did not know about vaccination campaign</t>
+  </si>
+  <si>
+    <t>unaware_campaign</t>
+  </si>
+  <si>
+    <t>Ne savait pas qu'il pouvait vacciner l'enfant</t>
+  </si>
+  <si>
+    <t>Did not know that s/he could vaccinate the child</t>
+  </si>
+  <si>
+    <t>unaware_eligible</t>
+  </si>
+  <si>
+    <t>other_routine</t>
+  </si>
+  <si>
+    <t>reason_routine</t>
+  </si>
+  <si>
+    <t>L'enfant a déjà été vacciné</t>
+  </si>
+  <si>
+    <t>already_vaccinated</t>
+  </si>
+  <si>
+    <t>L'enfant était trop vieux</t>
+  </si>
+  <si>
+    <t>child_old</t>
+  </si>
+  <si>
+    <t>L'enfant était trop jeune</t>
+  </si>
+  <si>
+    <t>child_young</t>
+  </si>
+  <si>
+    <t>Croyances religieuses</t>
+  </si>
+  <si>
+    <t>religious_beliefs</t>
+  </si>
+  <si>
+    <t>Le père n'a pas permis à la mère de vacciner l'enfant</t>
+  </si>
+  <si>
+    <t>father_refused</t>
+  </si>
+  <si>
+    <t>La vaccination est douloureuse pour l'enfant</t>
+  </si>
+  <si>
+    <t>painful</t>
+  </si>
+  <si>
+    <t>Les vaccins ne sont pas bénéfiques</t>
+  </si>
+  <si>
+    <t>Vaccines are not beneficial</t>
+  </si>
+  <si>
+    <t>not_beneficial</t>
+  </si>
+  <si>
+    <t>Mauvaise expérience antérieure en matière de vaccination</t>
+  </si>
+  <si>
+    <t>bad_experience</t>
+  </si>
+  <si>
+    <t>Les vaccins sont dangereux pour les enfants</t>
+  </si>
+  <si>
+    <t>Vaccines dangerous for the child</t>
+  </si>
+  <si>
+    <t>dangerous</t>
+  </si>
+  <si>
+    <t>vaccination</t>
+  </si>
+  <si>
+    <t>Oui, avec carte</t>
+  </si>
+  <si>
+    <t>Yes, card</t>
+  </si>
+  <si>
+    <t>card</t>
+  </si>
+  <si>
+    <t>Oui, verbal</t>
+  </si>
+  <si>
+    <t>Yes, verbal</t>
+  </si>
+  <si>
+    <t>verbal</t>
+  </si>
+  <si>
+    <t>Femme</t>
+  </si>
+  <si>
+    <t>Homme</t>
+  </si>
+  <si>
+    <t>Il n'y a aucun avantage pour moi et ma famille</t>
+  </si>
+  <si>
+    <t>J'ai eu une expérience négative lors d'une précédente enquête</t>
+  </si>
+  <si>
+    <t>Je n'ai pas du temps</t>
+  </si>
+  <si>
+    <t>autre</t>
+  </si>
+  <si>
+    <t>vp4xBmVjJ7cMEAwbm4nAPv</t>
+  </si>
+  <si>
+    <t>concat(${cluster_number},'_',${household_number}, '_',${date})</t>
+  </si>
+  <si>
+    <t>vaccine_coverage_survey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1888,6 +2573,18 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1965,7 +2662,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2010,6 +2707,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2320,8 +3035,8 @@
   </sheetPr>
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4031,8 +4746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6095,6 +6810,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="C120:C123"/>
+    <mergeCell ref="C125:C127"/>
+    <mergeCell ref="C90:C92"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="C100:C109"/>
+    <mergeCell ref="C111:C116"/>
+    <mergeCell ref="C65:C70"/>
+    <mergeCell ref="C74:C78"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="B120:B123"/>
+    <mergeCell ref="B125:B127"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="C34:C42"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:C54"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="B90:B92"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="B100:B109"/>
+    <mergeCell ref="B111:B116"/>
+    <mergeCell ref="B65:B70"/>
+    <mergeCell ref="B74:B78"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="B87:B88"/>
     <mergeCell ref="A2:A19"/>
     <mergeCell ref="A20:A129"/>
     <mergeCell ref="B7:B8"/>
@@ -6111,44 +6864,6 @@
     <mergeCell ref="B46:B54"/>
     <mergeCell ref="B56:B59"/>
     <mergeCell ref="B62:B64"/>
-    <mergeCell ref="B65:B70"/>
-    <mergeCell ref="B74:B78"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="B90:B92"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="B100:B109"/>
-    <mergeCell ref="B111:B116"/>
-    <mergeCell ref="B120:B123"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="C34:C42"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:C54"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="C65:C70"/>
-    <mergeCell ref="C74:C78"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="C120:C123"/>
-    <mergeCell ref="C125:C127"/>
-    <mergeCell ref="C90:C92"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="C100:C109"/>
-    <mergeCell ref="C111:C116"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6701,6 +7416,2196 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:L63"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.42578125" style="9" customWidth="1"/>
+    <col min="5" max="6" width="28.85546875" style="18" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>519</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>517</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>516</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>514</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>513</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>512</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>510</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>511</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>508</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>508</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>507</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>504</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>504</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>503</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>501</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>500</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>499</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>497</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>497</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>493</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>486</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>483</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>714</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="12" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>476</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>713</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>473</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>712</v>
+      </c>
+      <c r="G15" s="23"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="12" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="12" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="L16" s="12" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="12" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>467</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>465</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+    </row>
+    <row r="18" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
+        <v>334</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>460</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>711</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>710</v>
+      </c>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+    </row>
+    <row r="21" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
+        <v>709</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>708</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>707</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>706</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+    </row>
+    <row r="22" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>705</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>704</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>703</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="H22" s="20" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>701</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>700</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>699</v>
+      </c>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+    </row>
+    <row r="24" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>698</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="H24" s="10" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="H25" s="10" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>697</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>696</v>
+      </c>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="H27" s="10" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>695</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>694</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>693</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="I28" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="30" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>440</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="J30" s="10" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>690</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>689</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="H31" s="10" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>688</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>687</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="K32" s="10" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+    </row>
+    <row r="34" spans="1:11" s="11" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>685</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>430</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>684</v>
+      </c>
+      <c r="K34" s="10" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>682</v>
+      </c>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="H35" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+    </row>
+    <row r="37" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="H37" s="10" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>674</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>635</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>634</v>
+      </c>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="H39" s="10" t="s">
+        <v>669</v>
+      </c>
+      <c r="I39" s="10" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
+        <v>673</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>672</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>670</v>
+      </c>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="H40" s="10" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>667</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>666</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="H41" s="10" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>663</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>623</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="H42" s="10" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>661</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>660</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>659</v>
+      </c>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="H44" s="10" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>658</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>657</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>656</v>
+      </c>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+    </row>
+    <row r="46" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>655</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>635</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>634</v>
+      </c>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="H46" s="10" t="s">
+        <v>650</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
+        <v>654</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>653</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>652</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>651</v>
+      </c>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="H47" s="10" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="10" t="s">
+        <v>629</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>649</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>648</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>647</v>
+      </c>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="H48" s="10" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>645</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>623</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="H49" s="10" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+    </row>
+    <row r="51" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>643</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>642</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>641</v>
+      </c>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="H51" s="10" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>639</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>638</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>637</v>
+      </c>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+    </row>
+    <row r="53" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>636</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>635</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>634</v>
+      </c>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="H53" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>633</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>632</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>631</v>
+      </c>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="H54" s="10" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="10" t="s">
+        <v>629</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>628</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>627</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>626</v>
+      </c>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="H55" s="10" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>624</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>623</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="H56" s="10" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+    </row>
+    <row r="58" spans="1:12" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A58" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>619</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>618</v>
+      </c>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="H58" s="10" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="10" t="s">
+        <v>616</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>615</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>614</v>
+      </c>
+      <c r="D59" s="19" t="s">
+        <v>613</v>
+      </c>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+    </row>
+    <row r="60" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>612</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>611</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>610</v>
+      </c>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="H60" s="10" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+    </row>
+    <row r="62" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+    </row>
+    <row r="63" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="10"/>
+      <c r="B63" s="10"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="L63" s="10"/>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;P</oddHeader>
+    <oddFooter>&amp;F</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:D75"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H93" sqref="H93"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>519</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>601</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>600</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>598</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>597</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>596</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>595</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>594</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>593</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>591</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>590</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>589</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>586</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>585</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>583</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>582</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>524</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>524</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>579</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>581</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>579</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>578</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>567</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>576</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>575</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>567</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>573</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>572</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>567</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>570</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>569</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>567</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>524</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>566</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>564</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>820</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>578</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>820</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>826</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>825</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>820</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>823</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>822</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>820</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>536</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>820</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>769</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>819</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>818</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>816</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>814</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>813</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>809</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>807</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>805</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>803</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>801</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>798</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>797</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>796</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>793</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>791</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>789</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>788</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>785</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>783</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>781</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>780</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>778</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>777</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>775</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>772</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>578</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>581</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>536</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>769</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="25" t="s">
+        <v>708</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>767</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="25" t="s">
+        <v>708</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>765</v>
+      </c>
+      <c r="C51" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="25" t="s">
+        <v>708</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>763</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="25" t="s">
+        <v>708</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>761</v>
+      </c>
+      <c r="C53" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="25" t="s">
+        <v>708</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>759</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="25" t="s">
+        <v>708</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>757</v>
+      </c>
+      <c r="C55" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="25" t="s">
+        <v>708</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>755</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="25" t="s">
+        <v>708</v>
+      </c>
+      <c r="B57" s="25" t="s">
+        <v>753</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="25" t="s">
+        <v>708</v>
+      </c>
+      <c r="B58" s="25" t="s">
+        <v>524</v>
+      </c>
+      <c r="C58" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>751</v>
+      </c>
+      <c r="C59" s="25" t="s">
+        <v>750</v>
+      </c>
+      <c r="D59" s="25" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>749</v>
+      </c>
+      <c r="C60" s="25" t="s">
+        <v>748</v>
+      </c>
+      <c r="D60" s="25" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="C61" s="25" t="s">
+        <v>746</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>745</v>
+      </c>
+      <c r="C62" s="25" t="s">
+        <v>744</v>
+      </c>
+      <c r="D62" s="25" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B63" s="25" t="s">
+        <v>743</v>
+      </c>
+      <c r="C63" s="25" t="s">
+        <v>742</v>
+      </c>
+      <c r="D63" s="25" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>741</v>
+      </c>
+      <c r="C64" s="25" t="s">
+        <v>740</v>
+      </c>
+      <c r="D64" s="25" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B65" s="25" t="s">
+        <v>739</v>
+      </c>
+      <c r="C65" s="25" t="s">
+        <v>738</v>
+      </c>
+      <c r="D65" s="25" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B66" s="25" t="s">
+        <v>737</v>
+      </c>
+      <c r="C66" s="25" t="s">
+        <v>736</v>
+      </c>
+      <c r="D66" s="25" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B67" s="25" t="s">
+        <v>734</v>
+      </c>
+      <c r="C67" s="25" t="s">
+        <v>733</v>
+      </c>
+      <c r="D67" s="25" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="25" t="s">
+        <v>718</v>
+      </c>
+      <c r="B68" s="25" t="s">
+        <v>732</v>
+      </c>
+      <c r="C68" s="25" t="s">
+        <v>731</v>
+      </c>
+      <c r="D68" s="25" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="25" t="s">
+        <v>718</v>
+      </c>
+      <c r="B69" s="25" t="s">
+        <v>730</v>
+      </c>
+      <c r="C69" s="25" t="s">
+        <v>729</v>
+      </c>
+      <c r="D69" s="25" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="25" t="s">
+        <v>718</v>
+      </c>
+      <c r="B70" s="25" t="s">
+        <v>728</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>727</v>
+      </c>
+      <c r="D70" s="25" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="25" t="s">
+        <v>718</v>
+      </c>
+      <c r="B71" s="25" t="s">
+        <v>726</v>
+      </c>
+      <c r="C71" s="25" t="s">
+        <v>725</v>
+      </c>
+      <c r="D71" s="25" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="25" t="s">
+        <v>718</v>
+      </c>
+      <c r="B72" s="25" t="s">
+        <v>724</v>
+      </c>
+      <c r="C72" s="25" t="s">
+        <v>723</v>
+      </c>
+      <c r="D72" s="25" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="25" t="s">
+        <v>718</v>
+      </c>
+      <c r="B73" s="25" t="s">
+        <v>722</v>
+      </c>
+      <c r="C73" s="25" t="s">
+        <v>721</v>
+      </c>
+      <c r="D73" s="25" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="25" t="s">
+        <v>718</v>
+      </c>
+      <c r="B74" s="25" t="s">
+        <v>720</v>
+      </c>
+      <c r="C74" s="25" t="s">
+        <v>719</v>
+      </c>
+      <c r="D74" s="25" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="25" t="s">
+        <v>718</v>
+      </c>
+      <c r="B75" s="25" t="s">
+        <v>717</v>
+      </c>
+      <c r="C75" s="25" t="s">
+        <v>716</v>
+      </c>
+      <c r="D75" s="25" t="s">
+        <v>716</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;P</oddHeader>
+    <oddFooter>&amp;F</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>608</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>607</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>833</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;P</oddHeader>
+    <oddFooter>&amp;F</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F114"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -8485,6 +11390,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B110:B112"/>
+    <mergeCell ref="C110:C112"/>
+    <mergeCell ref="C55:C59"/>
+    <mergeCell ref="C60:C69"/>
+    <mergeCell ref="C90:C108"/>
+    <mergeCell ref="C44:C53"/>
+    <mergeCell ref="C85:C88"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C73:C76"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C19"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="C39:C42"/>
     <mergeCell ref="A2:A27"/>
     <mergeCell ref="A28:A114"/>
     <mergeCell ref="B85:B88"/>
@@ -8501,22 +11422,6 @@
     <mergeCell ref="B32:B36"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="B44:B53"/>
-    <mergeCell ref="C44:C53"/>
-    <mergeCell ref="C85:C88"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C73:C76"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C19"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="B110:B112"/>
-    <mergeCell ref="C110:C112"/>
-    <mergeCell ref="C55:C59"/>
-    <mergeCell ref="C60:C69"/>
-    <mergeCell ref="C90:C108"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updating restriction for treatment_delay in xlsx dict
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-survey-dict.xlsx
+++ b/inst/extdata/MSF-survey-dict.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2581" uniqueCount="1386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2582" uniqueCount="1386">
   <si>
     <t>type</t>
   </si>
@@ -4787,8 +4787,8 @@
   </sheetPr>
   <dimension ref="A1:L209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D149" sqref="D149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8145,7 +8145,9 @@
       <c r="E148" s="14"/>
       <c r="F148" s="14"/>
       <c r="G148" s="14"/>
-      <c r="H148" s="13"/>
+      <c r="H148" s="13" t="s">
+        <v>661</v>
+      </c>
       <c r="I148" s="14"/>
       <c r="J148" s="14"/>
       <c r="K148" s="14"/>

</xml_diff>

<commit_message>
fix restriction on reason_first_hf_selected mort dict xlsx
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-survey-dict.xlsx
+++ b/inst/extdata/MSF-survey-dict.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2582" uniqueCount="1386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2583" uniqueCount="1386">
   <si>
     <t>type</t>
   </si>
@@ -4787,8 +4787,8 @@
   </sheetPr>
   <dimension ref="A1:L209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D149" sqref="D149"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H153" sqref="H153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8217,7 +8217,9 @@
       <c r="E151" s="14"/>
       <c r="F151" s="14"/>
       <c r="G151" s="14"/>
-      <c r="H151" s="15"/>
+      <c r="H151" s="15" t="s">
+        <v>663</v>
+      </c>
       <c r="I151" s="15"/>
       <c r="J151" s="15"/>
       <c r="K151" s="15"/>

</xml_diff>

<commit_message>
delete empty rows vacc dict xlsx
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-survey-dict.xlsx
+++ b/inst/extdata/MSF-survey-dict.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Mortality" sheetId="11" r:id="rId1"/>
@@ -22,6 +22,9 @@
     <sheet name="Vaccination_options" sheetId="15" r:id="rId8"/>
     <sheet name="Vaccination_settings" sheetId="16" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Vaccination!$A$1:$L$125</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
@@ -4787,7 +4790,7 @@
   </sheetPr>
   <dimension ref="A1:L209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A141" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H153" sqref="H153"/>
     </sheetView>
   </sheetViews>
@@ -12816,11 +12819,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L128"/>
+  <dimension ref="A1:L125"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13747,118 +13750,132 @@
       <c r="K41" s="57"/>
     </row>
     <row r="42" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="51"/>
-      <c r="B42" s="57"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="57"/>
+      <c r="A42" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="B42" s="51" t="s">
+        <v>317</v>
+      </c>
+      <c r="C42" s="51" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D42" s="51" t="s">
+        <v>1059</v>
+      </c>
       <c r="E42" s="52"/>
       <c r="F42" s="52"/>
       <c r="G42" s="57"/>
-      <c r="H42" s="57"/>
+      <c r="H42" s="51" t="s">
+        <v>1060</v>
+      </c>
       <c r="I42" s="57"/>
       <c r="J42" s="57"/>
       <c r="K42" s="57"/>
     </row>
-    <row r="43" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A43" s="51" t="s">
-        <v>160</v>
+        <v>312</v>
       </c>
       <c r="B43" s="51" t="s">
-        <v>317</v>
-      </c>
-      <c r="C43" s="51" t="s">
-        <v>1058</v>
-      </c>
-      <c r="D43" s="51" t="s">
-        <v>1059</v>
+        <v>1061</v>
+      </c>
+      <c r="C43" s="58" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D43" s="58" t="s">
+        <v>1063</v>
       </c>
       <c r="E43" s="52"/>
       <c r="F43" s="52"/>
       <c r="G43" s="57"/>
-      <c r="H43" s="51" t="s">
-        <v>1060</v>
-      </c>
+      <c r="H43" s="57"/>
       <c r="I43" s="57"/>
       <c r="J43" s="57"/>
       <c r="K43" s="57"/>
     </row>
-    <row r="44" spans="1:11" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="51" t="s">
-        <v>312</v>
+        <v>1064</v>
       </c>
       <c r="B44" s="51" t="s">
-        <v>1061</v>
+        <v>1065</v>
       </c>
       <c r="C44" s="58" t="s">
-        <v>1062</v>
+        <v>1066</v>
       </c>
       <c r="D44" s="58" t="s">
-        <v>1063</v>
+        <v>1067</v>
       </c>
       <c r="E44" s="52"/>
       <c r="F44" s="52"/>
       <c r="G44" s="57"/>
-      <c r="H44" s="57"/>
-      <c r="I44" s="57"/>
+      <c r="H44" s="51" t="s">
+        <v>1068</v>
+      </c>
+      <c r="I44" s="51"/>
       <c r="J44" s="57"/>
       <c r="K44" s="57"/>
     </row>
-    <row r="45" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="51" t="s">
-        <v>1064</v>
+        <v>312</v>
       </c>
       <c r="B45" s="51" t="s">
-        <v>1065</v>
+        <v>1069</v>
       </c>
       <c r="C45" s="58" t="s">
-        <v>1066</v>
+        <v>1070</v>
       </c>
       <c r="D45" s="58" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c r="E45" s="52"/>
       <c r="F45" s="52"/>
       <c r="G45" s="57"/>
-      <c r="H45" s="51" t="s">
-        <v>1068</v>
-      </c>
-      <c r="I45" s="51"/>
+      <c r="H45" s="51"/>
+      <c r="I45" s="57"/>
       <c r="J45" s="57"/>
       <c r="K45" s="57"/>
     </row>
     <row r="46" spans="1:11" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A46" s="51" t="s">
-        <v>312</v>
+        <v>49</v>
       </c>
       <c r="B46" s="51" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
       <c r="C46" s="58" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
       <c r="D46" s="58" t="s">
-        <v>1071</v>
-      </c>
-      <c r="E46" s="52"/>
-      <c r="F46" s="52"/>
+        <v>1074</v>
+      </c>
+      <c r="E46" s="52" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F46" s="52" t="s">
+        <v>1076</v>
+      </c>
       <c r="G46" s="57"/>
-      <c r="H46" s="51"/>
+      <c r="H46" s="51" t="s">
+        <v>1077</v>
+      </c>
       <c r="I46" s="57"/>
       <c r="J46" s="57"/>
       <c r="K46" s="57"/>
     </row>
-    <row r="47" spans="1:11" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A47" s="51" t="s">
         <v>49</v>
       </c>
       <c r="B47" s="51" t="s">
-        <v>1072</v>
+        <v>1078</v>
       </c>
       <c r="C47" s="58" t="s">
-        <v>1073</v>
+        <v>1079</v>
       </c>
       <c r="D47" s="58" t="s">
-        <v>1074</v>
+        <v>1080</v>
       </c>
       <c r="E47" s="52" t="s">
         <v>1075</v>
@@ -13874,196 +13891,190 @@
       <c r="J47" s="57"/>
       <c r="K47" s="57"/>
     </row>
-    <row r="48" spans="1:11" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="3" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A48" s="51" t="s">
+        <v>312</v>
+      </c>
+      <c r="B48" s="57" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C48" s="58" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D48" s="52" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="57"/>
+      <c r="H48" s="57"/>
+      <c r="I48" s="57"/>
+    </row>
+    <row r="49" spans="1:12" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A49" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="51" t="s">
-        <v>1078</v>
-      </c>
-      <c r="C48" s="58" t="s">
-        <v>1079</v>
-      </c>
-      <c r="D48" s="58" t="s">
-        <v>1080</v>
-      </c>
-      <c r="E48" s="52" t="s">
+      <c r="B49" s="57" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C49" s="58" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D49" s="52" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E49" s="52" t="s">
         <v>1075</v>
       </c>
-      <c r="F48" s="52" t="s">
+      <c r="F49" s="52" t="s">
         <v>1076</v>
       </c>
-      <c r="G48" s="57"/>
-      <c r="H48" s="51" t="s">
-        <v>1077</v>
-      </c>
-      <c r="I48" s="57"/>
-      <c r="J48" s="57"/>
-      <c r="K48" s="57"/>
-    </row>
-    <row r="49" spans="1:12" s="3" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="51" t="s">
+      <c r="G49" s="57"/>
+      <c r="H49" s="51" t="s">
+        <v>1087</v>
+      </c>
+      <c r="I49" s="57"/>
+    </row>
+    <row r="50" spans="1:12" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="57" t="s">
         <v>312</v>
       </c>
-      <c r="B49" s="57" t="s">
-        <v>1081</v>
-      </c>
-      <c r="C49" s="58" t="s">
-        <v>1082</v>
-      </c>
-      <c r="D49" s="52" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E49" s="52"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="57"/>
-      <c r="H49" s="57"/>
-      <c r="I49" s="57"/>
-    </row>
-    <row r="50" spans="1:12" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A50" s="51" t="s">
+      <c r="B50" s="57" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C50" s="58" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D50" s="52" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E50" s="52"/>
+      <c r="F50" s="52"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+    </row>
+    <row r="51" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="57" t="s">
-        <v>1084</v>
-      </c>
-      <c r="C50" s="58" t="s">
-        <v>1085</v>
-      </c>
-      <c r="D50" s="52" t="s">
-        <v>1086</v>
-      </c>
-      <c r="E50" s="52" t="s">
-        <v>1075</v>
-      </c>
-      <c r="F50" s="52" t="s">
-        <v>1076</v>
-      </c>
-      <c r="G50" s="57"/>
-      <c r="H50" s="51" t="s">
-        <v>1087</v>
-      </c>
-      <c r="I50" s="57"/>
-    </row>
-    <row r="51" spans="1:12" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="57" t="s">
-        <v>312</v>
-      </c>
       <c r="B51" s="57" t="s">
-        <v>1088</v>
+        <v>1091</v>
       </c>
       <c r="C51" s="58" t="s">
-        <v>1089</v>
+        <v>1092</v>
       </c>
       <c r="D51" s="52" t="s">
-        <v>1090</v>
+        <v>1093</v>
       </c>
       <c r="E51" s="52"/>
       <c r="F51" s="52"/>
       <c r="G51" s="57"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="57"/>
-    </row>
-    <row r="52" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H51" s="51" t="s">
+        <v>1094</v>
+      </c>
+      <c r="I51" s="51"/>
+    </row>
+    <row r="52" spans="1:12" s="3" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A52" s="57" t="s">
+        <v>312</v>
+      </c>
+      <c r="B52" s="57" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C52" s="58" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D52" s="52" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E52" s="52" t="s">
+        <v>1098</v>
+      </c>
+      <c r="F52" s="52" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G52" s="57"/>
+      <c r="H52" s="51"/>
+      <c r="I52" s="57"/>
+    </row>
+    <row r="53" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="B52" s="57" t="s">
-        <v>1091</v>
-      </c>
-      <c r="C52" s="58" t="s">
+      <c r="B53" s="57" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C53" s="58" t="s">
         <v>1092</v>
       </c>
-      <c r="D52" s="52" t="s">
+      <c r="D53" s="52" t="s">
         <v>1093</v>
       </c>
-      <c r="E52" s="52"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="57"/>
-      <c r="H52" s="51" t="s">
-        <v>1094</v>
-      </c>
-      <c r="I52" s="51"/>
-    </row>
-    <row r="53" spans="1:12" s="3" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A53" s="57" t="s">
+      <c r="E53" s="52"/>
+      <c r="F53" s="52"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="51" t="s">
+        <v>1101</v>
+      </c>
+      <c r="I53" s="57"/>
+    </row>
+    <row r="54" spans="1:12" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A54" s="57" t="s">
         <v>312</v>
       </c>
-      <c r="B53" s="57" t="s">
-        <v>1095</v>
-      </c>
-      <c r="C53" s="58" t="s">
-        <v>1096</v>
-      </c>
-      <c r="D53" s="52" t="s">
-        <v>1097</v>
-      </c>
-      <c r="E53" s="52" t="s">
-        <v>1098</v>
-      </c>
-      <c r="F53" s="52" t="s">
-        <v>1099</v>
-      </c>
-      <c r="G53" s="57"/>
-      <c r="H53" s="51"/>
-      <c r="I53" s="57"/>
-    </row>
-    <row r="54" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="57" t="s">
+      <c r="B54" s="57" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C54" s="58" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D54" s="52" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E54" s="52" t="s">
+        <v>1105</v>
+      </c>
+      <c r="F54" s="52" t="s">
+        <v>1106</v>
+      </c>
+      <c r="G54" s="57"/>
+      <c r="H54" s="51"/>
+      <c r="I54" s="57"/>
+    </row>
+    <row r="55" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="57" t="s">
-        <v>1100</v>
-      </c>
-      <c r="C54" s="58" t="s">
+      <c r="B55" s="57" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C55" s="58" t="s">
         <v>1092</v>
       </c>
-      <c r="D54" s="52" t="s">
+      <c r="D55" s="52" t="s">
         <v>1093</v>
       </c>
-      <c r="E54" s="52"/>
-      <c r="F54" s="52"/>
-      <c r="G54" s="57"/>
-      <c r="H54" s="51" t="s">
-        <v>1101</v>
-      </c>
-      <c r="I54" s="57"/>
-    </row>
-    <row r="55" spans="1:12" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A55" s="57" t="s">
-        <v>312</v>
-      </c>
-      <c r="B55" s="57" t="s">
-        <v>1102</v>
-      </c>
-      <c r="C55" s="58" t="s">
-        <v>1103</v>
-      </c>
-      <c r="D55" s="52" t="s">
-        <v>1104</v>
-      </c>
-      <c r="E55" s="52" t="s">
-        <v>1105</v>
-      </c>
-      <c r="F55" s="52" t="s">
-        <v>1106</v>
-      </c>
+      <c r="E55" s="52"/>
+      <c r="F55" s="52"/>
       <c r="G55" s="57"/>
-      <c r="H55" s="51"/>
+      <c r="H55" s="57" t="s">
+        <v>1108</v>
+      </c>
       <c r="I55" s="57"/>
     </row>
-    <row r="56" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A56" s="57" t="s">
         <v>49</v>
       </c>
       <c r="B56" s="57" t="s">
-        <v>1107</v>
+        <v>1109</v>
       </c>
       <c r="C56" s="58" t="s">
-        <v>1092</v>
+        <v>1110</v>
       </c>
       <c r="D56" s="52" t="s">
-        <v>1093</v>
+        <v>1111</v>
       </c>
       <c r="E56" s="52"/>
       <c r="F56" s="52"/>
@@ -14073,18 +14084,18 @@
       </c>
       <c r="I56" s="57"/>
     </row>
-    <row r="57" spans="1:12" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A57" s="57" t="s">
         <v>49</v>
       </c>
       <c r="B57" s="57" t="s">
-        <v>1109</v>
+        <v>1112</v>
       </c>
       <c r="C57" s="58" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="D57" s="52" t="s">
-        <v>1111</v>
+        <v>1114</v>
       </c>
       <c r="E57" s="52"/>
       <c r="F57" s="52"/>
@@ -14094,58 +14105,58 @@
       </c>
       <c r="I57" s="57"/>
     </row>
-    <row r="58" spans="1:12" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="57" t="s">
-        <v>49</v>
+        <v>312</v>
       </c>
       <c r="B58" s="57" t="s">
-        <v>1112</v>
+        <v>1115</v>
       </c>
       <c r="C58" s="58" t="s">
-        <v>1113</v>
+        <v>1116</v>
       </c>
       <c r="D58" s="52" t="s">
-        <v>1114</v>
+        <v>1117</v>
       </c>
       <c r="E58" s="52"/>
       <c r="F58" s="52"/>
       <c r="G58" s="57"/>
-      <c r="H58" s="57" t="s">
-        <v>1108</v>
-      </c>
-      <c r="I58" s="57"/>
+      <c r="H58" s="51"/>
+      <c r="I58" s="51"/>
     </row>
     <row r="59" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="57" t="s">
-        <v>312</v>
+        <v>49</v>
       </c>
       <c r="B59" s="57" t="s">
-        <v>1115</v>
+        <v>1118</v>
       </c>
       <c r="C59" s="58" t="s">
-        <v>1116</v>
+        <v>1092</v>
       </c>
       <c r="D59" s="52" t="s">
-        <v>1117</v>
+        <v>1093</v>
       </c>
       <c r="E59" s="52"/>
       <c r="F59" s="52"/>
       <c r="G59" s="57"/>
-      <c r="H59" s="51"/>
+      <c r="H59" s="51" t="s">
+        <v>1119</v>
+      </c>
       <c r="I59" s="51"/>
     </row>
-    <row r="60" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A60" s="57" t="s">
         <v>49</v>
       </c>
       <c r="B60" s="57" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="C60" s="58" t="s">
-        <v>1092</v>
+        <v>1121</v>
       </c>
       <c r="D60" s="52" t="s">
-        <v>1093</v>
+        <v>1122</v>
       </c>
       <c r="E60" s="52"/>
       <c r="F60" s="52"/>
@@ -14155,18 +14166,18 @@
       </c>
       <c r="I60" s="51"/>
     </row>
-    <row r="61" spans="1:12" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A61" s="57" t="s">
         <v>49</v>
       </c>
       <c r="B61" s="57" t="s">
-        <v>1120</v>
+        <v>1123</v>
       </c>
       <c r="C61" s="58" t="s">
-        <v>1121</v>
+        <v>1124</v>
       </c>
       <c r="D61" s="52" t="s">
-        <v>1122</v>
+        <v>1125</v>
       </c>
       <c r="E61" s="52"/>
       <c r="F61" s="52"/>
@@ -14174,207 +14185,202 @@
       <c r="H61" s="51" t="s">
         <v>1119</v>
       </c>
-      <c r="I61" s="51"/>
-    </row>
-    <row r="62" spans="1:12" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="I61" s="57"/>
+    </row>
+    <row r="62" spans="1:12" s="3" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A62" s="57" t="s">
-        <v>49</v>
+        <v>312</v>
       </c>
       <c r="B62" s="57" t="s">
-        <v>1123</v>
+        <v>1126</v>
       </c>
       <c r="C62" s="58" t="s">
-        <v>1124</v>
+        <v>1127</v>
       </c>
       <c r="D62" s="52" t="s">
-        <v>1125</v>
+        <v>1128</v>
       </c>
       <c r="E62" s="52"/>
       <c r="F62" s="52"/>
       <c r="G62" s="57"/>
-      <c r="H62" s="51" t="s">
-        <v>1119</v>
-      </c>
+      <c r="H62" s="57"/>
       <c r="I62" s="57"/>
-    </row>
-    <row r="63" spans="1:12" s="3" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="57" t="s">
-        <v>312</v>
+        <v>49</v>
       </c>
       <c r="B63" s="57" t="s">
-        <v>1126</v>
+        <v>1129</v>
       </c>
       <c r="C63" s="58" t="s">
-        <v>1127</v>
+        <v>1092</v>
       </c>
       <c r="D63" s="52" t="s">
-        <v>1128</v>
+        <v>1093</v>
       </c>
       <c r="E63" s="52"/>
       <c r="F63" s="52"/>
       <c r="G63" s="57"/>
-      <c r="H63" s="57"/>
+      <c r="H63" s="57" t="s">
+        <v>1130</v>
+      </c>
       <c r="I63" s="57"/>
-      <c r="L63" s="2"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A64" s="57" t="s">
-        <v>49</v>
+        <v>1131</v>
       </c>
       <c r="B64" s="57" t="s">
-        <v>1129</v>
+        <v>1132</v>
       </c>
       <c r="C64" s="58" t="s">
-        <v>1092</v>
+        <v>1133</v>
       </c>
       <c r="D64" s="52" t="s">
-        <v>1093</v>
+        <v>1134</v>
       </c>
       <c r="E64" s="52"/>
       <c r="F64" s="52"/>
       <c r="G64" s="57"/>
-      <c r="H64" s="57" t="s">
-        <v>1130</v>
-      </c>
+      <c r="H64" s="51"/>
       <c r="I64" s="57"/>
-    </row>
-    <row r="65" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="J64" s="57"/>
+      <c r="K64" s="57"/>
+      <c r="L64" s="57"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="57" t="s">
-        <v>1131</v>
+        <v>39</v>
       </c>
       <c r="B65" s="57" t="s">
-        <v>1132</v>
+        <v>1135</v>
       </c>
       <c r="C65" s="58" t="s">
-        <v>1133</v>
+        <v>1136</v>
       </c>
       <c r="D65" s="52" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="E65" s="52"/>
       <c r="F65" s="52"/>
       <c r="G65" s="57"/>
-      <c r="H65" s="51"/>
+      <c r="H65" s="57" t="s">
+        <v>1138</v>
+      </c>
       <c r="I65" s="57"/>
       <c r="J65" s="57"/>
       <c r="K65" s="57"/>
-      <c r="L65" s="57"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L65" s="51"/>
+    </row>
+    <row r="66" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A66" s="57" t="s">
         <v>39</v>
       </c>
       <c r="B66" s="57" t="s">
-        <v>1135</v>
+        <v>1139</v>
       </c>
       <c r="C66" s="58" t="s">
-        <v>1136</v>
+        <v>1140</v>
       </c>
       <c r="D66" s="52" t="s">
-        <v>1137</v>
-      </c>
-      <c r="E66" s="52"/>
-      <c r="F66" s="52"/>
+        <v>1141</v>
+      </c>
+      <c r="E66" s="52" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F66" s="52" t="s">
+        <v>1143</v>
+      </c>
       <c r="G66" s="57"/>
-      <c r="H66" s="57" t="s">
-        <v>1138</v>
-      </c>
+      <c r="H66" s="57"/>
       <c r="I66" s="57"/>
       <c r="J66" s="57"/>
       <c r="K66" s="57"/>
-      <c r="L66" s="51"/>
-    </row>
-    <row r="67" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="L66" s="57"/>
+    </row>
+    <row r="67" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A67" s="57" t="s">
-        <v>39</v>
+        <v>312</v>
       </c>
       <c r="B67" s="57" t="s">
-        <v>1139</v>
+        <v>1144</v>
       </c>
       <c r="C67" s="58" t="s">
-        <v>1140</v>
-      </c>
-      <c r="D67" s="52" t="s">
-        <v>1141</v>
-      </c>
-      <c r="E67" s="52" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F67" s="52" t="s">
-        <v>1143</v>
-      </c>
-      <c r="G67" s="57"/>
-      <c r="H67" s="57"/>
-      <c r="I67" s="57"/>
-      <c r="J67" s="57"/>
-      <c r="K67" s="57"/>
-      <c r="L67" s="57"/>
+        <v>1145</v>
+      </c>
+      <c r="D67" s="53" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E67" s="38"/>
+      <c r="F67" s="38"/>
+      <c r="G67" s="38"/>
+      <c r="H67" s="38"/>
+      <c r="I67" s="38"/>
+      <c r="J67" s="38"/>
+      <c r="K67" s="38"/>
+      <c r="L67" s="38"/>
     </row>
     <row r="68" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A68" s="57" t="s">
         <v>312</v>
       </c>
       <c r="B68" s="57" t="s">
-        <v>1144</v>
-      </c>
-      <c r="C68" s="58" t="s">
-        <v>1145</v>
+        <v>1147</v>
+      </c>
+      <c r="C68" s="57" t="s">
+        <v>1148</v>
       </c>
       <c r="D68" s="53" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E68" s="38"/>
       <c r="F68" s="38"/>
       <c r="G68" s="38"/>
-      <c r="H68" s="38"/>
+      <c r="H68" s="57" t="s">
+        <v>1150</v>
+      </c>
       <c r="I68" s="38"/>
       <c r="J68" s="38"/>
       <c r="K68" s="38"/>
       <c r="L68" s="38"/>
     </row>
-    <row r="69" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A69" s="57" t="s">
-        <v>312</v>
+        <v>178</v>
       </c>
       <c r="B69" s="57" t="s">
-        <v>1147</v>
-      </c>
-      <c r="C69" s="57" t="s">
-        <v>1148</v>
+        <v>1151</v>
+      </c>
+      <c r="C69" s="52" t="s">
+        <v>1152</v>
       </c>
       <c r="D69" s="53" t="s">
-        <v>1149</v>
+        <v>1153</v>
       </c>
       <c r="E69" s="38"/>
       <c r="F69" s="38"/>
       <c r="G69" s="38"/>
       <c r="H69" s="57" t="s">
-        <v>1150</v>
+        <v>1154</v>
       </c>
       <c r="I69" s="38"/>
       <c r="J69" s="38"/>
       <c r="K69" s="38"/>
       <c r="L69" s="38"/>
     </row>
-    <row r="70" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="57" t="s">
-        <v>178</v>
-      </c>
-      <c r="B70" s="57" t="s">
-        <v>1151</v>
-      </c>
-      <c r="C70" s="52" t="s">
-        <v>1152</v>
-      </c>
-      <c r="D70" s="53" t="s">
-        <v>1153</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="B70" s="38"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="53"/>
       <c r="E70" s="38"/>
       <c r="F70" s="38"/>
       <c r="G70" s="38"/>
-      <c r="H70" s="57" t="s">
-        <v>1154</v>
-      </c>
+      <c r="H70" s="38"/>
       <c r="I70" s="38"/>
       <c r="J70" s="38"/>
       <c r="K70" s="38"/>
@@ -14382,25 +14388,41 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="57" t="s">
-        <v>152</v>
-      </c>
-      <c r="B71" s="38"/>
-      <c r="C71" s="38"/>
-      <c r="D71" s="53"/>
+        <v>160</v>
+      </c>
+      <c r="B71" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="C71" s="57" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D71" s="53" t="s">
+        <v>1156</v>
+      </c>
       <c r="E71" s="38"/>
       <c r="F71" s="38"/>
       <c r="G71" s="38"/>
-      <c r="H71" s="38"/>
+      <c r="H71" s="57" t="s">
+        <v>1157</v>
+      </c>
       <c r="I71" s="38"/>
       <c r="J71" s="38"/>
       <c r="K71" s="38"/>
       <c r="L71" s="38"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A72" s="38"/>
-      <c r="B72" s="38"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="53"/>
+      <c r="A72" s="57" t="s">
+        <v>178</v>
+      </c>
+      <c r="B72" s="57" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C72" s="57" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D72" s="51" t="s">
+        <v>1160</v>
+      </c>
       <c r="E72" s="38"/>
       <c r="F72" s="38"/>
       <c r="G72" s="38"/>
@@ -14411,46 +14433,46 @@
       <c r="L72" s="38"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A73" s="57" t="s">
-        <v>160</v>
-      </c>
-      <c r="B73" s="57" t="s">
-        <v>316</v>
-      </c>
-      <c r="C73" s="57" t="s">
-        <v>1155</v>
-      </c>
-      <c r="D73" s="53" t="s">
-        <v>1156</v>
+      <c r="A73" s="51" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B73" s="51" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C73" s="51" t="s">
+        <v>1163</v>
+      </c>
+      <c r="D73" s="51" t="s">
+        <v>1163</v>
       </c>
       <c r="E73" s="38"/>
       <c r="F73" s="38"/>
       <c r="G73" s="38"/>
-      <c r="H73" s="57" t="s">
-        <v>1157</v>
-      </c>
+      <c r="H73" s="38"/>
       <c r="I73" s="38"/>
       <c r="J73" s="38"/>
       <c r="K73" s="38"/>
       <c r="L73" s="38"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A74" s="57" t="s">
-        <v>178</v>
-      </c>
-      <c r="B74" s="57" t="s">
-        <v>1158</v>
-      </c>
-      <c r="C74" s="57" t="s">
-        <v>1159</v>
+      <c r="A74" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="B74" s="51" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C74" s="51" t="s">
+        <v>1165</v>
       </c>
       <c r="D74" s="51" t="s">
-        <v>1160</v>
+        <v>1166</v>
       </c>
       <c r="E74" s="38"/>
       <c r="F74" s="38"/>
       <c r="G74" s="38"/>
-      <c r="H74" s="38"/>
+      <c r="H74" s="57" t="s">
+        <v>1167</v>
+      </c>
       <c r="I74" s="38"/>
       <c r="J74" s="38"/>
       <c r="K74" s="38"/>
@@ -14461,13 +14483,13 @@
         <v>1161</v>
       </c>
       <c r="B75" s="51" t="s">
-        <v>1162</v>
+        <v>1168</v>
       </c>
       <c r="C75" s="51" t="s">
-        <v>1163</v>
+        <v>1169</v>
       </c>
       <c r="D75" s="51" t="s">
-        <v>1163</v>
+        <v>1169</v>
       </c>
       <c r="E75" s="38"/>
       <c r="F75" s="38"/>
@@ -14483,19 +14505,19 @@
         <v>67</v>
       </c>
       <c r="B76" s="51" t="s">
-        <v>1164</v>
+        <v>1170</v>
       </c>
       <c r="C76" s="51" t="s">
-        <v>1165</v>
+        <v>1171</v>
       </c>
       <c r="D76" s="51" t="s">
-        <v>1166</v>
+        <v>1172</v>
       </c>
       <c r="E76" s="38"/>
       <c r="F76" s="38"/>
       <c r="G76" s="38"/>
       <c r="H76" s="57" t="s">
-        <v>1167</v>
+        <v>1173</v>
       </c>
       <c r="I76" s="38"/>
       <c r="J76" s="38"/>
@@ -14507,13 +14529,13 @@
         <v>1161</v>
       </c>
       <c r="B77" s="51" t="s">
-        <v>1168</v>
+        <v>1174</v>
       </c>
       <c r="C77" s="51" t="s">
-        <v>1169</v>
+        <v>1175</v>
       </c>
       <c r="D77" s="51" t="s">
-        <v>1169</v>
+        <v>1175</v>
       </c>
       <c r="E77" s="38"/>
       <c r="F77" s="38"/>
@@ -14529,19 +14551,19 @@
         <v>67</v>
       </c>
       <c r="B78" s="51" t="s">
-        <v>1170</v>
+        <v>1176</v>
       </c>
       <c r="C78" s="51" t="s">
-        <v>1171</v>
-      </c>
-      <c r="D78" s="51" t="s">
-        <v>1172</v>
+        <v>1177</v>
+      </c>
+      <c r="D78" s="57" t="s">
+        <v>1178</v>
       </c>
       <c r="E78" s="38"/>
       <c r="F78" s="38"/>
       <c r="G78" s="38"/>
       <c r="H78" s="57" t="s">
-        <v>1173</v>
+        <v>1179</v>
       </c>
       <c r="I78" s="38"/>
       <c r="J78" s="38"/>
@@ -14553,59 +14575,51 @@
         <v>1161</v>
       </c>
       <c r="B79" s="51" t="s">
-        <v>1174</v>
+        <v>1180</v>
       </c>
       <c r="C79" s="51" t="s">
-        <v>1175</v>
+        <v>1181</v>
       </c>
       <c r="D79" s="51" t="s">
-        <v>1175</v>
+        <v>1181</v>
       </c>
       <c r="E79" s="38"/>
       <c r="F79" s="38"/>
       <c r="G79" s="38"/>
       <c r="H79" s="38"/>
-      <c r="I79" s="38"/>
-      <c r="J79" s="38"/>
-      <c r="K79" s="38"/>
-      <c r="L79" s="38"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="51" t="s">
         <v>67</v>
       </c>
       <c r="B80" s="51" t="s">
-        <v>1176</v>
+        <v>1182</v>
       </c>
       <c r="C80" s="51" t="s">
-        <v>1177</v>
-      </c>
-      <c r="D80" s="57" t="s">
-        <v>1178</v>
+        <v>1183</v>
+      </c>
+      <c r="D80" s="51" t="s">
+        <v>1184</v>
       </c>
       <c r="E80" s="38"/>
       <c r="F80" s="38"/>
       <c r="G80" s="38"/>
       <c r="H80" s="57" t="s">
-        <v>1179</v>
-      </c>
-      <c r="I80" s="38"/>
-      <c r="J80" s="38"/>
-      <c r="K80" s="38"/>
-      <c r="L80" s="38"/>
+        <v>1185</v>
+      </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="51" t="s">
         <v>1161</v>
       </c>
       <c r="B81" s="51" t="s">
-        <v>1180</v>
+        <v>1186</v>
       </c>
       <c r="C81" s="51" t="s">
-        <v>1181</v>
+        <v>1187</v>
       </c>
       <c r="D81" s="51" t="s">
-        <v>1181</v>
+        <v>1188</v>
       </c>
       <c r="E81" s="38"/>
       <c r="F81" s="38"/>
@@ -14617,19 +14631,19 @@
         <v>67</v>
       </c>
       <c r="B82" s="51" t="s">
-        <v>1182</v>
+        <v>1189</v>
       </c>
       <c r="C82" s="51" t="s">
-        <v>1183</v>
+        <v>1190</v>
       </c>
       <c r="D82" s="51" t="s">
-        <v>1184</v>
+        <v>1191</v>
       </c>
       <c r="E82" s="38"/>
       <c r="F82" s="38"/>
       <c r="G82" s="38"/>
       <c r="H82" s="57" t="s">
-        <v>1185</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -14637,13 +14651,13 @@
         <v>1161</v>
       </c>
       <c r="B83" s="51" t="s">
-        <v>1186</v>
+        <v>1193</v>
       </c>
       <c r="C83" s="51" t="s">
-        <v>1187</v>
+        <v>1194</v>
       </c>
       <c r="D83" s="51" t="s">
-        <v>1188</v>
+        <v>1195</v>
       </c>
       <c r="E83" s="38"/>
       <c r="F83" s="38"/>
@@ -14655,19 +14669,19 @@
         <v>67</v>
       </c>
       <c r="B84" s="51" t="s">
-        <v>1189</v>
+        <v>1196</v>
       </c>
       <c r="C84" s="51" t="s">
-        <v>1190</v>
+        <v>1197</v>
       </c>
       <c r="D84" s="51" t="s">
-        <v>1191</v>
+        <v>1198</v>
       </c>
       <c r="E84" s="38"/>
       <c r="F84" s="38"/>
       <c r="G84" s="38"/>
       <c r="H84" s="57" t="s">
-        <v>1192</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -14675,13 +14689,13 @@
         <v>1161</v>
       </c>
       <c r="B85" s="51" t="s">
-        <v>1193</v>
+        <v>1200</v>
       </c>
       <c r="C85" s="51" t="s">
-        <v>1194</v>
-      </c>
-      <c r="D85" s="51" t="s">
-        <v>1195</v>
+        <v>1201</v>
+      </c>
+      <c r="D85" s="57" t="s">
+        <v>1202</v>
       </c>
       <c r="E85" s="38"/>
       <c r="F85" s="38"/>
@@ -14693,19 +14707,19 @@
         <v>67</v>
       </c>
       <c r="B86" s="51" t="s">
-        <v>1196</v>
-      </c>
-      <c r="C86" s="51" t="s">
-        <v>1197</v>
-      </c>
-      <c r="D86" s="51" t="s">
-        <v>1198</v>
+        <v>1203</v>
+      </c>
+      <c r="C86" s="57" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D86" s="58" t="s">
+        <v>1205</v>
       </c>
       <c r="E86" s="38"/>
       <c r="F86" s="38"/>
       <c r="G86" s="38"/>
       <c r="H86" s="57" t="s">
-        <v>1199</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -14713,13 +14727,13 @@
         <v>1161</v>
       </c>
       <c r="B87" s="51" t="s">
-        <v>1200</v>
+        <v>1207</v>
       </c>
       <c r="C87" s="51" t="s">
-        <v>1201</v>
-      </c>
-      <c r="D87" s="57" t="s">
-        <v>1202</v>
+        <v>1208</v>
+      </c>
+      <c r="D87" s="58" t="s">
+        <v>1209</v>
       </c>
       <c r="E87" s="38"/>
       <c r="F87" s="38"/>
@@ -14731,19 +14745,19 @@
         <v>67</v>
       </c>
       <c r="B88" s="51" t="s">
-        <v>1203</v>
-      </c>
-      <c r="C88" s="57" t="s">
-        <v>1204</v>
-      </c>
-      <c r="D88" s="58" t="s">
-        <v>1205</v>
+        <v>1210</v>
+      </c>
+      <c r="C88" s="51" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D88" s="51" t="s">
+        <v>1212</v>
       </c>
       <c r="E88" s="38"/>
       <c r="F88" s="38"/>
       <c r="G88" s="38"/>
       <c r="H88" s="57" t="s">
-        <v>1206</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -14751,13 +14765,13 @@
         <v>1161</v>
       </c>
       <c r="B89" s="51" t="s">
-        <v>1207</v>
+        <v>1214</v>
       </c>
       <c r="C89" s="51" t="s">
-        <v>1208</v>
-      </c>
-      <c r="D89" s="58" t="s">
-        <v>1209</v>
+        <v>1215</v>
+      </c>
+      <c r="D89" s="57" t="s">
+        <v>1216</v>
       </c>
       <c r="E89" s="38"/>
       <c r="F89" s="38"/>
@@ -14769,33 +14783,33 @@
         <v>67</v>
       </c>
       <c r="B90" s="51" t="s">
-        <v>1210</v>
-      </c>
-      <c r="C90" s="51" t="s">
-        <v>1211</v>
-      </c>
-      <c r="D90" s="51" t="s">
-        <v>1212</v>
+        <v>1217</v>
+      </c>
+      <c r="C90" s="57" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D90" s="57" t="s">
+        <v>1219</v>
       </c>
       <c r="E90" s="38"/>
       <c r="F90" s="38"/>
       <c r="G90" s="38"/>
       <c r="H90" s="57" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="51" t="s">
         <v>1161</v>
       </c>
-      <c r="B91" s="51" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C91" s="51" t="s">
-        <v>1215</v>
+      <c r="B91" s="57" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C91" s="57" t="s">
+        <v>1222</v>
       </c>
       <c r="D91" s="57" t="s">
-        <v>1216</v>
+        <v>1222</v>
       </c>
       <c r="E91" s="38"/>
       <c r="F91" s="38"/>
@@ -14807,19 +14821,19 @@
         <v>67</v>
       </c>
       <c r="B92" s="51" t="s">
-        <v>1217</v>
+        <v>1223</v>
       </c>
       <c r="C92" s="57" t="s">
-        <v>1218</v>
-      </c>
-      <c r="D92" s="57" t="s">
-        <v>1219</v>
+        <v>1224</v>
+      </c>
+      <c r="D92" s="38" t="s">
+        <v>1225</v>
       </c>
       <c r="E92" s="38"/>
       <c r="F92" s="38"/>
       <c r="G92" s="38"/>
       <c r="H92" s="57" t="s">
-        <v>1220</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -14827,13 +14841,13 @@
         <v>1161</v>
       </c>
       <c r="B93" s="57" t="s">
-        <v>1221</v>
+        <v>1227</v>
       </c>
       <c r="C93" s="57" t="s">
-        <v>1222</v>
-      </c>
-      <c r="D93" s="57" t="s">
-        <v>1222</v>
+        <v>1228</v>
+      </c>
+      <c r="D93" s="38" t="s">
+        <v>1228</v>
       </c>
       <c r="E93" s="38"/>
       <c r="F93" s="38"/>
@@ -14845,19 +14859,19 @@
         <v>67</v>
       </c>
       <c r="B94" s="51" t="s">
-        <v>1223</v>
+        <v>1229</v>
       </c>
       <c r="C94" s="57" t="s">
-        <v>1224</v>
+        <v>1230</v>
       </c>
       <c r="D94" s="38" t="s">
-        <v>1225</v>
+        <v>1231</v>
       </c>
       <c r="E94" s="38"/>
       <c r="F94" s="38"/>
       <c r="G94" s="38"/>
       <c r="H94" s="57" t="s">
-        <v>1226</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -14865,13 +14879,13 @@
         <v>1161</v>
       </c>
       <c r="B95" s="57" t="s">
-        <v>1227</v>
+        <v>1233</v>
       </c>
       <c r="C95" s="57" t="s">
-        <v>1228</v>
+        <v>1234</v>
       </c>
       <c r="D95" s="38" t="s">
-        <v>1228</v>
+        <v>1234</v>
       </c>
       <c r="E95" s="38"/>
       <c r="F95" s="38"/>
@@ -14883,19 +14897,19 @@
         <v>67</v>
       </c>
       <c r="B96" s="51" t="s">
-        <v>1229</v>
+        <v>1235</v>
       </c>
       <c r="C96" s="57" t="s">
-        <v>1230</v>
+        <v>1236</v>
       </c>
       <c r="D96" s="38" t="s">
-        <v>1231</v>
+        <v>1237</v>
       </c>
       <c r="E96" s="38"/>
       <c r="F96" s="38"/>
       <c r="G96" s="38"/>
       <c r="H96" s="57" t="s">
-        <v>1232</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -14903,13 +14917,13 @@
         <v>1161</v>
       </c>
       <c r="B97" s="57" t="s">
-        <v>1233</v>
+        <v>1239</v>
       </c>
       <c r="C97" s="57" t="s">
-        <v>1234</v>
+        <v>1240</v>
       </c>
       <c r="D97" s="38" t="s">
-        <v>1234</v>
+        <v>1241</v>
       </c>
       <c r="E97" s="38"/>
       <c r="F97" s="38"/>
@@ -14920,20 +14934,20 @@
       <c r="A98" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="B98" s="51" t="s">
-        <v>1235</v>
+      <c r="B98" s="57" t="s">
+        <v>1242</v>
       </c>
       <c r="C98" s="57" t="s">
-        <v>1236</v>
+        <v>1243</v>
       </c>
       <c r="D98" s="38" t="s">
-        <v>1237</v>
+        <v>1244</v>
       </c>
       <c r="E98" s="38"/>
       <c r="F98" s="38"/>
       <c r="G98" s="38"/>
       <c r="H98" s="57" t="s">
-        <v>1238</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -14941,13 +14955,13 @@
         <v>1161</v>
       </c>
       <c r="B99" s="57" t="s">
-        <v>1239</v>
+        <v>1246</v>
       </c>
       <c r="C99" s="57" t="s">
-        <v>1240</v>
+        <v>1247</v>
       </c>
       <c r="D99" s="38" t="s">
-        <v>1241</v>
+        <v>1247</v>
       </c>
       <c r="E99" s="38"/>
       <c r="F99" s="38"/>
@@ -14959,19 +14973,19 @@
         <v>67</v>
       </c>
       <c r="B100" s="57" t="s">
-        <v>1242</v>
+        <v>1248</v>
       </c>
       <c r="C100" s="57" t="s">
-        <v>1243</v>
+        <v>1249</v>
       </c>
       <c r="D100" s="38" t="s">
-        <v>1244</v>
+        <v>1250</v>
       </c>
       <c r="E100" s="38"/>
       <c r="F100" s="38"/>
       <c r="G100" s="38"/>
       <c r="H100" s="57" t="s">
-        <v>1245</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -14979,13 +14993,13 @@
         <v>1161</v>
       </c>
       <c r="B101" s="57" t="s">
-        <v>1246</v>
+        <v>1252</v>
       </c>
       <c r="C101" s="57" t="s">
-        <v>1247</v>
+        <v>1253</v>
       </c>
       <c r="D101" s="38" t="s">
-        <v>1247</v>
+        <v>1253</v>
       </c>
       <c r="E101" s="38"/>
       <c r="F101" s="38"/>
@@ -14997,19 +15011,19 @@
         <v>67</v>
       </c>
       <c r="B102" s="57" t="s">
-        <v>1248</v>
+        <v>1254</v>
       </c>
       <c r="C102" s="57" t="s">
-        <v>1249</v>
+        <v>1255</v>
       </c>
       <c r="D102" s="38" t="s">
-        <v>1250</v>
+        <v>1256</v>
       </c>
       <c r="E102" s="38"/>
       <c r="F102" s="38"/>
       <c r="G102" s="38"/>
       <c r="H102" s="57" t="s">
-        <v>1251</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
@@ -15017,13 +15031,13 @@
         <v>1161</v>
       </c>
       <c r="B103" s="57" t="s">
-        <v>1252</v>
+        <v>1258</v>
       </c>
       <c r="C103" s="57" t="s">
-        <v>1253</v>
+        <v>1259</v>
       </c>
       <c r="D103" s="38" t="s">
-        <v>1253</v>
+        <v>1259</v>
       </c>
       <c r="E103" s="38"/>
       <c r="F103" s="38"/>
@@ -15035,19 +15049,19 @@
         <v>67</v>
       </c>
       <c r="B104" s="57" t="s">
-        <v>1254</v>
+        <v>1260</v>
       </c>
       <c r="C104" s="57" t="s">
-        <v>1255</v>
-      </c>
-      <c r="D104" s="38" t="s">
-        <v>1256</v>
+        <v>1261</v>
+      </c>
+      <c r="D104" s="57" t="s">
+        <v>1262</v>
       </c>
       <c r="E104" s="38"/>
       <c r="F104" s="38"/>
       <c r="G104" s="38"/>
       <c r="H104" s="57" t="s">
-        <v>1257</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
@@ -15055,13 +15069,13 @@
         <v>1161</v>
       </c>
       <c r="B105" s="57" t="s">
-        <v>1258</v>
+        <v>1264</v>
       </c>
       <c r="C105" s="57" t="s">
-        <v>1259</v>
+        <v>1265</v>
       </c>
       <c r="D105" s="38" t="s">
-        <v>1259</v>
+        <v>1266</v>
       </c>
       <c r="E105" s="38"/>
       <c r="F105" s="38"/>
@@ -15073,19 +15087,19 @@
         <v>67</v>
       </c>
       <c r="B106" s="57" t="s">
-        <v>1260</v>
+        <v>1267</v>
       </c>
       <c r="C106" s="57" t="s">
-        <v>1261</v>
-      </c>
-      <c r="D106" s="57" t="s">
-        <v>1262</v>
+        <v>1268</v>
+      </c>
+      <c r="D106" s="38" t="s">
+        <v>1269</v>
       </c>
       <c r="E106" s="38"/>
       <c r="F106" s="38"/>
       <c r="G106" s="38"/>
       <c r="H106" s="57" t="s">
-        <v>1263</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -15093,13 +15107,13 @@
         <v>1161</v>
       </c>
       <c r="B107" s="57" t="s">
-        <v>1264</v>
+        <v>1271</v>
       </c>
       <c r="C107" s="57" t="s">
-        <v>1265</v>
+        <v>1272</v>
       </c>
       <c r="D107" s="38" t="s">
-        <v>1266</v>
+        <v>1273</v>
       </c>
       <c r="E107" s="38"/>
       <c r="F107" s="38"/>
@@ -15111,19 +15125,19 @@
         <v>67</v>
       </c>
       <c r="B108" s="57" t="s">
-        <v>1267</v>
+        <v>1274</v>
       </c>
       <c r="C108" s="57" t="s">
-        <v>1268</v>
+        <v>1275</v>
       </c>
       <c r="D108" s="38" t="s">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="E108" s="38"/>
       <c r="F108" s="38"/>
       <c r="G108" s="38"/>
       <c r="H108" s="57" t="s">
-        <v>1270</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
@@ -15131,13 +15145,13 @@
         <v>1161</v>
       </c>
       <c r="B109" s="57" t="s">
-        <v>1271</v>
+        <v>1278</v>
       </c>
       <c r="C109" s="57" t="s">
-        <v>1272</v>
+        <v>1279</v>
       </c>
       <c r="D109" s="38" t="s">
-        <v>1273</v>
+        <v>1279</v>
       </c>
       <c r="E109" s="38"/>
       <c r="F109" s="38"/>
@@ -15149,19 +15163,19 @@
         <v>67</v>
       </c>
       <c r="B110" s="57" t="s">
-        <v>1274</v>
+        <v>1280</v>
       </c>
       <c r="C110" s="57" t="s">
-        <v>1275</v>
+        <v>1281</v>
       </c>
       <c r="D110" s="38" t="s">
-        <v>1276</v>
+        <v>1282</v>
       </c>
       <c r="E110" s="38"/>
       <c r="F110" s="38"/>
       <c r="G110" s="38"/>
       <c r="H110" s="57" t="s">
-        <v>1277</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
@@ -15169,13 +15183,13 @@
         <v>1161</v>
       </c>
       <c r="B111" s="57" t="s">
-        <v>1278</v>
+        <v>1284</v>
       </c>
       <c r="C111" s="57" t="s">
-        <v>1279</v>
+        <v>1285</v>
       </c>
       <c r="D111" s="38" t="s">
-        <v>1279</v>
+        <v>1286</v>
       </c>
       <c r="E111" s="38"/>
       <c r="F111" s="38"/>
@@ -15187,19 +15201,19 @@
         <v>67</v>
       </c>
       <c r="B112" s="57" t="s">
-        <v>1280</v>
+        <v>1287</v>
       </c>
       <c r="C112" s="57" t="s">
-        <v>1281</v>
+        <v>1288</v>
       </c>
       <c r="D112" s="38" t="s">
-        <v>1282</v>
+        <v>1289</v>
       </c>
       <c r="E112" s="38"/>
       <c r="F112" s="38"/>
       <c r="G112" s="38"/>
       <c r="H112" s="57" t="s">
-        <v>1283</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
@@ -15207,13 +15221,13 @@
         <v>1161</v>
       </c>
       <c r="B113" s="57" t="s">
-        <v>1284</v>
+        <v>1291</v>
       </c>
       <c r="C113" s="57" t="s">
-        <v>1285</v>
+        <v>1292</v>
       </c>
       <c r="D113" s="38" t="s">
-        <v>1286</v>
+        <v>1293</v>
       </c>
       <c r="E113" s="38"/>
       <c r="F113" s="38"/>
@@ -15225,19 +15239,19 @@
         <v>67</v>
       </c>
       <c r="B114" s="57" t="s">
-        <v>1287</v>
+        <v>1294</v>
       </c>
       <c r="C114" s="57" t="s">
-        <v>1288</v>
+        <v>1295</v>
       </c>
       <c r="D114" s="38" t="s">
-        <v>1289</v>
+        <v>1296</v>
       </c>
       <c r="E114" s="38"/>
       <c r="F114" s="38"/>
       <c r="G114" s="38"/>
       <c r="H114" s="57" t="s">
-        <v>1290</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
@@ -15245,13 +15259,13 @@
         <v>1161</v>
       </c>
       <c r="B115" s="57" t="s">
-        <v>1291</v>
+        <v>1298</v>
       </c>
       <c r="C115" s="57" t="s">
-        <v>1292</v>
+        <v>1299</v>
       </c>
       <c r="D115" s="38" t="s">
-        <v>1293</v>
+        <v>1300</v>
       </c>
       <c r="E115" s="38"/>
       <c r="F115" s="38"/>
@@ -15263,216 +15277,168 @@
         <v>67</v>
       </c>
       <c r="B116" s="57" t="s">
-        <v>1294</v>
+        <v>1301</v>
       </c>
       <c r="C116" s="57" t="s">
-        <v>1295</v>
+        <v>1302</v>
       </c>
       <c r="D116" s="38" t="s">
-        <v>1296</v>
+        <v>1303</v>
       </c>
       <c r="E116" s="38"/>
       <c r="F116" s="38"/>
       <c r="G116" s="38"/>
       <c r="H116" s="57" t="s">
-        <v>1297</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A117" s="51" t="s">
-        <v>1161</v>
+        <v>178</v>
       </c>
       <c r="B117" s="57" t="s">
-        <v>1298</v>
-      </c>
-      <c r="C117" s="57" t="s">
-        <v>1299</v>
-      </c>
-      <c r="D117" s="38" t="s">
-        <v>1300</v>
+        <v>1305</v>
+      </c>
+      <c r="C117" s="52" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D117" s="53" t="s">
+        <v>1307</v>
       </c>
       <c r="E117" s="38"/>
       <c r="F117" s="38"/>
       <c r="G117" s="38"/>
-      <c r="H117" s="38"/>
+      <c r="H117" s="57"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A118" s="51" t="s">
-        <v>67</v>
+      <c r="A118" s="57" t="s">
+        <v>312</v>
       </c>
       <c r="B118" s="57" t="s">
-        <v>1301</v>
+        <v>1308</v>
       </c>
       <c r="C118" s="57" t="s">
-        <v>1302</v>
+        <v>1148</v>
       </c>
       <c r="D118" s="38" t="s">
-        <v>1303</v>
+        <v>1149</v>
       </c>
       <c r="E118" s="38"/>
       <c r="F118" s="38"/>
       <c r="G118" s="38"/>
-      <c r="H118" s="57" t="s">
-        <v>1304</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="H118" s="57"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="51" t="s">
-        <v>178</v>
-      </c>
-      <c r="B119" s="57" t="s">
-        <v>1305</v>
-      </c>
-      <c r="C119" s="52" t="s">
-        <v>1306</v>
-      </c>
-      <c r="D119" s="53" t="s">
-        <v>1307</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="B119" s="38"/>
+      <c r="C119" s="38"/>
+      <c r="D119" s="38"/>
       <c r="E119" s="38"/>
       <c r="F119" s="38"/>
       <c r="G119" s="38"/>
-      <c r="H119" s="57"/>
+      <c r="H119" s="38"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A120" s="57" t="s">
-        <v>312</v>
+      <c r="A120" s="51" t="s">
+        <v>160</v>
       </c>
       <c r="B120" s="57" t="s">
-        <v>1308</v>
+        <v>315</v>
       </c>
       <c r="C120" s="57" t="s">
-        <v>1148</v>
+        <v>1309</v>
       </c>
       <c r="D120" s="38" t="s">
-        <v>1149</v>
+        <v>1310</v>
       </c>
       <c r="E120" s="38"/>
       <c r="F120" s="38"/>
       <c r="G120" s="38"/>
-      <c r="H120" s="57"/>
+      <c r="H120" s="57" t="s">
+        <v>1311</v>
+      </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" s="51" t="s">
-        <v>152</v>
-      </c>
-      <c r="B121" s="38"/>
-      <c r="C121" s="38"/>
-      <c r="D121" s="38"/>
+      <c r="A121" s="57" t="s">
+        <v>178</v>
+      </c>
+      <c r="B121" s="57" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C121" s="57" t="s">
+        <v>1313</v>
+      </c>
+      <c r="D121" s="57" t="s">
+        <v>1314</v>
+      </c>
       <c r="E121" s="38"/>
       <c r="F121" s="38"/>
       <c r="G121" s="38"/>
       <c r="H121" s="38"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A122" s="51"/>
-      <c r="B122" s="38"/>
-      <c r="C122" s="38"/>
-      <c r="D122" s="38"/>
+      <c r="A122" s="57" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B122" s="57" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C122" s="57" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D122" s="38" t="s">
+        <v>1318</v>
+      </c>
       <c r="E122" s="38"/>
       <c r="F122" s="38"/>
       <c r="G122" s="38"/>
       <c r="H122" s="38"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A123" s="51" t="s">
-        <v>160</v>
+      <c r="A123" s="57" t="s">
+        <v>39</v>
       </c>
       <c r="B123" s="57" t="s">
-        <v>315</v>
+        <v>1319</v>
       </c>
       <c r="C123" s="57" t="s">
-        <v>1309</v>
+        <v>1320</v>
       </c>
       <c r="D123" s="38" t="s">
-        <v>1310</v>
+        <v>1321</v>
       </c>
       <c r="E123" s="38"/>
       <c r="F123" s="38"/>
       <c r="G123" s="38"/>
       <c r="H123" s="57" t="s">
-        <v>1311</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="57" t="s">
-        <v>178</v>
-      </c>
-      <c r="B124" s="57" t="s">
-        <v>1312</v>
-      </c>
-      <c r="C124" s="57" t="s">
-        <v>1313</v>
-      </c>
-      <c r="D124" s="57" t="s">
-        <v>1314</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="B124" s="57"/>
+      <c r="C124" s="57"/>
+      <c r="D124" s="38"/>
       <c r="E124" s="38"/>
       <c r="F124" s="38"/>
       <c r="G124" s="38"/>
-      <c r="H124" s="38"/>
+      <c r="H124" s="57"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="57" t="s">
-        <v>1315</v>
-      </c>
-      <c r="B125" s="57" t="s">
-        <v>1316</v>
-      </c>
-      <c r="C125" s="57" t="s">
-        <v>1317</v>
-      </c>
-      <c r="D125" s="38" t="s">
-        <v>1318</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B125" s="38"/>
+      <c r="C125" s="38"/>
+      <c r="D125" s="38"/>
       <c r="E125" s="38"/>
       <c r="F125" s="38"/>
       <c r="G125" s="38"/>
       <c r="H125" s="38"/>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A126" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="B126" s="57" t="s">
-        <v>1319</v>
-      </c>
-      <c r="C126" s="57" t="s">
-        <v>1320</v>
-      </c>
-      <c r="D126" s="38" t="s">
-        <v>1321</v>
-      </c>
-      <c r="E126" s="38"/>
-      <c r="F126" s="38"/>
-      <c r="G126" s="38"/>
-      <c r="H126" s="57" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A127" s="57" t="s">
-        <v>152</v>
-      </c>
-      <c r="B127" s="57"/>
-      <c r="C127" s="57"/>
-      <c r="D127" s="38"/>
-      <c r="E127" s="38"/>
-      <c r="F127" s="38"/>
-      <c r="G127" s="38"/>
-      <c r="H127" s="57"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A128" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="B128" s="38"/>
-      <c r="C128" s="38"/>
-      <c r="D128" s="38"/>
-      <c r="E128" s="38"/>
-      <c r="F128" s="38"/>
-      <c r="G128" s="38"/>
-      <c r="H128" s="38"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
fix typo in vacc dict xlsx
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-survey-dict.xlsx
+++ b/inst/extdata/MSF-survey-dict.xlsx
@@ -3377,9 +3377,6 @@
     <t>L'enfant a-t-il déjà reçu une injection sur la partie supérieure de la cuisse au cours des deux premières années de sa vie - il s'agit d'une vaccination quadruple ou penta pour le protéger contre des maladies comme le tétanos, la coqueluche, la diphtérie, la grippe ou l'hépatite ?</t>
   </si>
   <si>
-    <t>num_quand_penta_woc</t>
-  </si>
-  <si>
     <t>How many times?</t>
   </si>
   <si>
@@ -4271,6 +4268,9 @@
   </si>
   <si>
     <t>${care_fever} = "no" or ${care_fever} = "don’t_know"</t>
+  </si>
+  <si>
+    <t>num_quad_penta_woc</t>
   </si>
 </sst>
 </file>
@@ -5786,7 +5786,7 @@
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
       <c r="H43" s="9" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
@@ -6263,7 +6263,7 @@
       <c r="F68" s="14"/>
       <c r="G68" s="14"/>
       <c r="H68" s="13" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="I68" s="13"/>
     </row>
@@ -7291,7 +7291,7 @@
       <c r="F111" s="15"/>
       <c r="G111" s="15"/>
       <c r="H111" s="14" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="I111" s="15"/>
       <c r="J111" s="15"/>
@@ -7315,7 +7315,7 @@
       <c r="F112" s="15"/>
       <c r="G112" s="15"/>
       <c r="H112" s="14" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="I112" s="15"/>
       <c r="J112" s="15"/>
@@ -7339,7 +7339,7 @@
       <c r="F113" s="15"/>
       <c r="G113" s="15"/>
       <c r="H113" s="14" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="I113" s="15"/>
       <c r="J113" s="15"/>
@@ -12822,8 +12822,8 @@
   <dimension ref="A1:L125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A132" sqref="A132"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13959,19 +13959,19 @@
         <v>49</v>
       </c>
       <c r="B51" s="57" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C51" s="58" t="s">
         <v>1091</v>
       </c>
-      <c r="C51" s="58" t="s">
+      <c r="D51" s="52" t="s">
         <v>1092</v>
-      </c>
-      <c r="D51" s="52" t="s">
-        <v>1093</v>
       </c>
       <c r="E51" s="52"/>
       <c r="F51" s="52"/>
       <c r="G51" s="57"/>
       <c r="H51" s="51" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="I51" s="51"/>
     </row>
@@ -13980,19 +13980,19 @@
         <v>312</v>
       </c>
       <c r="B52" s="57" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C52" s="58" t="s">
         <v>1095</v>
       </c>
-      <c r="C52" s="58" t="s">
+      <c r="D52" s="52" t="s">
         <v>1096</v>
       </c>
-      <c r="D52" s="52" t="s">
+      <c r="E52" s="52" t="s">
         <v>1097</v>
       </c>
-      <c r="E52" s="52" t="s">
+      <c r="F52" s="52" t="s">
         <v>1098</v>
-      </c>
-      <c r="F52" s="52" t="s">
-        <v>1099</v>
       </c>
       <c r="G52" s="57"/>
       <c r="H52" s="51"/>
@@ -14003,19 +14003,19 @@
         <v>49</v>
       </c>
       <c r="B53" s="57" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="C53" s="58" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D53" s="52" t="s">
         <v>1092</v>
-      </c>
-      <c r="D53" s="52" t="s">
-        <v>1093</v>
       </c>
       <c r="E53" s="52"/>
       <c r="F53" s="52"/>
       <c r="G53" s="57"/>
       <c r="H53" s="51" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="I53" s="57"/>
     </row>
@@ -14024,19 +14024,19 @@
         <v>312</v>
       </c>
       <c r="B54" s="57" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C54" s="58" t="s">
         <v>1102</v>
       </c>
-      <c r="C54" s="58" t="s">
+      <c r="D54" s="52" t="s">
         <v>1103</v>
       </c>
-      <c r="D54" s="52" t="s">
+      <c r="E54" s="52" t="s">
         <v>1104</v>
       </c>
-      <c r="E54" s="52" t="s">
+      <c r="F54" s="52" t="s">
         <v>1105</v>
-      </c>
-      <c r="F54" s="52" t="s">
-        <v>1106</v>
       </c>
       <c r="G54" s="57"/>
       <c r="H54" s="51"/>
@@ -14047,19 +14047,19 @@
         <v>49</v>
       </c>
       <c r="B55" s="57" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="C55" s="58" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D55" s="52" t="s">
         <v>1092</v>
-      </c>
-      <c r="D55" s="52" t="s">
-        <v>1093</v>
       </c>
       <c r="E55" s="52"/>
       <c r="F55" s="52"/>
       <c r="G55" s="57"/>
       <c r="H55" s="57" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="I55" s="57"/>
     </row>
@@ -14068,19 +14068,19 @@
         <v>49</v>
       </c>
       <c r="B56" s="57" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C56" s="58" t="s">
         <v>1109</v>
       </c>
-      <c r="C56" s="58" t="s">
+      <c r="D56" s="52" t="s">
         <v>1110</v>
-      </c>
-      <c r="D56" s="52" t="s">
-        <v>1111</v>
       </c>
       <c r="E56" s="52"/>
       <c r="F56" s="52"/>
       <c r="G56" s="57"/>
       <c r="H56" s="57" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="I56" s="57"/>
     </row>
@@ -14089,19 +14089,19 @@
         <v>49</v>
       </c>
       <c r="B57" s="57" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C57" s="58" t="s">
         <v>1112</v>
       </c>
-      <c r="C57" s="58" t="s">
+      <c r="D57" s="52" t="s">
         <v>1113</v>
-      </c>
-      <c r="D57" s="52" t="s">
-        <v>1114</v>
       </c>
       <c r="E57" s="52"/>
       <c r="F57" s="52"/>
       <c r="G57" s="57"/>
       <c r="H57" s="57" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="I57" s="57"/>
     </row>
@@ -14110,13 +14110,13 @@
         <v>312</v>
       </c>
       <c r="B58" s="57" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C58" s="58" t="s">
         <v>1115</v>
       </c>
-      <c r="C58" s="58" t="s">
+      <c r="D58" s="52" t="s">
         <v>1116</v>
-      </c>
-      <c r="D58" s="52" t="s">
-        <v>1117</v>
       </c>
       <c r="E58" s="52"/>
       <c r="F58" s="52"/>
@@ -14129,19 +14129,19 @@
         <v>49</v>
       </c>
       <c r="B59" s="57" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="C59" s="58" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D59" s="52" t="s">
         <v>1092</v>
-      </c>
-      <c r="D59" s="52" t="s">
-        <v>1093</v>
       </c>
       <c r="E59" s="52"/>
       <c r="F59" s="52"/>
       <c r="G59" s="57"/>
       <c r="H59" s="51" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="I59" s="51"/>
     </row>
@@ -14150,19 +14150,19 @@
         <v>49</v>
       </c>
       <c r="B60" s="57" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C60" s="58" t="s">
         <v>1120</v>
       </c>
-      <c r="C60" s="58" t="s">
+      <c r="D60" s="52" t="s">
         <v>1121</v>
-      </c>
-      <c r="D60" s="52" t="s">
-        <v>1122</v>
       </c>
       <c r="E60" s="52"/>
       <c r="F60" s="52"/>
       <c r="G60" s="57"/>
       <c r="H60" s="51" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="I60" s="51"/>
     </row>
@@ -14171,19 +14171,19 @@
         <v>49</v>
       </c>
       <c r="B61" s="57" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C61" s="58" t="s">
         <v>1123</v>
       </c>
-      <c r="C61" s="58" t="s">
+      <c r="D61" s="52" t="s">
         <v>1124</v>
-      </c>
-      <c r="D61" s="52" t="s">
-        <v>1125</v>
       </c>
       <c r="E61" s="52"/>
       <c r="F61" s="52"/>
       <c r="G61" s="57"/>
       <c r="H61" s="51" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="I61" s="57"/>
     </row>
@@ -14192,13 +14192,13 @@
         <v>312</v>
       </c>
       <c r="B62" s="57" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C62" s="58" t="s">
         <v>1126</v>
       </c>
-      <c r="C62" s="58" t="s">
+      <c r="D62" s="52" t="s">
         <v>1127</v>
-      </c>
-      <c r="D62" s="52" t="s">
-        <v>1128</v>
       </c>
       <c r="E62" s="52"/>
       <c r="F62" s="52"/>
@@ -14212,34 +14212,34 @@
         <v>49</v>
       </c>
       <c r="B63" s="57" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="C63" s="58" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D63" s="52" t="s">
         <v>1092</v>
-      </c>
-      <c r="D63" s="52" t="s">
-        <v>1093</v>
       </c>
       <c r="E63" s="52"/>
       <c r="F63" s="52"/>
       <c r="G63" s="57"/>
       <c r="H63" s="57" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="I63" s="57"/>
     </row>
     <row r="64" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A64" s="57" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B64" s="57" t="s">
         <v>1131</v>
       </c>
-      <c r="B64" s="57" t="s">
+      <c r="C64" s="58" t="s">
         <v>1132</v>
       </c>
-      <c r="C64" s="58" t="s">
+      <c r="D64" s="52" t="s">
         <v>1133</v>
-      </c>
-      <c r="D64" s="52" t="s">
-        <v>1134</v>
       </c>
       <c r="E64" s="52"/>
       <c r="F64" s="52"/>
@@ -14255,19 +14255,19 @@
         <v>39</v>
       </c>
       <c r="B65" s="57" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C65" s="58" t="s">
         <v>1135</v>
       </c>
-      <c r="C65" s="58" t="s">
+      <c r="D65" s="52" t="s">
         <v>1136</v>
-      </c>
-      <c r="D65" s="52" t="s">
-        <v>1137</v>
       </c>
       <c r="E65" s="52"/>
       <c r="F65" s="52"/>
       <c r="G65" s="57"/>
       <c r="H65" s="57" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="I65" s="57"/>
       <c r="J65" s="57"/>
@@ -14279,19 +14279,19 @@
         <v>39</v>
       </c>
       <c r="B66" s="57" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C66" s="58" t="s">
         <v>1139</v>
       </c>
-      <c r="C66" s="58" t="s">
+      <c r="D66" s="52" t="s">
         <v>1140</v>
       </c>
-      <c r="D66" s="52" t="s">
+      <c r="E66" s="52" t="s">
         <v>1141</v>
       </c>
-      <c r="E66" s="52" t="s">
+      <c r="F66" s="52" t="s">
         <v>1142</v>
-      </c>
-      <c r="F66" s="52" t="s">
-        <v>1143</v>
       </c>
       <c r="G66" s="57"/>
       <c r="H66" s="57"/>
@@ -14305,13 +14305,13 @@
         <v>312</v>
       </c>
       <c r="B67" s="57" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C67" s="58" t="s">
         <v>1144</v>
       </c>
-      <c r="C67" s="58" t="s">
+      <c r="D67" s="53" t="s">
         <v>1145</v>
-      </c>
-      <c r="D67" s="53" t="s">
-        <v>1146</v>
       </c>
       <c r="E67" s="38"/>
       <c r="F67" s="38"/>
@@ -14327,19 +14327,19 @@
         <v>312</v>
       </c>
       <c r="B68" s="57" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C68" s="57" t="s">
         <v>1147</v>
       </c>
-      <c r="C68" s="57" t="s">
+      <c r="D68" s="53" t="s">
         <v>1148</v>
-      </c>
-      <c r="D68" s="53" t="s">
-        <v>1149</v>
       </c>
       <c r="E68" s="38"/>
       <c r="F68" s="38"/>
       <c r="G68" s="38"/>
       <c r="H68" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="I68" s="38"/>
       <c r="J68" s="38"/>
@@ -14351,19 +14351,19 @@
         <v>178</v>
       </c>
       <c r="B69" s="57" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C69" s="52" t="s">
         <v>1151</v>
       </c>
-      <c r="C69" s="52" t="s">
+      <c r="D69" s="53" t="s">
         <v>1152</v>
-      </c>
-      <c r="D69" s="53" t="s">
-        <v>1153</v>
       </c>
       <c r="E69" s="38"/>
       <c r="F69" s="38"/>
       <c r="G69" s="38"/>
       <c r="H69" s="57" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="I69" s="38"/>
       <c r="J69" s="38"/>
@@ -14394,16 +14394,16 @@
         <v>316</v>
       </c>
       <c r="C71" s="57" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D71" s="53" t="s">
         <v>1155</v>
-      </c>
-      <c r="D71" s="53" t="s">
-        <v>1156</v>
       </c>
       <c r="E71" s="38"/>
       <c r="F71" s="38"/>
       <c r="G71" s="38"/>
       <c r="H71" s="57" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="I71" s="38"/>
       <c r="J71" s="38"/>
@@ -14415,13 +14415,13 @@
         <v>178</v>
       </c>
       <c r="B72" s="57" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C72" s="57" t="s">
         <v>1158</v>
       </c>
-      <c r="C72" s="57" t="s">
+      <c r="D72" s="51" t="s">
         <v>1159</v>
-      </c>
-      <c r="D72" s="51" t="s">
-        <v>1160</v>
       </c>
       <c r="E72" s="38"/>
       <c r="F72" s="38"/>
@@ -14434,16 +14434,16 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="51" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B73" s="51" t="s">
         <v>1161</v>
       </c>
-      <c r="B73" s="51" t="s">
+      <c r="C73" s="51" t="s">
         <v>1162</v>
       </c>
-      <c r="C73" s="51" t="s">
-        <v>1163</v>
-      </c>
       <c r="D73" s="51" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="E73" s="38"/>
       <c r="F73" s="38"/>
@@ -14459,19 +14459,19 @@
         <v>67</v>
       </c>
       <c r="B74" s="51" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C74" s="51" t="s">
         <v>1164</v>
       </c>
-      <c r="C74" s="51" t="s">
+      <c r="D74" s="51" t="s">
         <v>1165</v>
-      </c>
-      <c r="D74" s="51" t="s">
-        <v>1166</v>
       </c>
       <c r="E74" s="38"/>
       <c r="F74" s="38"/>
       <c r="G74" s="38"/>
       <c r="H74" s="57" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="I74" s="38"/>
       <c r="J74" s="38"/>
@@ -14480,16 +14480,16 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B75" s="51" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C75" s="51" t="s">
         <v>1168</v>
       </c>
-      <c r="C75" s="51" t="s">
-        <v>1169</v>
-      </c>
       <c r="D75" s="51" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="E75" s="38"/>
       <c r="F75" s="38"/>
@@ -14505,19 +14505,19 @@
         <v>67</v>
       </c>
       <c r="B76" s="51" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C76" s="51" t="s">
         <v>1170</v>
       </c>
-      <c r="C76" s="51" t="s">
+      <c r="D76" s="51" t="s">
         <v>1171</v>
-      </c>
-      <c r="D76" s="51" t="s">
-        <v>1172</v>
       </c>
       <c r="E76" s="38"/>
       <c r="F76" s="38"/>
       <c r="G76" s="38"/>
       <c r="H76" s="57" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="I76" s="38"/>
       <c r="J76" s="38"/>
@@ -14526,16 +14526,16 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B77" s="51" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C77" s="51" t="s">
         <v>1174</v>
       </c>
-      <c r="C77" s="51" t="s">
-        <v>1175</v>
-      </c>
       <c r="D77" s="51" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="E77" s="38"/>
       <c r="F77" s="38"/>
@@ -14551,19 +14551,19 @@
         <v>67</v>
       </c>
       <c r="B78" s="51" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C78" s="51" t="s">
         <v>1176</v>
       </c>
-      <c r="C78" s="51" t="s">
+      <c r="D78" s="57" t="s">
         <v>1177</v>
-      </c>
-      <c r="D78" s="57" t="s">
-        <v>1178</v>
       </c>
       <c r="E78" s="38"/>
       <c r="F78" s="38"/>
       <c r="G78" s="38"/>
       <c r="H78" s="57" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="I78" s="38"/>
       <c r="J78" s="38"/>
@@ -14572,16 +14572,16 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B79" s="51" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C79" s="51" t="s">
         <v>1180</v>
       </c>
-      <c r="C79" s="51" t="s">
-        <v>1181</v>
-      </c>
       <c r="D79" s="51" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E79" s="38"/>
       <c r="F79" s="38"/>
@@ -14593,33 +14593,33 @@
         <v>67</v>
       </c>
       <c r="B80" s="51" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C80" s="51" t="s">
         <v>1182</v>
       </c>
-      <c r="C80" s="51" t="s">
+      <c r="D80" s="51" t="s">
         <v>1183</v>
-      </c>
-      <c r="D80" s="51" t="s">
-        <v>1184</v>
       </c>
       <c r="E80" s="38"/>
       <c r="F80" s="38"/>
       <c r="G80" s="38"/>
       <c r="H80" s="57" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B81" s="51" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C81" s="51" t="s">
         <v>1186</v>
       </c>
-      <c r="C81" s="51" t="s">
+      <c r="D81" s="51" t="s">
         <v>1187</v>
-      </c>
-      <c r="D81" s="51" t="s">
-        <v>1188</v>
       </c>
       <c r="E81" s="38"/>
       <c r="F81" s="38"/>
@@ -14631,33 +14631,33 @@
         <v>67</v>
       </c>
       <c r="B82" s="51" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C82" s="51" t="s">
         <v>1189</v>
       </c>
-      <c r="C82" s="51" t="s">
+      <c r="D82" s="51" t="s">
         <v>1190</v>
-      </c>
-      <c r="D82" s="51" t="s">
-        <v>1191</v>
       </c>
       <c r="E82" s="38"/>
       <c r="F82" s="38"/>
       <c r="G82" s="38"/>
       <c r="H82" s="57" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B83" s="51" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C83" s="51" t="s">
         <v>1193</v>
       </c>
-      <c r="C83" s="51" t="s">
+      <c r="D83" s="51" t="s">
         <v>1194</v>
-      </c>
-      <c r="D83" s="51" t="s">
-        <v>1195</v>
       </c>
       <c r="E83" s="38"/>
       <c r="F83" s="38"/>
@@ -14669,33 +14669,33 @@
         <v>67</v>
       </c>
       <c r="B84" s="51" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C84" s="51" t="s">
         <v>1196</v>
       </c>
-      <c r="C84" s="51" t="s">
+      <c r="D84" s="51" t="s">
         <v>1197</v>
-      </c>
-      <c r="D84" s="51" t="s">
-        <v>1198</v>
       </c>
       <c r="E84" s="38"/>
       <c r="F84" s="38"/>
       <c r="G84" s="38"/>
       <c r="H84" s="57" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B85" s="51" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C85" s="51" t="s">
         <v>1200</v>
       </c>
-      <c r="C85" s="51" t="s">
+      <c r="D85" s="57" t="s">
         <v>1201</v>
-      </c>
-      <c r="D85" s="57" t="s">
-        <v>1202</v>
       </c>
       <c r="E85" s="38"/>
       <c r="F85" s="38"/>
@@ -14707,33 +14707,33 @@
         <v>67</v>
       </c>
       <c r="B86" s="51" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C86" s="57" t="s">
         <v>1203</v>
       </c>
-      <c r="C86" s="57" t="s">
+      <c r="D86" s="58" t="s">
         <v>1204</v>
-      </c>
-      <c r="D86" s="58" t="s">
-        <v>1205</v>
       </c>
       <c r="E86" s="38"/>
       <c r="F86" s="38"/>
       <c r="G86" s="38"/>
       <c r="H86" s="57" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B87" s="51" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C87" s="51" t="s">
         <v>1207</v>
       </c>
-      <c r="C87" s="51" t="s">
+      <c r="D87" s="58" t="s">
         <v>1208</v>
-      </c>
-      <c r="D87" s="58" t="s">
-        <v>1209</v>
       </c>
       <c r="E87" s="38"/>
       <c r="F87" s="38"/>
@@ -14745,33 +14745,33 @@
         <v>67</v>
       </c>
       <c r="B88" s="51" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C88" s="51" t="s">
         <v>1210</v>
       </c>
-      <c r="C88" s="51" t="s">
+      <c r="D88" s="51" t="s">
         <v>1211</v>
-      </c>
-      <c r="D88" s="51" t="s">
-        <v>1212</v>
       </c>
       <c r="E88" s="38"/>
       <c r="F88" s="38"/>
       <c r="G88" s="38"/>
       <c r="H88" s="57" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B89" s="51" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C89" s="51" t="s">
         <v>1214</v>
       </c>
-      <c r="C89" s="51" t="s">
+      <c r="D89" s="57" t="s">
         <v>1215</v>
-      </c>
-      <c r="D89" s="57" t="s">
-        <v>1216</v>
       </c>
       <c r="E89" s="38"/>
       <c r="F89" s="38"/>
@@ -14783,33 +14783,33 @@
         <v>67</v>
       </c>
       <c r="B90" s="51" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C90" s="57" t="s">
         <v>1217</v>
       </c>
-      <c r="C90" s="57" t="s">
+      <c r="D90" s="57" t="s">
         <v>1218</v>
-      </c>
-      <c r="D90" s="57" t="s">
-        <v>1219</v>
       </c>
       <c r="E90" s="38"/>
       <c r="F90" s="38"/>
       <c r="G90" s="38"/>
       <c r="H90" s="57" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B91" s="57" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C91" s="57" t="s">
         <v>1221</v>
       </c>
-      <c r="C91" s="57" t="s">
-        <v>1222</v>
-      </c>
       <c r="D91" s="57" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="E91" s="38"/>
       <c r="F91" s="38"/>
@@ -14821,33 +14821,33 @@
         <v>67</v>
       </c>
       <c r="B92" s="51" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C92" s="57" t="s">
         <v>1223</v>
       </c>
-      <c r="C92" s="57" t="s">
+      <c r="D92" s="38" t="s">
         <v>1224</v>
-      </c>
-      <c r="D92" s="38" t="s">
-        <v>1225</v>
       </c>
       <c r="E92" s="38"/>
       <c r="F92" s="38"/>
       <c r="G92" s="38"/>
       <c r="H92" s="57" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B93" s="57" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C93" s="57" t="s">
         <v>1227</v>
       </c>
-      <c r="C93" s="57" t="s">
-        <v>1228</v>
-      </c>
       <c r="D93" s="38" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="E93" s="38"/>
       <c r="F93" s="38"/>
@@ -14859,33 +14859,33 @@
         <v>67</v>
       </c>
       <c r="B94" s="51" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C94" s="57" t="s">
         <v>1229</v>
       </c>
-      <c r="C94" s="57" t="s">
+      <c r="D94" s="38" t="s">
         <v>1230</v>
-      </c>
-      <c r="D94" s="38" t="s">
-        <v>1231</v>
       </c>
       <c r="E94" s="38"/>
       <c r="F94" s="38"/>
       <c r="G94" s="38"/>
       <c r="H94" s="57" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B95" s="57" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C95" s="57" t="s">
         <v>1233</v>
       </c>
-      <c r="C95" s="57" t="s">
-        <v>1234</v>
-      </c>
       <c r="D95" s="38" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="E95" s="38"/>
       <c r="F95" s="38"/>
@@ -14897,33 +14897,33 @@
         <v>67</v>
       </c>
       <c r="B96" s="51" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C96" s="57" t="s">
         <v>1235</v>
       </c>
-      <c r="C96" s="57" t="s">
+      <c r="D96" s="38" t="s">
         <v>1236</v>
-      </c>
-      <c r="D96" s="38" t="s">
-        <v>1237</v>
       </c>
       <c r="E96" s="38"/>
       <c r="F96" s="38"/>
       <c r="G96" s="38"/>
       <c r="H96" s="57" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B97" s="57" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C97" s="57" t="s">
         <v>1239</v>
       </c>
-      <c r="C97" s="57" t="s">
+      <c r="D97" s="38" t="s">
         <v>1240</v>
-      </c>
-      <c r="D97" s="38" t="s">
-        <v>1241</v>
       </c>
       <c r="E97" s="38"/>
       <c r="F97" s="38"/>
@@ -14935,33 +14935,33 @@
         <v>67</v>
       </c>
       <c r="B98" s="57" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C98" s="57" t="s">
         <v>1242</v>
       </c>
-      <c r="C98" s="57" t="s">
+      <c r="D98" s="38" t="s">
         <v>1243</v>
-      </c>
-      <c r="D98" s="38" t="s">
-        <v>1244</v>
       </c>
       <c r="E98" s="38"/>
       <c r="F98" s="38"/>
       <c r="G98" s="38"/>
       <c r="H98" s="57" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B99" s="57" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C99" s="57" t="s">
         <v>1246</v>
       </c>
-      <c r="C99" s="57" t="s">
-        <v>1247</v>
-      </c>
       <c r="D99" s="38" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="E99" s="38"/>
       <c r="F99" s="38"/>
@@ -14973,33 +14973,33 @@
         <v>67</v>
       </c>
       <c r="B100" s="57" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C100" s="57" t="s">
         <v>1248</v>
       </c>
-      <c r="C100" s="57" t="s">
+      <c r="D100" s="38" t="s">
         <v>1249</v>
-      </c>
-      <c r="D100" s="38" t="s">
-        <v>1250</v>
       </c>
       <c r="E100" s="38"/>
       <c r="F100" s="38"/>
       <c r="G100" s="38"/>
       <c r="H100" s="57" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B101" s="57" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C101" s="57" t="s">
         <v>1252</v>
       </c>
-      <c r="C101" s="57" t="s">
-        <v>1253</v>
-      </c>
       <c r="D101" s="38" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="E101" s="38"/>
       <c r="F101" s="38"/>
@@ -15011,33 +15011,33 @@
         <v>67</v>
       </c>
       <c r="B102" s="57" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C102" s="57" t="s">
         <v>1254</v>
       </c>
-      <c r="C102" s="57" t="s">
+      <c r="D102" s="38" t="s">
         <v>1255</v>
-      </c>
-      <c r="D102" s="38" t="s">
-        <v>1256</v>
       </c>
       <c r="E102" s="38"/>
       <c r="F102" s="38"/>
       <c r="G102" s="38"/>
       <c r="H102" s="57" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B103" s="57" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C103" s="57" t="s">
         <v>1258</v>
       </c>
-      <c r="C103" s="57" t="s">
-        <v>1259</v>
-      </c>
       <c r="D103" s="38" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="E103" s="38"/>
       <c r="F103" s="38"/>
@@ -15049,33 +15049,33 @@
         <v>67</v>
       </c>
       <c r="B104" s="57" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C104" s="57" t="s">
         <v>1260</v>
       </c>
-      <c r="C104" s="57" t="s">
+      <c r="D104" s="57" t="s">
         <v>1261</v>
-      </c>
-      <c r="D104" s="57" t="s">
-        <v>1262</v>
       </c>
       <c r="E104" s="38"/>
       <c r="F104" s="38"/>
       <c r="G104" s="38"/>
       <c r="H104" s="57" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B105" s="57" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C105" s="57" t="s">
         <v>1264</v>
       </c>
-      <c r="C105" s="57" t="s">
+      <c r="D105" s="38" t="s">
         <v>1265</v>
-      </c>
-      <c r="D105" s="38" t="s">
-        <v>1266</v>
       </c>
       <c r="E105" s="38"/>
       <c r="F105" s="38"/>
@@ -15087,33 +15087,33 @@
         <v>67</v>
       </c>
       <c r="B106" s="57" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C106" s="57" t="s">
         <v>1267</v>
       </c>
-      <c r="C106" s="57" t="s">
+      <c r="D106" s="38" t="s">
         <v>1268</v>
-      </c>
-      <c r="D106" s="38" t="s">
-        <v>1269</v>
       </c>
       <c r="E106" s="38"/>
       <c r="F106" s="38"/>
       <c r="G106" s="38"/>
       <c r="H106" s="57" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B107" s="57" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C107" s="57" t="s">
         <v>1271</v>
       </c>
-      <c r="C107" s="57" t="s">
+      <c r="D107" s="38" t="s">
         <v>1272</v>
-      </c>
-      <c r="D107" s="38" t="s">
-        <v>1273</v>
       </c>
       <c r="E107" s="38"/>
       <c r="F107" s="38"/>
@@ -15125,33 +15125,33 @@
         <v>67</v>
       </c>
       <c r="B108" s="57" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C108" s="57" t="s">
         <v>1274</v>
       </c>
-      <c r="C108" s="57" t="s">
+      <c r="D108" s="38" t="s">
         <v>1275</v>
-      </c>
-      <c r="D108" s="38" t="s">
-        <v>1276</v>
       </c>
       <c r="E108" s="38"/>
       <c r="F108" s="38"/>
       <c r="G108" s="38"/>
       <c r="H108" s="57" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B109" s="57" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C109" s="57" t="s">
         <v>1278</v>
       </c>
-      <c r="C109" s="57" t="s">
-        <v>1279</v>
-      </c>
       <c r="D109" s="38" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E109" s="38"/>
       <c r="F109" s="38"/>
@@ -15163,33 +15163,33 @@
         <v>67</v>
       </c>
       <c r="B110" s="57" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C110" s="57" t="s">
         <v>1280</v>
       </c>
-      <c r="C110" s="57" t="s">
+      <c r="D110" s="38" t="s">
         <v>1281</v>
-      </c>
-      <c r="D110" s="38" t="s">
-        <v>1282</v>
       </c>
       <c r="E110" s="38"/>
       <c r="F110" s="38"/>
       <c r="G110" s="38"/>
       <c r="H110" s="57" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B111" s="57" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C111" s="57" t="s">
         <v>1284</v>
       </c>
-      <c r="C111" s="57" t="s">
+      <c r="D111" s="38" t="s">
         <v>1285</v>
-      </c>
-      <c r="D111" s="38" t="s">
-        <v>1286</v>
       </c>
       <c r="E111" s="38"/>
       <c r="F111" s="38"/>
@@ -15201,33 +15201,33 @@
         <v>67</v>
       </c>
       <c r="B112" s="57" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C112" s="57" t="s">
         <v>1287</v>
       </c>
-      <c r="C112" s="57" t="s">
+      <c r="D112" s="38" t="s">
         <v>1288</v>
-      </c>
-      <c r="D112" s="38" t="s">
-        <v>1289</v>
       </c>
       <c r="E112" s="38"/>
       <c r="F112" s="38"/>
       <c r="G112" s="38"/>
       <c r="H112" s="57" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B113" s="57" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C113" s="57" t="s">
         <v>1291</v>
       </c>
-      <c r="C113" s="57" t="s">
+      <c r="D113" s="38" t="s">
         <v>1292</v>
-      </c>
-      <c r="D113" s="38" t="s">
-        <v>1293</v>
       </c>
       <c r="E113" s="38"/>
       <c r="F113" s="38"/>
@@ -15239,33 +15239,33 @@
         <v>67</v>
       </c>
       <c r="B114" s="57" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C114" s="57" t="s">
         <v>1294</v>
       </c>
-      <c r="C114" s="57" t="s">
+      <c r="D114" s="38" t="s">
         <v>1295</v>
-      </c>
-      <c r="D114" s="38" t="s">
-        <v>1296</v>
       </c>
       <c r="E114" s="38"/>
       <c r="F114" s="38"/>
       <c r="G114" s="38"/>
       <c r="H114" s="57" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="51" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B115" s="57" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C115" s="57" t="s">
         <v>1298</v>
       </c>
-      <c r="C115" s="57" t="s">
+      <c r="D115" s="38" t="s">
         <v>1299</v>
-      </c>
-      <c r="D115" s="38" t="s">
-        <v>1300</v>
       </c>
       <c r="E115" s="38"/>
       <c r="F115" s="38"/>
@@ -15277,19 +15277,19 @@
         <v>67</v>
       </c>
       <c r="B116" s="57" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C116" s="57" t="s">
         <v>1301</v>
       </c>
-      <c r="C116" s="57" t="s">
+      <c r="D116" s="38" t="s">
         <v>1302</v>
-      </c>
-      <c r="D116" s="38" t="s">
-        <v>1303</v>
       </c>
       <c r="E116" s="38"/>
       <c r="F116" s="38"/>
       <c r="G116" s="38"/>
       <c r="H116" s="57" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -15297,13 +15297,13 @@
         <v>178</v>
       </c>
       <c r="B117" s="57" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C117" s="52" t="s">
         <v>1305</v>
       </c>
-      <c r="C117" s="52" t="s">
+      <c r="D117" s="53" t="s">
         <v>1306</v>
-      </c>
-      <c r="D117" s="53" t="s">
-        <v>1307</v>
       </c>
       <c r="E117" s="38"/>
       <c r="F117" s="38"/>
@@ -15315,13 +15315,13 @@
         <v>312</v>
       </c>
       <c r="B118" s="57" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="C118" s="57" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D118" s="38" t="s">
         <v>1148</v>
-      </c>
-      <c r="D118" s="38" t="s">
-        <v>1149</v>
       </c>
       <c r="E118" s="38"/>
       <c r="F118" s="38"/>
@@ -15348,16 +15348,16 @@
         <v>315</v>
       </c>
       <c r="C120" s="57" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D120" s="38" t="s">
         <v>1309</v>
-      </c>
-      <c r="D120" s="38" t="s">
-        <v>1310</v>
       </c>
       <c r="E120" s="38"/>
       <c r="F120" s="38"/>
       <c r="G120" s="38"/>
       <c r="H120" s="57" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
@@ -15365,13 +15365,13 @@
         <v>178</v>
       </c>
       <c r="B121" s="57" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C121" s="57" t="s">
         <v>1312</v>
       </c>
-      <c r="C121" s="57" t="s">
+      <c r="D121" s="57" t="s">
         <v>1313</v>
-      </c>
-      <c r="D121" s="57" t="s">
-        <v>1314</v>
       </c>
       <c r="E121" s="38"/>
       <c r="F121" s="38"/>
@@ -15380,16 +15380,16 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="57" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B122" s="57" t="s">
         <v>1315</v>
       </c>
-      <c r="B122" s="57" t="s">
+      <c r="C122" s="57" t="s">
         <v>1316</v>
       </c>
-      <c r="C122" s="57" t="s">
+      <c r="D122" s="38" t="s">
         <v>1317</v>
-      </c>
-      <c r="D122" s="38" t="s">
-        <v>1318</v>
       </c>
       <c r="E122" s="38"/>
       <c r="F122" s="38"/>
@@ -15401,19 +15401,19 @@
         <v>39</v>
       </c>
       <c r="B123" s="57" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C123" s="57" t="s">
         <v>1319</v>
       </c>
-      <c r="C123" s="57" t="s">
+      <c r="D123" s="38" t="s">
         <v>1320</v>
-      </c>
-      <c r="D123" s="38" t="s">
-        <v>1321</v>
       </c>
       <c r="E123" s="38"/>
       <c r="F123" s="38"/>
       <c r="G123" s="38"/>
       <c r="H123" s="57" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
@@ -15920,128 +15920,128 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="64" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="B33" s="64" t="s">
         <v>1065</v>
       </c>
       <c r="C33" s="64" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D33" s="61" t="s">
         <v>1324</v>
-      </c>
-      <c r="D33" s="61" t="s">
-        <v>1325</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="64" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="B34" s="64" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C34" s="64" t="s">
         <v>1326</v>
       </c>
-      <c r="C34" s="64" t="s">
+      <c r="D34" s="61" t="s">
         <v>1327</v>
-      </c>
-      <c r="D34" s="61" t="s">
-        <v>1328</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="64" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="B35" s="64" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C35" s="64" t="s">
         <v>1329</v>
       </c>
-      <c r="C35" s="64" t="s">
+      <c r="D35" s="61" t="s">
         <v>1330</v>
-      </c>
-      <c r="D35" s="61" t="s">
-        <v>1331</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="64" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B36" s="64" t="s">
         <v>1332</v>
       </c>
-      <c r="B36" s="64" t="s">
+      <c r="C36" s="64" t="s">
         <v>1333</v>
       </c>
-      <c r="C36" s="64" t="s">
+      <c r="D36" s="61" t="s">
         <v>1334</v>
-      </c>
-      <c r="D36" s="61" t="s">
-        <v>1335</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="64" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B37" s="64" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C37" s="64" t="s">
         <v>1336</v>
       </c>
-      <c r="C37" s="64" t="s">
+      <c r="D37" s="61" t="s">
         <v>1337</v>
-      </c>
-      <c r="D37" s="61" t="s">
-        <v>1338</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="64" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B38" s="64" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C38" s="64" t="s">
         <v>1339</v>
       </c>
-      <c r="C38" s="64" t="s">
+      <c r="D38" s="61" t="s">
         <v>1340</v>
-      </c>
-      <c r="D38" s="61" t="s">
-        <v>1341</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="64" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B39" s="64" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C39" s="64" t="s">
         <v>1342</v>
       </c>
-      <c r="C39" s="64" t="s">
+      <c r="D39" s="61" t="s">
         <v>1343</v>
-      </c>
-      <c r="D39" s="61" t="s">
-        <v>1344</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="64" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B40" s="64" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C40" s="64" t="s">
         <v>1345</v>
       </c>
-      <c r="C40" s="64" t="s">
+      <c r="D40" s="61" t="s">
         <v>1346</v>
-      </c>
-      <c r="D40" s="61" t="s">
-        <v>1347</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="64" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B41" s="64" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C41" s="64" t="s">
         <v>1348</v>
       </c>
-      <c r="C41" s="64" t="s">
+      <c r="D41" s="61" t="s">
         <v>1349</v>
-      </c>
-      <c r="D41" s="61" t="s">
-        <v>1350</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -16049,13 +16049,13 @@
         <v>1044</v>
       </c>
       <c r="B42" s="64" t="s">
+        <v>1350</v>
+      </c>
+      <c r="C42" s="64" t="s">
         <v>1351</v>
       </c>
-      <c r="C42" s="64" t="s">
+      <c r="D42" s="64" t="s">
         <v>1352</v>
-      </c>
-      <c r="D42" s="64" t="s">
-        <v>1353</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -16063,13 +16063,13 @@
         <v>1044</v>
       </c>
       <c r="B43" s="64" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C43" s="64" t="s">
         <v>1354</v>
       </c>
-      <c r="C43" s="64" t="s">
+      <c r="D43" s="64" t="s">
         <v>1355</v>
-      </c>
-      <c r="D43" s="64" t="s">
-        <v>1356</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -16088,35 +16088,35 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="64" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B45" s="64" t="s">
         <v>1357</v>
       </c>
-      <c r="B45" s="64" t="s">
+      <c r="C45" s="64" t="s">
         <v>1358</v>
       </c>
-      <c r="C45" s="64" t="s">
+      <c r="D45" s="61" t="s">
         <v>1359</v>
-      </c>
-      <c r="D45" s="61" t="s">
-        <v>1360</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B46" s="64" t="s">
         <v>366</v>
       </c>
       <c r="C46" s="64" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D46" s="61" t="s">
         <v>1361</v>
-      </c>
-      <c r="D46" s="61" t="s">
-        <v>1362</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B47" s="64" t="s">
         <v>365</v>
@@ -16130,7 +16130,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B48" s="64" t="s">
         <v>362</v>
@@ -16144,10 +16144,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B49" s="64" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="C49" s="64" t="s">
         <v>30</v>
@@ -16158,10 +16158,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B50" s="64" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="C50" s="64" t="s">
         <v>31</v>
@@ -16172,24 +16172,24 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B51" s="64" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="C51" s="64" t="s">
         <v>358</v>
       </c>
       <c r="D51" s="61" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B52" s="64" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="C52" s="64" t="s">
         <v>32</v>
@@ -16200,66 +16200,66 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B53" s="64" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C53" s="64" t="s">
         <v>1368</v>
       </c>
-      <c r="C53" s="64" t="s">
+      <c r="D53" s="61" t="s">
         <v>1369</v>
-      </c>
-      <c r="D53" s="61" t="s">
-        <v>1370</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B54" s="64" t="s">
+        <v>1370</v>
+      </c>
+      <c r="C54" s="64" t="s">
         <v>1371</v>
       </c>
-      <c r="C54" s="64" t="s">
+      <c r="D54" s="61" t="s">
         <v>1372</v>
-      </c>
-      <c r="D54" s="61" t="s">
-        <v>1373</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B55" s="64" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C55" s="64" t="s">
         <v>1374</v>
       </c>
-      <c r="C55" s="64" t="s">
+      <c r="D55" s="61" t="s">
         <v>1375</v>
-      </c>
-      <c r="D55" s="61" t="s">
-        <v>1376</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B56" s="64" t="s">
         <v>877</v>
       </c>
       <c r="C56" s="64" t="s">
+        <v>1376</v>
+      </c>
+      <c r="D56" s="61" t="s">
         <v>1377</v>
-      </c>
-      <c r="D56" s="61" t="s">
-        <v>1378</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B57" s="64" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="C57" s="64" t="s">
         <v>33</v>
@@ -16270,21 +16270,21 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B58" s="64" t="s">
+        <v>1379</v>
+      </c>
+      <c r="C58" s="64" t="s">
         <v>1380</v>
       </c>
-      <c r="C58" s="64" t="s">
+      <c r="D58" s="61" t="s">
         <v>1381</v>
-      </c>
-      <c r="D58" s="61" t="s">
-        <v>1382</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B59" s="64" t="s">
         <v>233</v>
@@ -16298,7 +16298,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="64" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B60" s="64" t="s">
         <v>245</v>

</xml_diff>

<commit_message>
remove num_ from vacc dict xlsx
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-survey-dict.xlsx
+++ b/inst/extdata/MSF-survey-dict.xlsx
@@ -3248,9 +3248,6 @@
     <t>L'enfant a-t-il déjà reçu une "goutte de vaccin dans la bouche" - c'est-à-dire un vaccin contre la polio ?</t>
   </si>
   <si>
-    <t>num_poliodrop_hf_woc</t>
-  </si>
-  <si>
     <t>How many times has the child received a polio drops vaccine at a health facility?</t>
   </si>
   <si>
@@ -3264,9 +3261,6 @@
   </si>
   <si>
     <t>${poliodrop_woc} = "yes"</t>
-  </si>
-  <si>
-    <t>num_poliodrop_camp_woc</t>
   </si>
   <si>
     <t>How many times has the child received a polio drops vaccine during a large campaign, usually involving a large group of children in the area and perhaps vaccinating at your house?</t>
@@ -4271,6 +4265,12 @@
   </si>
   <si>
     <t>num_quad_penta_woc</t>
+  </si>
+  <si>
+    <t>poliodrop_hf_woc</t>
+  </si>
+  <si>
+    <t>poliodrop_camp_woc</t>
   </si>
 </sst>
 </file>
@@ -5786,7 +5786,7 @@
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
       <c r="H43" s="9" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
@@ -6263,7 +6263,7 @@
       <c r="F68" s="14"/>
       <c r="G68" s="14"/>
       <c r="H68" s="13" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="I68" s="13"/>
     </row>
@@ -7291,7 +7291,7 @@
       <c r="F111" s="15"/>
       <c r="G111" s="15"/>
       <c r="H111" s="14" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="I111" s="15"/>
       <c r="J111" s="15"/>
@@ -7315,7 +7315,7 @@
       <c r="F112" s="15"/>
       <c r="G112" s="15"/>
       <c r="H112" s="14" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="I112" s="15"/>
       <c r="J112" s="15"/>
@@ -7339,7 +7339,7 @@
       <c r="F113" s="15"/>
       <c r="G113" s="15"/>
       <c r="H113" s="14" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="I113" s="15"/>
       <c r="J113" s="15"/>
@@ -12823,7 +12823,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
+      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13842,23 +13842,23 @@
         <v>49</v>
       </c>
       <c r="B46" s="51" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C46" s="58" t="s">
         <v>1072</v>
       </c>
-      <c r="C46" s="58" t="s">
+      <c r="D46" s="58" t="s">
         <v>1073</v>
       </c>
-      <c r="D46" s="58" t="s">
+      <c r="E46" s="52" t="s">
         <v>1074</v>
       </c>
-      <c r="E46" s="52" t="s">
+      <c r="F46" s="52" t="s">
         <v>1075</v>
-      </c>
-      <c r="F46" s="52" t="s">
-        <v>1076</v>
       </c>
       <c r="G46" s="57"/>
       <c r="H46" s="51" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="I46" s="57"/>
       <c r="J46" s="57"/>
@@ -13869,23 +13869,23 @@
         <v>49</v>
       </c>
       <c r="B47" s="51" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C47" s="58" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D47" s="58" t="s">
         <v>1078</v>
       </c>
-      <c r="C47" s="58" t="s">
-        <v>1079</v>
-      </c>
-      <c r="D47" s="58" t="s">
-        <v>1080</v>
-      </c>
       <c r="E47" s="52" t="s">
+        <v>1074</v>
+      </c>
+      <c r="F47" s="52" t="s">
         <v>1075</v>
-      </c>
-      <c r="F47" s="52" t="s">
-        <v>1076</v>
       </c>
       <c r="G47" s="57"/>
       <c r="H47" s="51" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="I47" s="57"/>
       <c r="J47" s="57"/>
@@ -13896,13 +13896,13 @@
         <v>312</v>
       </c>
       <c r="B48" s="57" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C48" s="58" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D48" s="52" t="s">
         <v>1081</v>
-      </c>
-      <c r="C48" s="58" t="s">
-        <v>1082</v>
-      </c>
-      <c r="D48" s="52" t="s">
-        <v>1083</v>
       </c>
       <c r="E48" s="52"/>
       <c r="F48" s="52"/>
@@ -13915,23 +13915,23 @@
         <v>49</v>
       </c>
       <c r="B49" s="57" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C49" s="58" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D49" s="52" t="s">
         <v>1084</v>
       </c>
-      <c r="C49" s="58" t="s">
-        <v>1085</v>
-      </c>
-      <c r="D49" s="52" t="s">
-        <v>1086</v>
-      </c>
       <c r="E49" s="52" t="s">
+        <v>1074</v>
+      </c>
+      <c r="F49" s="52" t="s">
         <v>1075</v>
-      </c>
-      <c r="F49" s="52" t="s">
-        <v>1076</v>
       </c>
       <c r="G49" s="57"/>
       <c r="H49" s="51" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="I49" s="57"/>
     </row>
@@ -13940,13 +13940,13 @@
         <v>312</v>
       </c>
       <c r="B50" s="57" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C50" s="58" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D50" s="52" t="s">
         <v>1088</v>
-      </c>
-      <c r="C50" s="58" t="s">
-        <v>1089</v>
-      </c>
-      <c r="D50" s="52" t="s">
-        <v>1090</v>
       </c>
       <c r="E50" s="52"/>
       <c r="F50" s="52"/>
@@ -13959,19 +13959,19 @@
         <v>49</v>
       </c>
       <c r="B51" s="57" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="C51" s="58" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="D51" s="52" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E51" s="52"/>
       <c r="F51" s="52"/>
       <c r="G51" s="57"/>
       <c r="H51" s="51" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="I51" s="51"/>
     </row>
@@ -13980,19 +13980,19 @@
         <v>312</v>
       </c>
       <c r="B52" s="57" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C52" s="58" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D52" s="52" t="s">
         <v>1094</v>
       </c>
-      <c r="C52" s="58" t="s">
+      <c r="E52" s="52" t="s">
         <v>1095</v>
       </c>
-      <c r="D52" s="52" t="s">
+      <c r="F52" s="52" t="s">
         <v>1096</v>
-      </c>
-      <c r="E52" s="52" t="s">
-        <v>1097</v>
-      </c>
-      <c r="F52" s="52" t="s">
-        <v>1098</v>
       </c>
       <c r="G52" s="57"/>
       <c r="H52" s="51"/>
@@ -14003,19 +14003,19 @@
         <v>49</v>
       </c>
       <c r="B53" s="57" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="C53" s="58" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="D53" s="52" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E53" s="52"/>
       <c r="F53" s="52"/>
       <c r="G53" s="57"/>
       <c r="H53" s="51" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="I53" s="57"/>
     </row>
@@ -14024,19 +14024,19 @@
         <v>312</v>
       </c>
       <c r="B54" s="57" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C54" s="58" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D54" s="52" t="s">
         <v>1101</v>
       </c>
-      <c r="C54" s="58" t="s">
+      <c r="E54" s="52" t="s">
         <v>1102</v>
       </c>
-      <c r="D54" s="52" t="s">
+      <c r="F54" s="52" t="s">
         <v>1103</v>
-      </c>
-      <c r="E54" s="52" t="s">
-        <v>1104</v>
-      </c>
-      <c r="F54" s="52" t="s">
-        <v>1105</v>
       </c>
       <c r="G54" s="57"/>
       <c r="H54" s="51"/>
@@ -14047,19 +14047,19 @@
         <v>49</v>
       </c>
       <c r="B55" s="57" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="C55" s="58" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="D55" s="52" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E55" s="52"/>
       <c r="F55" s="52"/>
       <c r="G55" s="57"/>
       <c r="H55" s="57" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="I55" s="57"/>
     </row>
@@ -14068,19 +14068,19 @@
         <v>49</v>
       </c>
       <c r="B56" s="57" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C56" s="58" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D56" s="52" t="s">
         <v>1108</v>
-      </c>
-      <c r="C56" s="58" t="s">
-        <v>1109</v>
-      </c>
-      <c r="D56" s="52" t="s">
-        <v>1110</v>
       </c>
       <c r="E56" s="52"/>
       <c r="F56" s="52"/>
       <c r="G56" s="57"/>
       <c r="H56" s="57" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="I56" s="57"/>
     </row>
@@ -14089,19 +14089,19 @@
         <v>49</v>
       </c>
       <c r="B57" s="57" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C57" s="58" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D57" s="52" t="s">
         <v>1111</v>
-      </c>
-      <c r="C57" s="58" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D57" s="52" t="s">
-        <v>1113</v>
       </c>
       <c r="E57" s="52"/>
       <c r="F57" s="52"/>
       <c r="G57" s="57"/>
       <c r="H57" s="57" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="I57" s="57"/>
     </row>
@@ -14110,13 +14110,13 @@
         <v>312</v>
       </c>
       <c r="B58" s="57" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C58" s="58" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D58" s="52" t="s">
         <v>1114</v>
-      </c>
-      <c r="C58" s="58" t="s">
-        <v>1115</v>
-      </c>
-      <c r="D58" s="52" t="s">
-        <v>1116</v>
       </c>
       <c r="E58" s="52"/>
       <c r="F58" s="52"/>
@@ -14129,19 +14129,19 @@
         <v>49</v>
       </c>
       <c r="B59" s="57" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="C59" s="58" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="D59" s="52" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E59" s="52"/>
       <c r="F59" s="52"/>
       <c r="G59" s="57"/>
       <c r="H59" s="51" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="I59" s="51"/>
     </row>
@@ -14150,19 +14150,19 @@
         <v>49</v>
       </c>
       <c r="B60" s="57" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C60" s="58" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D60" s="52" t="s">
         <v>1119</v>
-      </c>
-      <c r="C60" s="58" t="s">
-        <v>1120</v>
-      </c>
-      <c r="D60" s="52" t="s">
-        <v>1121</v>
       </c>
       <c r="E60" s="52"/>
       <c r="F60" s="52"/>
       <c r="G60" s="57"/>
       <c r="H60" s="51" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="I60" s="51"/>
     </row>
@@ -14171,19 +14171,19 @@
         <v>49</v>
       </c>
       <c r="B61" s="57" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C61" s="58" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D61" s="52" t="s">
         <v>1122</v>
-      </c>
-      <c r="C61" s="58" t="s">
-        <v>1123</v>
-      </c>
-      <c r="D61" s="52" t="s">
-        <v>1124</v>
       </c>
       <c r="E61" s="52"/>
       <c r="F61" s="52"/>
       <c r="G61" s="57"/>
       <c r="H61" s="51" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="I61" s="57"/>
     </row>
@@ -14192,13 +14192,13 @@
         <v>312</v>
       </c>
       <c r="B62" s="57" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C62" s="58" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D62" s="52" t="s">
         <v>1125</v>
-      </c>
-      <c r="C62" s="58" t="s">
-        <v>1126</v>
-      </c>
-      <c r="D62" s="52" t="s">
-        <v>1127</v>
       </c>
       <c r="E62" s="52"/>
       <c r="F62" s="52"/>
@@ -14212,34 +14212,34 @@
         <v>49</v>
       </c>
       <c r="B63" s="57" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="C63" s="58" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="D63" s="52" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E63" s="52"/>
       <c r="F63" s="52"/>
       <c r="G63" s="57"/>
       <c r="H63" s="57" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="I63" s="57"/>
     </row>
     <row r="64" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A64" s="57" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B64" s="57" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C64" s="58" t="s">
         <v>1130</v>
       </c>
-      <c r="B64" s="57" t="s">
+      <c r="D64" s="52" t="s">
         <v>1131</v>
-      </c>
-      <c r="C64" s="58" t="s">
-        <v>1132</v>
-      </c>
-      <c r="D64" s="52" t="s">
-        <v>1133</v>
       </c>
       <c r="E64" s="52"/>
       <c r="F64" s="52"/>
@@ -14255,19 +14255,19 @@
         <v>39</v>
       </c>
       <c r="B65" s="57" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C65" s="58" t="s">
+        <v>1133</v>
+      </c>
+      <c r="D65" s="52" t="s">
         <v>1134</v>
-      </c>
-      <c r="C65" s="58" t="s">
-        <v>1135</v>
-      </c>
-      <c r="D65" s="52" t="s">
-        <v>1136</v>
       </c>
       <c r="E65" s="52"/>
       <c r="F65" s="52"/>
       <c r="G65" s="57"/>
       <c r="H65" s="57" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="I65" s="57"/>
       <c r="J65" s="57"/>
@@ -14279,19 +14279,19 @@
         <v>39</v>
       </c>
       <c r="B66" s="57" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C66" s="58" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D66" s="52" t="s">
         <v>1138</v>
       </c>
-      <c r="C66" s="58" t="s">
+      <c r="E66" s="52" t="s">
         <v>1139</v>
       </c>
-      <c r="D66" s="52" t="s">
+      <c r="F66" s="52" t="s">
         <v>1140</v>
-      </c>
-      <c r="E66" s="52" t="s">
-        <v>1141</v>
-      </c>
-      <c r="F66" s="52" t="s">
-        <v>1142</v>
       </c>
       <c r="G66" s="57"/>
       <c r="H66" s="57"/>
@@ -14305,13 +14305,13 @@
         <v>312</v>
       </c>
       <c r="B67" s="57" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C67" s="58" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D67" s="53" t="s">
         <v>1143</v>
-      </c>
-      <c r="C67" s="58" t="s">
-        <v>1144</v>
-      </c>
-      <c r="D67" s="53" t="s">
-        <v>1145</v>
       </c>
       <c r="E67" s="38"/>
       <c r="F67" s="38"/>
@@ -14327,19 +14327,19 @@
         <v>312</v>
       </c>
       <c r="B68" s="57" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C68" s="57" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D68" s="53" t="s">
         <v>1146</v>
-      </c>
-      <c r="C68" s="57" t="s">
-        <v>1147</v>
-      </c>
-      <c r="D68" s="53" t="s">
-        <v>1148</v>
       </c>
       <c r="E68" s="38"/>
       <c r="F68" s="38"/>
       <c r="G68" s="38"/>
       <c r="H68" s="57" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="I68" s="38"/>
       <c r="J68" s="38"/>
@@ -14351,19 +14351,19 @@
         <v>178</v>
       </c>
       <c r="B69" s="57" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C69" s="52" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D69" s="53" t="s">
         <v>1150</v>
-      </c>
-      <c r="C69" s="52" t="s">
-        <v>1151</v>
-      </c>
-      <c r="D69" s="53" t="s">
-        <v>1152</v>
       </c>
       <c r="E69" s="38"/>
       <c r="F69" s="38"/>
       <c r="G69" s="38"/>
       <c r="H69" s="57" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="I69" s="38"/>
       <c r="J69" s="38"/>
@@ -14394,16 +14394,16 @@
         <v>316</v>
       </c>
       <c r="C71" s="57" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="D71" s="53" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="E71" s="38"/>
       <c r="F71" s="38"/>
       <c r="G71" s="38"/>
       <c r="H71" s="57" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="I71" s="38"/>
       <c r="J71" s="38"/>
@@ -14415,13 +14415,13 @@
         <v>178</v>
       </c>
       <c r="B72" s="57" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C72" s="57" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D72" s="51" t="s">
         <v>1157</v>
-      </c>
-      <c r="C72" s="57" t="s">
-        <v>1158</v>
-      </c>
-      <c r="D72" s="51" t="s">
-        <v>1159</v>
       </c>
       <c r="E72" s="38"/>
       <c r="F72" s="38"/>
@@ -14434,16 +14434,16 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="51" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B73" s="51" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C73" s="51" t="s">
         <v>1160</v>
       </c>
-      <c r="B73" s="51" t="s">
-        <v>1161</v>
-      </c>
-      <c r="C73" s="51" t="s">
-        <v>1162</v>
-      </c>
       <c r="D73" s="51" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="E73" s="38"/>
       <c r="F73" s="38"/>
@@ -14459,19 +14459,19 @@
         <v>67</v>
       </c>
       <c r="B74" s="51" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C74" s="51" t="s">
+        <v>1162</v>
+      </c>
+      <c r="D74" s="51" t="s">
         <v>1163</v>
-      </c>
-      <c r="C74" s="51" t="s">
-        <v>1164</v>
-      </c>
-      <c r="D74" s="51" t="s">
-        <v>1165</v>
       </c>
       <c r="E74" s="38"/>
       <c r="F74" s="38"/>
       <c r="G74" s="38"/>
       <c r="H74" s="57" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="I74" s="38"/>
       <c r="J74" s="38"/>
@@ -14480,16 +14480,16 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B75" s="51" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="C75" s="51" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="D75" s="51" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="E75" s="38"/>
       <c r="F75" s="38"/>
@@ -14505,19 +14505,19 @@
         <v>67</v>
       </c>
       <c r="B76" s="51" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C76" s="51" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D76" s="51" t="s">
         <v>1169</v>
-      </c>
-      <c r="C76" s="51" t="s">
-        <v>1170</v>
-      </c>
-      <c r="D76" s="51" t="s">
-        <v>1171</v>
       </c>
       <c r="E76" s="38"/>
       <c r="F76" s="38"/>
       <c r="G76" s="38"/>
       <c r="H76" s="57" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="I76" s="38"/>
       <c r="J76" s="38"/>
@@ -14526,16 +14526,16 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B77" s="51" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="C77" s="51" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="D77" s="51" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="E77" s="38"/>
       <c r="F77" s="38"/>
@@ -14551,19 +14551,19 @@
         <v>67</v>
       </c>
       <c r="B78" s="51" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C78" s="51" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D78" s="57" t="s">
         <v>1175</v>
-      </c>
-      <c r="C78" s="51" t="s">
-        <v>1176</v>
-      </c>
-      <c r="D78" s="57" t="s">
-        <v>1177</v>
       </c>
       <c r="E78" s="38"/>
       <c r="F78" s="38"/>
       <c r="G78" s="38"/>
       <c r="H78" s="57" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="I78" s="38"/>
       <c r="J78" s="38"/>
@@ -14572,16 +14572,16 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B79" s="51" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="C79" s="51" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="D79" s="51" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="E79" s="38"/>
       <c r="F79" s="38"/>
@@ -14593,33 +14593,33 @@
         <v>67</v>
       </c>
       <c r="B80" s="51" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C80" s="51" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D80" s="51" t="s">
         <v>1181</v>
-      </c>
-      <c r="C80" s="51" t="s">
-        <v>1182</v>
-      </c>
-      <c r="D80" s="51" t="s">
-        <v>1183</v>
       </c>
       <c r="E80" s="38"/>
       <c r="F80" s="38"/>
       <c r="G80" s="38"/>
       <c r="H80" s="57" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B81" s="51" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C81" s="51" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D81" s="51" t="s">
         <v>1185</v>
-      </c>
-      <c r="C81" s="51" t="s">
-        <v>1186</v>
-      </c>
-      <c r="D81" s="51" t="s">
-        <v>1187</v>
       </c>
       <c r="E81" s="38"/>
       <c r="F81" s="38"/>
@@ -14631,33 +14631,33 @@
         <v>67</v>
       </c>
       <c r="B82" s="51" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C82" s="51" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D82" s="51" t="s">
         <v>1188</v>
-      </c>
-      <c r="C82" s="51" t="s">
-        <v>1189</v>
-      </c>
-      <c r="D82" s="51" t="s">
-        <v>1190</v>
       </c>
       <c r="E82" s="38"/>
       <c r="F82" s="38"/>
       <c r="G82" s="38"/>
       <c r="H82" s="57" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B83" s="51" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C83" s="51" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D83" s="51" t="s">
         <v>1192</v>
-      </c>
-      <c r="C83" s="51" t="s">
-        <v>1193</v>
-      </c>
-      <c r="D83" s="51" t="s">
-        <v>1194</v>
       </c>
       <c r="E83" s="38"/>
       <c r="F83" s="38"/>
@@ -14669,33 +14669,33 @@
         <v>67</v>
       </c>
       <c r="B84" s="51" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C84" s="51" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D84" s="51" t="s">
         <v>1195</v>
-      </c>
-      <c r="C84" s="51" t="s">
-        <v>1196</v>
-      </c>
-      <c r="D84" s="51" t="s">
-        <v>1197</v>
       </c>
       <c r="E84" s="38"/>
       <c r="F84" s="38"/>
       <c r="G84" s="38"/>
       <c r="H84" s="57" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B85" s="51" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C85" s="51" t="s">
+        <v>1198</v>
+      </c>
+      <c r="D85" s="57" t="s">
         <v>1199</v>
-      </c>
-      <c r="C85" s="51" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D85" s="57" t="s">
-        <v>1201</v>
       </c>
       <c r="E85" s="38"/>
       <c r="F85" s="38"/>
@@ -14707,33 +14707,33 @@
         <v>67</v>
       </c>
       <c r="B86" s="51" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C86" s="57" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D86" s="58" t="s">
         <v>1202</v>
-      </c>
-      <c r="C86" s="57" t="s">
-        <v>1203</v>
-      </c>
-      <c r="D86" s="58" t="s">
-        <v>1204</v>
       </c>
       <c r="E86" s="38"/>
       <c r="F86" s="38"/>
       <c r="G86" s="38"/>
       <c r="H86" s="57" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B87" s="51" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C87" s="51" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D87" s="58" t="s">
         <v>1206</v>
-      </c>
-      <c r="C87" s="51" t="s">
-        <v>1207</v>
-      </c>
-      <c r="D87" s="58" t="s">
-        <v>1208</v>
       </c>
       <c r="E87" s="38"/>
       <c r="F87" s="38"/>
@@ -14745,33 +14745,33 @@
         <v>67</v>
       </c>
       <c r="B88" s="51" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C88" s="51" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D88" s="51" t="s">
         <v>1209</v>
-      </c>
-      <c r="C88" s="51" t="s">
-        <v>1210</v>
-      </c>
-      <c r="D88" s="51" t="s">
-        <v>1211</v>
       </c>
       <c r="E88" s="38"/>
       <c r="F88" s="38"/>
       <c r="G88" s="38"/>
       <c r="H88" s="57" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B89" s="51" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C89" s="51" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D89" s="57" t="s">
         <v>1213</v>
-      </c>
-      <c r="C89" s="51" t="s">
-        <v>1214</v>
-      </c>
-      <c r="D89" s="57" t="s">
-        <v>1215</v>
       </c>
       <c r="E89" s="38"/>
       <c r="F89" s="38"/>
@@ -14783,33 +14783,33 @@
         <v>67</v>
       </c>
       <c r="B90" s="51" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C90" s="57" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D90" s="57" t="s">
         <v>1216</v>
-      </c>
-      <c r="C90" s="57" t="s">
-        <v>1217</v>
-      </c>
-      <c r="D90" s="57" t="s">
-        <v>1218</v>
       </c>
       <c r="E90" s="38"/>
       <c r="F90" s="38"/>
       <c r="G90" s="38"/>
       <c r="H90" s="57" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B91" s="57" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="C91" s="57" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="D91" s="57" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="E91" s="38"/>
       <c r="F91" s="38"/>
@@ -14821,33 +14821,33 @@
         <v>67</v>
       </c>
       <c r="B92" s="51" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C92" s="57" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D92" s="38" t="s">
         <v>1222</v>
-      </c>
-      <c r="C92" s="57" t="s">
-        <v>1223</v>
-      </c>
-      <c r="D92" s="38" t="s">
-        <v>1224</v>
       </c>
       <c r="E92" s="38"/>
       <c r="F92" s="38"/>
       <c r="G92" s="38"/>
       <c r="H92" s="57" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B93" s="57" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="C93" s="57" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="D93" s="38" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="E93" s="38"/>
       <c r="F93" s="38"/>
@@ -14859,33 +14859,33 @@
         <v>67</v>
       </c>
       <c r="B94" s="51" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C94" s="57" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D94" s="38" t="s">
         <v>1228</v>
-      </c>
-      <c r="C94" s="57" t="s">
-        <v>1229</v>
-      </c>
-      <c r="D94" s="38" t="s">
-        <v>1230</v>
       </c>
       <c r="E94" s="38"/>
       <c r="F94" s="38"/>
       <c r="G94" s="38"/>
       <c r="H94" s="57" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B95" s="57" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="C95" s="57" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="D95" s="38" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="E95" s="38"/>
       <c r="F95" s="38"/>
@@ -14897,33 +14897,33 @@
         <v>67</v>
       </c>
       <c r="B96" s="51" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C96" s="57" t="s">
+        <v>1233</v>
+      </c>
+      <c r="D96" s="38" t="s">
         <v>1234</v>
-      </c>
-      <c r="C96" s="57" t="s">
-        <v>1235</v>
-      </c>
-      <c r="D96" s="38" t="s">
-        <v>1236</v>
       </c>
       <c r="E96" s="38"/>
       <c r="F96" s="38"/>
       <c r="G96" s="38"/>
       <c r="H96" s="57" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B97" s="57" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C97" s="57" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D97" s="38" t="s">
         <v>1238</v>
-      </c>
-      <c r="C97" s="57" t="s">
-        <v>1239</v>
-      </c>
-      <c r="D97" s="38" t="s">
-        <v>1240</v>
       </c>
       <c r="E97" s="38"/>
       <c r="F97" s="38"/>
@@ -14935,33 +14935,33 @@
         <v>67</v>
       </c>
       <c r="B98" s="57" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C98" s="57" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D98" s="38" t="s">
         <v>1241</v>
-      </c>
-      <c r="C98" s="57" t="s">
-        <v>1242</v>
-      </c>
-      <c r="D98" s="38" t="s">
-        <v>1243</v>
       </c>
       <c r="E98" s="38"/>
       <c r="F98" s="38"/>
       <c r="G98" s="38"/>
       <c r="H98" s="57" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B99" s="57" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="C99" s="57" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="D99" s="38" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="E99" s="38"/>
       <c r="F99" s="38"/>
@@ -14973,33 +14973,33 @@
         <v>67</v>
       </c>
       <c r="B100" s="57" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C100" s="57" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D100" s="38" t="s">
         <v>1247</v>
-      </c>
-      <c r="C100" s="57" t="s">
-        <v>1248</v>
-      </c>
-      <c r="D100" s="38" t="s">
-        <v>1249</v>
       </c>
       <c r="E100" s="38"/>
       <c r="F100" s="38"/>
       <c r="G100" s="38"/>
       <c r="H100" s="57" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B101" s="57" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="C101" s="57" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="D101" s="38" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="E101" s="38"/>
       <c r="F101" s="38"/>
@@ -15011,33 +15011,33 @@
         <v>67</v>
       </c>
       <c r="B102" s="57" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C102" s="57" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D102" s="38" t="s">
         <v>1253</v>
-      </c>
-      <c r="C102" s="57" t="s">
-        <v>1254</v>
-      </c>
-      <c r="D102" s="38" t="s">
-        <v>1255</v>
       </c>
       <c r="E102" s="38"/>
       <c r="F102" s="38"/>
       <c r="G102" s="38"/>
       <c r="H102" s="57" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B103" s="57" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="C103" s="57" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="D103" s="38" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="E103" s="38"/>
       <c r="F103" s="38"/>
@@ -15049,33 +15049,33 @@
         <v>67</v>
       </c>
       <c r="B104" s="57" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C104" s="57" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D104" s="57" t="s">
         <v>1259</v>
-      </c>
-      <c r="C104" s="57" t="s">
-        <v>1260</v>
-      </c>
-      <c r="D104" s="57" t="s">
-        <v>1261</v>
       </c>
       <c r="E104" s="38"/>
       <c r="F104" s="38"/>
       <c r="G104" s="38"/>
       <c r="H104" s="57" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B105" s="57" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C105" s="57" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D105" s="38" t="s">
         <v>1263</v>
-      </c>
-      <c r="C105" s="57" t="s">
-        <v>1264</v>
-      </c>
-      <c r="D105" s="38" t="s">
-        <v>1265</v>
       </c>
       <c r="E105" s="38"/>
       <c r="F105" s="38"/>
@@ -15087,33 +15087,33 @@
         <v>67</v>
       </c>
       <c r="B106" s="57" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C106" s="57" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D106" s="38" t="s">
         <v>1266</v>
-      </c>
-      <c r="C106" s="57" t="s">
-        <v>1267</v>
-      </c>
-      <c r="D106" s="38" t="s">
-        <v>1268</v>
       </c>
       <c r="E106" s="38"/>
       <c r="F106" s="38"/>
       <c r="G106" s="38"/>
       <c r="H106" s="57" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B107" s="57" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C107" s="57" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D107" s="38" t="s">
         <v>1270</v>
-      </c>
-      <c r="C107" s="57" t="s">
-        <v>1271</v>
-      </c>
-      <c r="D107" s="38" t="s">
-        <v>1272</v>
       </c>
       <c r="E107" s="38"/>
       <c r="F107" s="38"/>
@@ -15125,33 +15125,33 @@
         <v>67</v>
       </c>
       <c r="B108" s="57" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C108" s="57" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D108" s="38" t="s">
         <v>1273</v>
-      </c>
-      <c r="C108" s="57" t="s">
-        <v>1274</v>
-      </c>
-      <c r="D108" s="38" t="s">
-        <v>1275</v>
       </c>
       <c r="E108" s="38"/>
       <c r="F108" s="38"/>
       <c r="G108" s="38"/>
       <c r="H108" s="57" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B109" s="57" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="C109" s="57" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="D109" s="38" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="E109" s="38"/>
       <c r="F109" s="38"/>
@@ -15163,33 +15163,33 @@
         <v>67</v>
       </c>
       <c r="B110" s="57" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C110" s="57" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D110" s="38" t="s">
         <v>1279</v>
-      </c>
-      <c r="C110" s="57" t="s">
-        <v>1280</v>
-      </c>
-      <c r="D110" s="38" t="s">
-        <v>1281</v>
       </c>
       <c r="E110" s="38"/>
       <c r="F110" s="38"/>
       <c r="G110" s="38"/>
       <c r="H110" s="57" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B111" s="57" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C111" s="57" t="s">
+        <v>1282</v>
+      </c>
+      <c r="D111" s="38" t="s">
         <v>1283</v>
-      </c>
-      <c r="C111" s="57" t="s">
-        <v>1284</v>
-      </c>
-      <c r="D111" s="38" t="s">
-        <v>1285</v>
       </c>
       <c r="E111" s="38"/>
       <c r="F111" s="38"/>
@@ -15201,33 +15201,33 @@
         <v>67</v>
       </c>
       <c r="B112" s="57" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C112" s="57" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D112" s="38" t="s">
         <v>1286</v>
-      </c>
-      <c r="C112" s="57" t="s">
-        <v>1287</v>
-      </c>
-      <c r="D112" s="38" t="s">
-        <v>1288</v>
       </c>
       <c r="E112" s="38"/>
       <c r="F112" s="38"/>
       <c r="G112" s="38"/>
       <c r="H112" s="57" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B113" s="57" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C113" s="57" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D113" s="38" t="s">
         <v>1290</v>
-      </c>
-      <c r="C113" s="57" t="s">
-        <v>1291</v>
-      </c>
-      <c r="D113" s="38" t="s">
-        <v>1292</v>
       </c>
       <c r="E113" s="38"/>
       <c r="F113" s="38"/>
@@ -15239,33 +15239,33 @@
         <v>67</v>
       </c>
       <c r="B114" s="57" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C114" s="57" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D114" s="38" t="s">
         <v>1293</v>
-      </c>
-      <c r="C114" s="57" t="s">
-        <v>1294</v>
-      </c>
-      <c r="D114" s="38" t="s">
-        <v>1295</v>
       </c>
       <c r="E114" s="38"/>
       <c r="F114" s="38"/>
       <c r="G114" s="38"/>
       <c r="H114" s="57" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="51" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B115" s="57" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C115" s="57" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D115" s="38" t="s">
         <v>1297</v>
-      </c>
-      <c r="C115" s="57" t="s">
-        <v>1298</v>
-      </c>
-      <c r="D115" s="38" t="s">
-        <v>1299</v>
       </c>
       <c r="E115" s="38"/>
       <c r="F115" s="38"/>
@@ -15277,19 +15277,19 @@
         <v>67</v>
       </c>
       <c r="B116" s="57" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C116" s="57" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D116" s="38" t="s">
         <v>1300</v>
-      </c>
-      <c r="C116" s="57" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D116" s="38" t="s">
-        <v>1302</v>
       </c>
       <c r="E116" s="38"/>
       <c r="F116" s="38"/>
       <c r="G116" s="38"/>
       <c r="H116" s="57" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -15297,13 +15297,13 @@
         <v>178</v>
       </c>
       <c r="B117" s="57" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C117" s="52" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D117" s="53" t="s">
         <v>1304</v>
-      </c>
-      <c r="C117" s="52" t="s">
-        <v>1305</v>
-      </c>
-      <c r="D117" s="53" t="s">
-        <v>1306</v>
       </c>
       <c r="E117" s="38"/>
       <c r="F117" s="38"/>
@@ -15315,13 +15315,13 @@
         <v>312</v>
       </c>
       <c r="B118" s="57" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="C118" s="57" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="D118" s="38" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="E118" s="38"/>
       <c r="F118" s="38"/>
@@ -15348,16 +15348,16 @@
         <v>315</v>
       </c>
       <c r="C120" s="57" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="D120" s="38" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="E120" s="38"/>
       <c r="F120" s="38"/>
       <c r="G120" s="38"/>
       <c r="H120" s="57" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
@@ -15365,13 +15365,13 @@
         <v>178</v>
       </c>
       <c r="B121" s="57" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C121" s="57" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D121" s="57" t="s">
         <v>1311</v>
-      </c>
-      <c r="C121" s="57" t="s">
-        <v>1312</v>
-      </c>
-      <c r="D121" s="57" t="s">
-        <v>1313</v>
       </c>
       <c r="E121" s="38"/>
       <c r="F121" s="38"/>
@@ -15380,16 +15380,16 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="57" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B122" s="57" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C122" s="57" t="s">
         <v>1314</v>
       </c>
-      <c r="B122" s="57" t="s">
+      <c r="D122" s="38" t="s">
         <v>1315</v>
-      </c>
-      <c r="C122" s="57" t="s">
-        <v>1316</v>
-      </c>
-      <c r="D122" s="38" t="s">
-        <v>1317</v>
       </c>
       <c r="E122" s="38"/>
       <c r="F122" s="38"/>
@@ -15401,19 +15401,19 @@
         <v>39</v>
       </c>
       <c r="B123" s="57" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C123" s="57" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D123" s="38" t="s">
         <v>1318</v>
-      </c>
-      <c r="C123" s="57" t="s">
-        <v>1319</v>
-      </c>
-      <c r="D123" s="38" t="s">
-        <v>1320</v>
       </c>
       <c r="E123" s="38"/>
       <c r="F123" s="38"/>
       <c r="G123" s="38"/>
       <c r="H123" s="57" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
@@ -15920,128 +15920,128 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="64" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="B33" s="64" t="s">
         <v>1065</v>
       </c>
       <c r="C33" s="64" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="D33" s="61" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="64" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="B34" s="64" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C34" s="64" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D34" s="61" t="s">
         <v>1325</v>
-      </c>
-      <c r="C34" s="64" t="s">
-        <v>1326</v>
-      </c>
-      <c r="D34" s="61" t="s">
-        <v>1327</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="64" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="B35" s="64" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C35" s="64" t="s">
+        <v>1327</v>
+      </c>
+      <c r="D35" s="61" t="s">
         <v>1328</v>
-      </c>
-      <c r="C35" s="64" t="s">
-        <v>1329</v>
-      </c>
-      <c r="D35" s="61" t="s">
-        <v>1330</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="64" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B36" s="64" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C36" s="64" t="s">
         <v>1331</v>
       </c>
-      <c r="B36" s="64" t="s">
+      <c r="D36" s="61" t="s">
         <v>1332</v>
-      </c>
-      <c r="C36" s="64" t="s">
-        <v>1333</v>
-      </c>
-      <c r="D36" s="61" t="s">
-        <v>1334</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="64" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="B37" s="64" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C37" s="64" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D37" s="61" t="s">
         <v>1335</v>
-      </c>
-      <c r="C37" s="64" t="s">
-        <v>1336</v>
-      </c>
-      <c r="D37" s="61" t="s">
-        <v>1337</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="64" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="B38" s="64" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C38" s="64" t="s">
+        <v>1337</v>
+      </c>
+      <c r="D38" s="61" t="s">
         <v>1338</v>
-      </c>
-      <c r="C38" s="64" t="s">
-        <v>1339</v>
-      </c>
-      <c r="D38" s="61" t="s">
-        <v>1340</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="64" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="B39" s="64" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C39" s="64" t="s">
+        <v>1340</v>
+      </c>
+      <c r="D39" s="61" t="s">
         <v>1341</v>
-      </c>
-      <c r="C39" s="64" t="s">
-        <v>1342</v>
-      </c>
-      <c r="D39" s="61" t="s">
-        <v>1343</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="64" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="B40" s="64" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C40" s="64" t="s">
+        <v>1343</v>
+      </c>
+      <c r="D40" s="61" t="s">
         <v>1344</v>
-      </c>
-      <c r="C40" s="64" t="s">
-        <v>1345</v>
-      </c>
-      <c r="D40" s="61" t="s">
-        <v>1346</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="64" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="B41" s="64" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C41" s="64" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D41" s="61" t="s">
         <v>1347</v>
-      </c>
-      <c r="C41" s="64" t="s">
-        <v>1348</v>
-      </c>
-      <c r="D41" s="61" t="s">
-        <v>1349</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -16049,13 +16049,13 @@
         <v>1044</v>
       </c>
       <c r="B42" s="64" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C42" s="64" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D42" s="64" t="s">
         <v>1350</v>
-      </c>
-      <c r="C42" s="64" t="s">
-        <v>1351</v>
-      </c>
-      <c r="D42" s="64" t="s">
-        <v>1352</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -16063,13 +16063,13 @@
         <v>1044</v>
       </c>
       <c r="B43" s="64" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C43" s="64" t="s">
+        <v>1352</v>
+      </c>
+      <c r="D43" s="64" t="s">
         <v>1353</v>
-      </c>
-      <c r="C43" s="64" t="s">
-        <v>1354</v>
-      </c>
-      <c r="D43" s="64" t="s">
-        <v>1355</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -16088,35 +16088,35 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="64" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B45" s="64" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C45" s="64" t="s">
         <v>1356</v>
       </c>
-      <c r="B45" s="64" t="s">
+      <c r="D45" s="61" t="s">
         <v>1357</v>
-      </c>
-      <c r="C45" s="64" t="s">
-        <v>1358</v>
-      </c>
-      <c r="D45" s="61" t="s">
-        <v>1359</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="64" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B46" s="64" t="s">
         <v>366</v>
       </c>
       <c r="C46" s="64" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="D46" s="61" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="64" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B47" s="64" t="s">
         <v>365</v>
@@ -16130,7 +16130,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="64" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B48" s="64" t="s">
         <v>362</v>
@@ -16144,10 +16144,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="64" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B49" s="64" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="C49" s="64" t="s">
         <v>30</v>
@@ -16158,10 +16158,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="64" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B50" s="64" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="C50" s="64" t="s">
         <v>31</v>
@@ -16172,24 +16172,24 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="64" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B51" s="64" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="C51" s="64" t="s">
         <v>358</v>
       </c>
       <c r="D51" s="61" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="64" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B52" s="64" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="C52" s="64" t="s">
         <v>32</v>
@@ -16200,66 +16200,66 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="64" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B53" s="64" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C53" s="64" t="s">
+        <v>1366</v>
+      </c>
+      <c r="D53" s="61" t="s">
         <v>1367</v>
-      </c>
-      <c r="C53" s="64" t="s">
-        <v>1368</v>
-      </c>
-      <c r="D53" s="61" t="s">
-        <v>1369</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="64" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B54" s="64" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C54" s="64" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D54" s="61" t="s">
         <v>1370</v>
-      </c>
-      <c r="C54" s="64" t="s">
-        <v>1371</v>
-      </c>
-      <c r="D54" s="61" t="s">
-        <v>1372</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="64" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B55" s="64" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C55" s="64" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D55" s="61" t="s">
         <v>1373</v>
-      </c>
-      <c r="C55" s="64" t="s">
-        <v>1374</v>
-      </c>
-      <c r="D55" s="61" t="s">
-        <v>1375</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="64" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B56" s="64" t="s">
         <v>877</v>
       </c>
       <c r="C56" s="64" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="D56" s="61" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="64" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B57" s="64" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="C57" s="64" t="s">
         <v>33</v>
@@ -16270,21 +16270,21 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="64" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B58" s="64" t="s">
+        <v>1377</v>
+      </c>
+      <c r="C58" s="64" t="s">
+        <v>1378</v>
+      </c>
+      <c r="D58" s="61" t="s">
         <v>1379</v>
-      </c>
-      <c r="C58" s="64" t="s">
-        <v>1380</v>
-      </c>
-      <c r="D58" s="61" t="s">
-        <v>1381</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="64" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B59" s="64" t="s">
         <v>233</v>
@@ -16298,7 +16298,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="64" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B60" s="64" t="s">
         <v>245</v>

</xml_diff>

<commit_message>
swap to vaccine long
There will now be two vaccination dictionaries one long and one short, updating code, documentation and pkgdown
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-survey-dict.xlsx
+++ b/inst/extdata/MSF-survey-dict.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Mortality" sheetId="11" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Nutrition" sheetId="8" r:id="rId4"/>
     <sheet name="Nutrition_options" sheetId="17" r:id="rId5"/>
     <sheet name="Nutrition_settings" sheetId="18" r:id="rId6"/>
-    <sheet name="Vaccination" sheetId="14" r:id="rId7"/>
-    <sheet name="Vaccination_options" sheetId="15" r:id="rId8"/>
-    <sheet name="Vaccination_settings" sheetId="16" r:id="rId9"/>
+    <sheet name="Vaccination_long" sheetId="14" r:id="rId7"/>
+    <sheet name="Vaccination_long_options" sheetId="15" r:id="rId8"/>
+    <sheet name="Vaccination_long_settings" sheetId="16" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Vaccination!$A$1:$L$125</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Vaccination_long!$A$1:$L$125</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -4787,8 +4787,8 @@
   </sheetPr>
   <dimension ref="A1:L209"/>
   <sheetViews>
-    <sheetView topLeftCell="A141" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H153" sqref="H153"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12818,7 +12818,7 @@
   </sheetPr>
   <dimension ref="A1:L125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
@@ -16338,7 +16338,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="P47" sqref="P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
reinstating vacc short dict
still needs cleaning up
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-survey-dict.xlsx
+++ b/inst/extdata/MSF-survey-dict.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Mortality" sheetId="11" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="Vaccination_long" sheetId="14" r:id="rId7"/>
     <sheet name="Vaccination_long_options" sheetId="15" r:id="rId8"/>
     <sheet name="Vaccination_long_settings" sheetId="16" r:id="rId9"/>
+    <sheet name="Vaccination_short" sheetId="20" r:id="rId10"/>
+    <sheet name="Vaccination_short_options" sheetId="21" r:id="rId11"/>
+    <sheet name="Vaccination_short_settings" sheetId="22" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Vaccination_long!$A$1:$L$125</definedName>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2583" uniqueCount="1385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3119" uniqueCount="1556">
   <si>
     <t>type</t>
   </si>
@@ -4268,6 +4271,520 @@
   </si>
   <si>
     <t>poliodrop_camp_woc</t>
+  </si>
+  <si>
+    <t>hxl</t>
+  </si>
+  <si>
+    <t>#date +collected</t>
+  </si>
+  <si>
+    <t>#loc +name</t>
+  </si>
+  <si>
+    <t>#loc +name +other</t>
+  </si>
+  <si>
+    <t>#population +children</t>
+  </si>
+  <si>
+    <t>How many children between 6 months and 9 years are in the household?</t>
+  </si>
+  <si>
+    <t>Combien d'enfants âgés de 6 mois à 9 ans se trouvent dans le ménage ?</t>
+  </si>
+  <si>
+    <t>Child Demographics</t>
+  </si>
+  <si>
+    <t>Routine vaccination</t>
+  </si>
+  <si>
+    <t>Vaccination de routine</t>
+  </si>
+  <si>
+    <t>${consent}='yes' and ${child_number} &gt;0</t>
+  </si>
+  <si>
+    <t>select_one vaccination</t>
+  </si>
+  <si>
+    <t>routine_vacc</t>
+  </si>
+  <si>
+    <t>Routine Vaccination - 9 months vaccine</t>
+  </si>
+  <si>
+    <t>Vaccination de routine - Vaccin de 9 mois</t>
+  </si>
+  <si>
+    <t>#x_routine_vaccinated</t>
+  </si>
+  <si>
+    <t>age_routine_vacc</t>
+  </si>
+  <si>
+    <t>Age of child at the time of vaccination (months)</t>
+  </si>
+  <si>
+    <t>Âge de l'enfant au moment de la vaccination (en mois)</t>
+  </si>
+  <si>
+    <t>${routine_vacc} = 'verbal' or ${routine_vacc} = 'card'</t>
+  </si>
+  <si>
+    <t>select_one place_routine</t>
+  </si>
+  <si>
+    <t>place_routine_vacc</t>
+  </si>
+  <si>
+    <t>Place of routine vaccination</t>
+  </si>
+  <si>
+    <t>Endroit de la vaccination de routine</t>
+  </si>
+  <si>
+    <t>#x_place_routine_vaccinated</t>
+  </si>
+  <si>
+    <t>select_one reason_routine</t>
+  </si>
+  <si>
+    <t>reason_route_vacc</t>
+  </si>
+  <si>
+    <t>Reason for non routine vaccination</t>
+  </si>
+  <si>
+    <t>Raison pour ne pas avoir pris la vaccination de routine</t>
+  </si>
+  <si>
+    <t>${routine_vacc} = 'no'</t>
+  </si>
+  <si>
+    <t>reason_route_other</t>
+  </si>
+  <si>
+    <t>Specify other reason</t>
+  </si>
+  <si>
+    <t>${reason_route_vacc}='other'</t>
+  </si>
+  <si>
+    <t>MSF vaccination</t>
+  </si>
+  <si>
+    <t>Vaccination de MSF</t>
+  </si>
+  <si>
+    <t>msf_vacc</t>
+  </si>
+  <si>
+    <t>MSF Vaccination Campaign - 6 months to 9 years</t>
+  </si>
+  <si>
+    <t>Campagne de vaccination de MSF - 6 mois à 9 ans</t>
+  </si>
+  <si>
+    <t>#x_campaign_vaccinated</t>
+  </si>
+  <si>
+    <t>age_msf_vacc</t>
+  </si>
+  <si>
+    <t>${msf_vacc} = 'verbal' or ${msf_vacc} = 'card'</t>
+  </si>
+  <si>
+    <t>select_one place_msf</t>
+  </si>
+  <si>
+    <t>place_msf_vacc</t>
+  </si>
+  <si>
+    <t>Place of MSF vaccination</t>
+  </si>
+  <si>
+    <t>Endroit de la vaccination de MSF</t>
+  </si>
+  <si>
+    <t>#x_place_campaign_vaccinated</t>
+  </si>
+  <si>
+    <t>select_one reason_msf</t>
+  </si>
+  <si>
+    <t>reason_msf_vacc</t>
+  </si>
+  <si>
+    <t>Reason for non MSF vaccination</t>
+  </si>
+  <si>
+    <t>Raison pour ne pas avoir pris la vaccination de MSF</t>
+  </si>
+  <si>
+    <t>${msf_vacc} = 'no'</t>
+  </si>
+  <si>
+    <t>reason_msf_other</t>
+  </si>
+  <si>
+    <t>${reason_msf_vacc}='other'</t>
+  </si>
+  <si>
+    <t>Immunisation SIA/NID</t>
+  </si>
+  <si>
+    <t>Activités de vaccination supplémentaire</t>
+  </si>
+  <si>
+    <t>sia_vacc</t>
+  </si>
+  <si>
+    <t>Immunisation SIA/NID - 6 months to 9 years</t>
+  </si>
+  <si>
+    <t>AVS - 6 mois à 9 ans</t>
+  </si>
+  <si>
+    <t>#x_supplementary_vaccinated</t>
+  </si>
+  <si>
+    <t>age_sia_vacc</t>
+  </si>
+  <si>
+    <t>${sia_vacc} = 'verbal' or ${sia_vacc} = 'card'</t>
+  </si>
+  <si>
+    <t>place_sia_vacc</t>
+  </si>
+  <si>
+    <t>Place of SIA vaccination</t>
+  </si>
+  <si>
+    <t>Endroit de l'activité de vaccination supplémentaire</t>
+  </si>
+  <si>
+    <t>#x_place_supplementary_vaccinated</t>
+  </si>
+  <si>
+    <t>reason_sia_vacc</t>
+  </si>
+  <si>
+    <t>Reason for non SIA vaccination</t>
+  </si>
+  <si>
+    <t>Raison pour ne pas avoir pris la vaccination d'avs</t>
+  </si>
+  <si>
+    <t>${sia_vacc} = 'no'</t>
+  </si>
+  <si>
+    <t>reason_sia_other</t>
+  </si>
+  <si>
+    <t>${reason_sia_vacc}='other'</t>
+  </si>
+  <si>
+    <t>Previous diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Antécédents de rougeole</t>
+  </si>
+  <si>
+    <t>diagnosis_disease</t>
+  </si>
+  <si>
+    <t>Did the child previously have measles?</t>
+  </si>
+  <si>
+    <t>L'enfant a-t-il déjà eu la rougeole?</t>
+  </si>
+  <si>
+    <t>#x_illness_measles</t>
+  </si>
+  <si>
+    <t>age_diagnosis</t>
+  </si>
+  <si>
+    <t>Age of child when they had measles (months)</t>
+  </si>
+  <si>
+    <t>Age de l'enfant lorsqu'il a eu la rougeole (en mois)</t>
+  </si>
+  <si>
+    <t>${diagnosis_disease}='yes'</t>
+  </si>
+  <si>
+    <t>vaccination</t>
+  </si>
+  <si>
+    <t>verbal</t>
+  </si>
+  <si>
+    <t>Yes, verbal</t>
+  </si>
+  <si>
+    <t>Oui, verbal</t>
+  </si>
+  <si>
+    <t>card</t>
+  </si>
+  <si>
+    <t>Yes, card</t>
+  </si>
+  <si>
+    <t>Oui, avec carte</t>
+  </si>
+  <si>
+    <t>no_answer</t>
+  </si>
+  <si>
+    <t>No answer</t>
+  </si>
+  <si>
+    <t>Pas de réponse</t>
+  </si>
+  <si>
+    <t>reason_routine</t>
+  </si>
+  <si>
+    <t>dangerous</t>
+  </si>
+  <si>
+    <t>Vaccines dangerous for the child</t>
+  </si>
+  <si>
+    <t>Les vaccins sont dangereux pour les enfants</t>
+  </si>
+  <si>
+    <t>Previous bad experience with vaccination</t>
+  </si>
+  <si>
+    <t>Mauvaise expérience antérieure en matière de vaccination</t>
+  </si>
+  <si>
+    <t>father_refused</t>
+  </si>
+  <si>
+    <t>religious_beliefs</t>
+  </si>
+  <si>
+    <t>child_young</t>
+  </si>
+  <si>
+    <t>Child was too young</t>
+  </si>
+  <si>
+    <t>L'enfant était trop jeune</t>
+  </si>
+  <si>
+    <t>child_old</t>
+  </si>
+  <si>
+    <t>Child was too old</t>
+  </si>
+  <si>
+    <t>L'enfant était trop vieux</t>
+  </si>
+  <si>
+    <t>already_vaccinated</t>
+  </si>
+  <si>
+    <t>Child was already vaccinated</t>
+  </si>
+  <si>
+    <t>L'enfant a déjà été vacciné</t>
+  </si>
+  <si>
+    <t>other_routine</t>
+  </si>
+  <si>
+    <t>Other reason</t>
+  </si>
+  <si>
+    <t>Autre raison</t>
+  </si>
+  <si>
+    <t>reason_msf</t>
+  </si>
+  <si>
+    <t>unaware_eligible</t>
+  </si>
+  <si>
+    <t>Ne savait pas qu'il pouvait vacciner l'enfant</t>
+  </si>
+  <si>
+    <t>unaware_campaign</t>
+  </si>
+  <si>
+    <t>Did not know about vaccination campaign</t>
+  </si>
+  <si>
+    <t>N'était pas au courant de la campagne de vaccination</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>working</t>
+  </si>
+  <si>
+    <t>S/he was working during the campaign</t>
+  </si>
+  <si>
+    <t>Il/elle travaillait pendant la campagne</t>
+  </si>
+  <si>
+    <t>timing</t>
+  </si>
+  <si>
+    <t>Campaign took place on Sunday</t>
+  </si>
+  <si>
+    <t>La campagne a eu lieu dimanche</t>
+  </si>
+  <si>
+    <t>family_away</t>
+  </si>
+  <si>
+    <t>Family was outside village during campaign</t>
+  </si>
+  <si>
+    <t>La famille était à l'extérieur du village pendant la campagne</t>
+  </si>
+  <si>
+    <t>child_sick</t>
+  </si>
+  <si>
+    <t>Child was sick during vaccination campaign</t>
+  </si>
+  <si>
+    <t>Un enfant a été malade lors d'une campagne de vaccination</t>
+  </si>
+  <si>
+    <t>vaccinator_refused</t>
+  </si>
+  <si>
+    <t>Vaccinator decided not to vaccinate the child</t>
+  </si>
+  <si>
+    <t>Le vaccinateur a décidé de ne pas vacciner l'enfant</t>
+  </si>
+  <si>
+    <t>no_vaccine</t>
+  </si>
+  <si>
+    <t>other_msf</t>
+  </si>
+  <si>
+    <t>place_msf</t>
+  </si>
+  <si>
+    <t>place_msf1</t>
+  </si>
+  <si>
+    <t>Place MSF1</t>
+  </si>
+  <si>
+    <t>place_msf2</t>
+  </si>
+  <si>
+    <t>Place MSF2</t>
+  </si>
+  <si>
+    <t>place_msf3</t>
+  </si>
+  <si>
+    <t>Place MSF3</t>
+  </si>
+  <si>
+    <t>place_msf4</t>
+  </si>
+  <si>
+    <t>Place MSF4</t>
+  </si>
+  <si>
+    <t>place_msf5</t>
+  </si>
+  <si>
+    <t>Place MSF5</t>
+  </si>
+  <si>
+    <t>place_msf6</t>
+  </si>
+  <si>
+    <t>Place MSF6</t>
+  </si>
+  <si>
+    <t>place_msf7</t>
+  </si>
+  <si>
+    <t>Place MSF7</t>
+  </si>
+  <si>
+    <t>place_msf8</t>
+  </si>
+  <si>
+    <t>Place MSF8</t>
+  </si>
+  <si>
+    <t>place_msf9</t>
+  </si>
+  <si>
+    <t>Place MSF9</t>
+  </si>
+  <si>
+    <t>place_routine</t>
+  </si>
+  <si>
+    <t>place_routine1</t>
+  </si>
+  <si>
+    <t>Place routine1</t>
+  </si>
+  <si>
+    <t>place_routine2</t>
+  </si>
+  <si>
+    <t>Place routine2</t>
+  </si>
+  <si>
+    <t>place_routine3</t>
+  </si>
+  <si>
+    <t>Place routine3</t>
+  </si>
+  <si>
+    <t>place_routine4</t>
+  </si>
+  <si>
+    <t>Place routine4</t>
+  </si>
+  <si>
+    <t>place_routine5</t>
+  </si>
+  <si>
+    <t>Place routine5</t>
+  </si>
+  <si>
+    <t>place_routine6</t>
+  </si>
+  <si>
+    <t>Place routine6</t>
+  </si>
+  <si>
+    <t>place_routine7</t>
+  </si>
+  <si>
+    <t>Place routine7</t>
+  </si>
+  <si>
+    <t>place_routine8</t>
+  </si>
+  <si>
+    <t>Place routine8</t>
   </si>
 </sst>
 </file>
@@ -4787,7 +5304,7 @@
   </sheetPr>
   <dimension ref="A1:L209"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
@@ -9541,6 +10058,3147 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;P</oddHeader>
+    <oddFooter>&amp;F</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:M60"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.42578125" style="61" customWidth="1"/>
+    <col min="5" max="6" width="28.85546875" style="53" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="61"/>
+    <col min="9" max="9" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="14" max="256" width="9.140625" style="61"/>
+    <col min="257" max="257" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="64.42578125" style="61" customWidth="1"/>
+    <col min="261" max="262" width="28.85546875" style="61" customWidth="1"/>
+    <col min="263" max="264" width="9.140625" style="61"/>
+    <col min="265" max="265" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="267" max="267" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="268" max="268" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="269" max="269" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="270" max="512" width="9.140625" style="61"/>
+    <col min="513" max="513" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="515" max="515" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="516" max="516" width="64.42578125" style="61" customWidth="1"/>
+    <col min="517" max="518" width="28.85546875" style="61" customWidth="1"/>
+    <col min="519" max="520" width="9.140625" style="61"/>
+    <col min="521" max="521" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="522" max="522" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="523" max="523" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="524" max="524" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="525" max="525" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="526" max="768" width="9.140625" style="61"/>
+    <col min="769" max="769" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="771" max="771" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="772" max="772" width="64.42578125" style="61" customWidth="1"/>
+    <col min="773" max="774" width="28.85546875" style="61" customWidth="1"/>
+    <col min="775" max="776" width="9.140625" style="61"/>
+    <col min="777" max="777" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="778" max="778" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="779" max="779" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="780" max="780" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="781" max="781" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="782" max="1024" width="9.140625" style="61"/>
+    <col min="1025" max="1025" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="1027" max="1027" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1028" max="1028" width="64.42578125" style="61" customWidth="1"/>
+    <col min="1029" max="1030" width="28.85546875" style="61" customWidth="1"/>
+    <col min="1031" max="1032" width="9.140625" style="61"/>
+    <col min="1033" max="1033" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1034" max="1034" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1035" max="1035" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="1036" max="1036" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1037" max="1037" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="1038" max="1280" width="9.140625" style="61"/>
+    <col min="1281" max="1281" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="1283" max="1283" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1284" max="1284" width="64.42578125" style="61" customWidth="1"/>
+    <col min="1285" max="1286" width="28.85546875" style="61" customWidth="1"/>
+    <col min="1287" max="1288" width="9.140625" style="61"/>
+    <col min="1289" max="1289" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1290" max="1290" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1291" max="1291" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="1292" max="1292" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1293" max="1293" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="1294" max="1536" width="9.140625" style="61"/>
+    <col min="1537" max="1537" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="1539" max="1539" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1540" max="1540" width="64.42578125" style="61" customWidth="1"/>
+    <col min="1541" max="1542" width="28.85546875" style="61" customWidth="1"/>
+    <col min="1543" max="1544" width="9.140625" style="61"/>
+    <col min="1545" max="1545" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1546" max="1546" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1547" max="1547" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="1548" max="1548" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1549" max="1549" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="1550" max="1792" width="9.140625" style="61"/>
+    <col min="1793" max="1793" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="1795" max="1795" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1796" max="1796" width="64.42578125" style="61" customWidth="1"/>
+    <col min="1797" max="1798" width="28.85546875" style="61" customWidth="1"/>
+    <col min="1799" max="1800" width="9.140625" style="61"/>
+    <col min="1801" max="1801" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1802" max="1802" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1803" max="1803" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="1804" max="1804" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1805" max="1805" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="1806" max="2048" width="9.140625" style="61"/>
+    <col min="2049" max="2049" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="2051" max="2051" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2052" max="2052" width="64.42578125" style="61" customWidth="1"/>
+    <col min="2053" max="2054" width="28.85546875" style="61" customWidth="1"/>
+    <col min="2055" max="2056" width="9.140625" style="61"/>
+    <col min="2057" max="2057" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2058" max="2058" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2059" max="2059" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="2060" max="2060" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2061" max="2061" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="2062" max="2304" width="9.140625" style="61"/>
+    <col min="2305" max="2305" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="2307" max="2307" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2308" max="2308" width="64.42578125" style="61" customWidth="1"/>
+    <col min="2309" max="2310" width="28.85546875" style="61" customWidth="1"/>
+    <col min="2311" max="2312" width="9.140625" style="61"/>
+    <col min="2313" max="2313" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2314" max="2314" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2315" max="2315" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="2316" max="2316" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2317" max="2317" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="2318" max="2560" width="9.140625" style="61"/>
+    <col min="2561" max="2561" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="2563" max="2563" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2564" max="2564" width="64.42578125" style="61" customWidth="1"/>
+    <col min="2565" max="2566" width="28.85546875" style="61" customWidth="1"/>
+    <col min="2567" max="2568" width="9.140625" style="61"/>
+    <col min="2569" max="2569" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2570" max="2570" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2571" max="2571" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="2572" max="2572" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2573" max="2573" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="2574" max="2816" width="9.140625" style="61"/>
+    <col min="2817" max="2817" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="2819" max="2819" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2820" max="2820" width="64.42578125" style="61" customWidth="1"/>
+    <col min="2821" max="2822" width="28.85546875" style="61" customWidth="1"/>
+    <col min="2823" max="2824" width="9.140625" style="61"/>
+    <col min="2825" max="2825" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2826" max="2826" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2827" max="2827" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="2828" max="2828" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2829" max="2829" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="2830" max="3072" width="9.140625" style="61"/>
+    <col min="3073" max="3073" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="3075" max="3075" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3076" max="3076" width="64.42578125" style="61" customWidth="1"/>
+    <col min="3077" max="3078" width="28.85546875" style="61" customWidth="1"/>
+    <col min="3079" max="3080" width="9.140625" style="61"/>
+    <col min="3081" max="3081" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3082" max="3082" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3083" max="3083" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="3084" max="3084" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3085" max="3085" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="3086" max="3328" width="9.140625" style="61"/>
+    <col min="3329" max="3329" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="3331" max="3331" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3332" max="3332" width="64.42578125" style="61" customWidth="1"/>
+    <col min="3333" max="3334" width="28.85546875" style="61" customWidth="1"/>
+    <col min="3335" max="3336" width="9.140625" style="61"/>
+    <col min="3337" max="3337" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3338" max="3338" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3339" max="3339" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="3340" max="3340" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3341" max="3341" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="3342" max="3584" width="9.140625" style="61"/>
+    <col min="3585" max="3585" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="3587" max="3587" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3588" max="3588" width="64.42578125" style="61" customWidth="1"/>
+    <col min="3589" max="3590" width="28.85546875" style="61" customWidth="1"/>
+    <col min="3591" max="3592" width="9.140625" style="61"/>
+    <col min="3593" max="3593" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3594" max="3594" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3595" max="3595" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="3596" max="3596" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3597" max="3597" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="3598" max="3840" width="9.140625" style="61"/>
+    <col min="3841" max="3841" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="3843" max="3843" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3844" max="3844" width="64.42578125" style="61" customWidth="1"/>
+    <col min="3845" max="3846" width="28.85546875" style="61" customWidth="1"/>
+    <col min="3847" max="3848" width="9.140625" style="61"/>
+    <col min="3849" max="3849" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3850" max="3850" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3851" max="3851" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="3852" max="3852" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3853" max="3853" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="3854" max="4096" width="9.140625" style="61"/>
+    <col min="4097" max="4097" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="4099" max="4099" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4100" max="4100" width="64.42578125" style="61" customWidth="1"/>
+    <col min="4101" max="4102" width="28.85546875" style="61" customWidth="1"/>
+    <col min="4103" max="4104" width="9.140625" style="61"/>
+    <col min="4105" max="4105" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4106" max="4106" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4107" max="4107" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="4108" max="4108" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4109" max="4109" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="4110" max="4352" width="9.140625" style="61"/>
+    <col min="4353" max="4353" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="4355" max="4355" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4356" max="4356" width="64.42578125" style="61" customWidth="1"/>
+    <col min="4357" max="4358" width="28.85546875" style="61" customWidth="1"/>
+    <col min="4359" max="4360" width="9.140625" style="61"/>
+    <col min="4361" max="4361" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4362" max="4362" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4363" max="4363" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="4364" max="4364" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4365" max="4365" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="4366" max="4608" width="9.140625" style="61"/>
+    <col min="4609" max="4609" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="4611" max="4611" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4612" max="4612" width="64.42578125" style="61" customWidth="1"/>
+    <col min="4613" max="4614" width="28.85546875" style="61" customWidth="1"/>
+    <col min="4615" max="4616" width="9.140625" style="61"/>
+    <col min="4617" max="4617" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4618" max="4618" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4619" max="4619" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="4620" max="4620" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4621" max="4621" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="4622" max="4864" width="9.140625" style="61"/>
+    <col min="4865" max="4865" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="4867" max="4867" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4868" max="4868" width="64.42578125" style="61" customWidth="1"/>
+    <col min="4869" max="4870" width="28.85546875" style="61" customWidth="1"/>
+    <col min="4871" max="4872" width="9.140625" style="61"/>
+    <col min="4873" max="4873" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4874" max="4874" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4875" max="4875" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="4876" max="4876" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4877" max="4877" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="4878" max="5120" width="9.140625" style="61"/>
+    <col min="5121" max="5121" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="5123" max="5123" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5124" max="5124" width="64.42578125" style="61" customWidth="1"/>
+    <col min="5125" max="5126" width="28.85546875" style="61" customWidth="1"/>
+    <col min="5127" max="5128" width="9.140625" style="61"/>
+    <col min="5129" max="5129" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5130" max="5130" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5131" max="5131" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="5132" max="5132" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5133" max="5133" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="5134" max="5376" width="9.140625" style="61"/>
+    <col min="5377" max="5377" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="5379" max="5379" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5380" max="5380" width="64.42578125" style="61" customWidth="1"/>
+    <col min="5381" max="5382" width="28.85546875" style="61" customWidth="1"/>
+    <col min="5383" max="5384" width="9.140625" style="61"/>
+    <col min="5385" max="5385" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5386" max="5386" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5387" max="5387" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="5388" max="5388" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5389" max="5389" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="5390" max="5632" width="9.140625" style="61"/>
+    <col min="5633" max="5633" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="5635" max="5635" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5636" max="5636" width="64.42578125" style="61" customWidth="1"/>
+    <col min="5637" max="5638" width="28.85546875" style="61" customWidth="1"/>
+    <col min="5639" max="5640" width="9.140625" style="61"/>
+    <col min="5641" max="5641" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5642" max="5642" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5643" max="5643" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="5644" max="5644" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5645" max="5645" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="5646" max="5888" width="9.140625" style="61"/>
+    <col min="5889" max="5889" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="5891" max="5891" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5892" max="5892" width="64.42578125" style="61" customWidth="1"/>
+    <col min="5893" max="5894" width="28.85546875" style="61" customWidth="1"/>
+    <col min="5895" max="5896" width="9.140625" style="61"/>
+    <col min="5897" max="5897" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5898" max="5898" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5899" max="5899" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="5900" max="5900" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5901" max="5901" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="5902" max="6144" width="9.140625" style="61"/>
+    <col min="6145" max="6145" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="6147" max="6147" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6148" max="6148" width="64.42578125" style="61" customWidth="1"/>
+    <col min="6149" max="6150" width="28.85546875" style="61" customWidth="1"/>
+    <col min="6151" max="6152" width="9.140625" style="61"/>
+    <col min="6153" max="6153" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6154" max="6154" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6155" max="6155" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="6156" max="6156" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6157" max="6157" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="6158" max="6400" width="9.140625" style="61"/>
+    <col min="6401" max="6401" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="6403" max="6403" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6404" max="6404" width="64.42578125" style="61" customWidth="1"/>
+    <col min="6405" max="6406" width="28.85546875" style="61" customWidth="1"/>
+    <col min="6407" max="6408" width="9.140625" style="61"/>
+    <col min="6409" max="6409" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6410" max="6410" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6411" max="6411" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="6412" max="6412" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6413" max="6413" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="6414" max="6656" width="9.140625" style="61"/>
+    <col min="6657" max="6657" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="6659" max="6659" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6660" max="6660" width="64.42578125" style="61" customWidth="1"/>
+    <col min="6661" max="6662" width="28.85546875" style="61" customWidth="1"/>
+    <col min="6663" max="6664" width="9.140625" style="61"/>
+    <col min="6665" max="6665" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6666" max="6666" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6667" max="6667" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="6668" max="6668" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6669" max="6669" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="6670" max="6912" width="9.140625" style="61"/>
+    <col min="6913" max="6913" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="6915" max="6915" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6916" max="6916" width="64.42578125" style="61" customWidth="1"/>
+    <col min="6917" max="6918" width="28.85546875" style="61" customWidth="1"/>
+    <col min="6919" max="6920" width="9.140625" style="61"/>
+    <col min="6921" max="6921" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6922" max="6922" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6923" max="6923" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="6924" max="6924" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6925" max="6925" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="6926" max="7168" width="9.140625" style="61"/>
+    <col min="7169" max="7169" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="7171" max="7171" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7172" max="7172" width="64.42578125" style="61" customWidth="1"/>
+    <col min="7173" max="7174" width="28.85546875" style="61" customWidth="1"/>
+    <col min="7175" max="7176" width="9.140625" style="61"/>
+    <col min="7177" max="7177" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7178" max="7178" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7179" max="7179" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="7180" max="7180" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7181" max="7181" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="7182" max="7424" width="9.140625" style="61"/>
+    <col min="7425" max="7425" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="7427" max="7427" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7428" max="7428" width="64.42578125" style="61" customWidth="1"/>
+    <col min="7429" max="7430" width="28.85546875" style="61" customWidth="1"/>
+    <col min="7431" max="7432" width="9.140625" style="61"/>
+    <col min="7433" max="7433" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7434" max="7434" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7435" max="7435" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="7436" max="7436" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7437" max="7437" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="7438" max="7680" width="9.140625" style="61"/>
+    <col min="7681" max="7681" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="7683" max="7683" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7684" max="7684" width="64.42578125" style="61" customWidth="1"/>
+    <col min="7685" max="7686" width="28.85546875" style="61" customWidth="1"/>
+    <col min="7687" max="7688" width="9.140625" style="61"/>
+    <col min="7689" max="7689" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7690" max="7690" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7691" max="7691" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="7692" max="7692" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7693" max="7693" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="7694" max="7936" width="9.140625" style="61"/>
+    <col min="7937" max="7937" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="7939" max="7939" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7940" max="7940" width="64.42578125" style="61" customWidth="1"/>
+    <col min="7941" max="7942" width="28.85546875" style="61" customWidth="1"/>
+    <col min="7943" max="7944" width="9.140625" style="61"/>
+    <col min="7945" max="7945" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7946" max="7946" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7947" max="7947" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="7948" max="7948" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7949" max="7949" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="7950" max="8192" width="9.140625" style="61"/>
+    <col min="8193" max="8193" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="8195" max="8195" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8196" max="8196" width="64.42578125" style="61" customWidth="1"/>
+    <col min="8197" max="8198" width="28.85546875" style="61" customWidth="1"/>
+    <col min="8199" max="8200" width="9.140625" style="61"/>
+    <col min="8201" max="8201" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8202" max="8202" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8203" max="8203" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="8204" max="8204" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8205" max="8205" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="8206" max="8448" width="9.140625" style="61"/>
+    <col min="8449" max="8449" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="8451" max="8451" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8452" max="8452" width="64.42578125" style="61" customWidth="1"/>
+    <col min="8453" max="8454" width="28.85546875" style="61" customWidth="1"/>
+    <col min="8455" max="8456" width="9.140625" style="61"/>
+    <col min="8457" max="8457" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8458" max="8458" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8459" max="8459" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="8460" max="8460" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8461" max="8461" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="8462" max="8704" width="9.140625" style="61"/>
+    <col min="8705" max="8705" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="8707" max="8707" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8708" max="8708" width="64.42578125" style="61" customWidth="1"/>
+    <col min="8709" max="8710" width="28.85546875" style="61" customWidth="1"/>
+    <col min="8711" max="8712" width="9.140625" style="61"/>
+    <col min="8713" max="8713" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8714" max="8714" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8715" max="8715" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="8716" max="8716" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8717" max="8717" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="8718" max="8960" width="9.140625" style="61"/>
+    <col min="8961" max="8961" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="8963" max="8963" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8964" max="8964" width="64.42578125" style="61" customWidth="1"/>
+    <col min="8965" max="8966" width="28.85546875" style="61" customWidth="1"/>
+    <col min="8967" max="8968" width="9.140625" style="61"/>
+    <col min="8969" max="8969" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8970" max="8970" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8971" max="8971" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="8972" max="8972" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8973" max="8973" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="8974" max="9216" width="9.140625" style="61"/>
+    <col min="9217" max="9217" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="9219" max="9219" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9220" max="9220" width="64.42578125" style="61" customWidth="1"/>
+    <col min="9221" max="9222" width="28.85546875" style="61" customWidth="1"/>
+    <col min="9223" max="9224" width="9.140625" style="61"/>
+    <col min="9225" max="9225" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9226" max="9226" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9227" max="9227" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="9228" max="9228" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9229" max="9229" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="9230" max="9472" width="9.140625" style="61"/>
+    <col min="9473" max="9473" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="9475" max="9475" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9476" max="9476" width="64.42578125" style="61" customWidth="1"/>
+    <col min="9477" max="9478" width="28.85546875" style="61" customWidth="1"/>
+    <col min="9479" max="9480" width="9.140625" style="61"/>
+    <col min="9481" max="9481" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9482" max="9482" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9483" max="9483" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="9484" max="9484" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9485" max="9485" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="9486" max="9728" width="9.140625" style="61"/>
+    <col min="9729" max="9729" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="9731" max="9731" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9732" max="9732" width="64.42578125" style="61" customWidth="1"/>
+    <col min="9733" max="9734" width="28.85546875" style="61" customWidth="1"/>
+    <col min="9735" max="9736" width="9.140625" style="61"/>
+    <col min="9737" max="9737" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9738" max="9738" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9739" max="9739" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="9740" max="9740" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9741" max="9741" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="9742" max="9984" width="9.140625" style="61"/>
+    <col min="9985" max="9985" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="9987" max="9987" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9988" max="9988" width="64.42578125" style="61" customWidth="1"/>
+    <col min="9989" max="9990" width="28.85546875" style="61" customWidth="1"/>
+    <col min="9991" max="9992" width="9.140625" style="61"/>
+    <col min="9993" max="9993" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9994" max="9994" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9995" max="9995" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="9996" max="9996" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9997" max="9997" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="9998" max="10240" width="9.140625" style="61"/>
+    <col min="10241" max="10241" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="10243" max="10243" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10244" max="10244" width="64.42578125" style="61" customWidth="1"/>
+    <col min="10245" max="10246" width="28.85546875" style="61" customWidth="1"/>
+    <col min="10247" max="10248" width="9.140625" style="61"/>
+    <col min="10249" max="10249" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10250" max="10250" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10251" max="10251" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="10252" max="10252" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10253" max="10253" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="10254" max="10496" width="9.140625" style="61"/>
+    <col min="10497" max="10497" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="10499" max="10499" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10500" max="10500" width="64.42578125" style="61" customWidth="1"/>
+    <col min="10501" max="10502" width="28.85546875" style="61" customWidth="1"/>
+    <col min="10503" max="10504" width="9.140625" style="61"/>
+    <col min="10505" max="10505" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10506" max="10506" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10507" max="10507" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="10508" max="10508" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10509" max="10509" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="10510" max="10752" width="9.140625" style="61"/>
+    <col min="10753" max="10753" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="10755" max="10755" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10756" max="10756" width="64.42578125" style="61" customWidth="1"/>
+    <col min="10757" max="10758" width="28.85546875" style="61" customWidth="1"/>
+    <col min="10759" max="10760" width="9.140625" style="61"/>
+    <col min="10761" max="10761" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10762" max="10762" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10763" max="10763" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="10764" max="10764" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10765" max="10765" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="10766" max="11008" width="9.140625" style="61"/>
+    <col min="11009" max="11009" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="11011" max="11011" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11012" max="11012" width="64.42578125" style="61" customWidth="1"/>
+    <col min="11013" max="11014" width="28.85546875" style="61" customWidth="1"/>
+    <col min="11015" max="11016" width="9.140625" style="61"/>
+    <col min="11017" max="11017" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11018" max="11018" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11019" max="11019" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="11020" max="11020" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11021" max="11021" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="11022" max="11264" width="9.140625" style="61"/>
+    <col min="11265" max="11265" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="11267" max="11267" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11268" max="11268" width="64.42578125" style="61" customWidth="1"/>
+    <col min="11269" max="11270" width="28.85546875" style="61" customWidth="1"/>
+    <col min="11271" max="11272" width="9.140625" style="61"/>
+    <col min="11273" max="11273" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11274" max="11274" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11275" max="11275" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="11276" max="11276" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11277" max="11277" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="11278" max="11520" width="9.140625" style="61"/>
+    <col min="11521" max="11521" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="11523" max="11523" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11524" max="11524" width="64.42578125" style="61" customWidth="1"/>
+    <col min="11525" max="11526" width="28.85546875" style="61" customWidth="1"/>
+    <col min="11527" max="11528" width="9.140625" style="61"/>
+    <col min="11529" max="11529" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11530" max="11530" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11531" max="11531" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="11532" max="11532" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11533" max="11533" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="11534" max="11776" width="9.140625" style="61"/>
+    <col min="11777" max="11777" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="11779" max="11779" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11780" max="11780" width="64.42578125" style="61" customWidth="1"/>
+    <col min="11781" max="11782" width="28.85546875" style="61" customWidth="1"/>
+    <col min="11783" max="11784" width="9.140625" style="61"/>
+    <col min="11785" max="11785" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11786" max="11786" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11787" max="11787" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="11788" max="11788" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11789" max="11789" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="11790" max="12032" width="9.140625" style="61"/>
+    <col min="12033" max="12033" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="12035" max="12035" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12036" max="12036" width="64.42578125" style="61" customWidth="1"/>
+    <col min="12037" max="12038" width="28.85546875" style="61" customWidth="1"/>
+    <col min="12039" max="12040" width="9.140625" style="61"/>
+    <col min="12041" max="12041" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12042" max="12042" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12043" max="12043" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="12044" max="12044" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12045" max="12045" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="12046" max="12288" width="9.140625" style="61"/>
+    <col min="12289" max="12289" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="12291" max="12291" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12292" max="12292" width="64.42578125" style="61" customWidth="1"/>
+    <col min="12293" max="12294" width="28.85546875" style="61" customWidth="1"/>
+    <col min="12295" max="12296" width="9.140625" style="61"/>
+    <col min="12297" max="12297" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12298" max="12298" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12299" max="12299" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="12300" max="12300" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12301" max="12301" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="12302" max="12544" width="9.140625" style="61"/>
+    <col min="12545" max="12545" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="12547" max="12547" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12548" max="12548" width="64.42578125" style="61" customWidth="1"/>
+    <col min="12549" max="12550" width="28.85546875" style="61" customWidth="1"/>
+    <col min="12551" max="12552" width="9.140625" style="61"/>
+    <col min="12553" max="12553" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12554" max="12554" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12555" max="12555" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="12556" max="12556" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12557" max="12557" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="12558" max="12800" width="9.140625" style="61"/>
+    <col min="12801" max="12801" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="12803" max="12803" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12804" max="12804" width="64.42578125" style="61" customWidth="1"/>
+    <col min="12805" max="12806" width="28.85546875" style="61" customWidth="1"/>
+    <col min="12807" max="12808" width="9.140625" style="61"/>
+    <col min="12809" max="12809" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12810" max="12810" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12811" max="12811" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="12812" max="12812" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12813" max="12813" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="12814" max="13056" width="9.140625" style="61"/>
+    <col min="13057" max="13057" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="13059" max="13059" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13060" max="13060" width="64.42578125" style="61" customWidth="1"/>
+    <col min="13061" max="13062" width="28.85546875" style="61" customWidth="1"/>
+    <col min="13063" max="13064" width="9.140625" style="61"/>
+    <col min="13065" max="13065" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13066" max="13066" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13067" max="13067" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="13068" max="13068" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13069" max="13069" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="13070" max="13312" width="9.140625" style="61"/>
+    <col min="13313" max="13313" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="13315" max="13315" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13316" max="13316" width="64.42578125" style="61" customWidth="1"/>
+    <col min="13317" max="13318" width="28.85546875" style="61" customWidth="1"/>
+    <col min="13319" max="13320" width="9.140625" style="61"/>
+    <col min="13321" max="13321" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13322" max="13322" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13323" max="13323" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="13324" max="13324" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13325" max="13325" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="13326" max="13568" width="9.140625" style="61"/>
+    <col min="13569" max="13569" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="13571" max="13571" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13572" max="13572" width="64.42578125" style="61" customWidth="1"/>
+    <col min="13573" max="13574" width="28.85546875" style="61" customWidth="1"/>
+    <col min="13575" max="13576" width="9.140625" style="61"/>
+    <col min="13577" max="13577" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13578" max="13578" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13579" max="13579" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="13580" max="13580" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13581" max="13581" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="13582" max="13824" width="9.140625" style="61"/>
+    <col min="13825" max="13825" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="13827" max="13827" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13828" max="13828" width="64.42578125" style="61" customWidth="1"/>
+    <col min="13829" max="13830" width="28.85546875" style="61" customWidth="1"/>
+    <col min="13831" max="13832" width="9.140625" style="61"/>
+    <col min="13833" max="13833" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13834" max="13834" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13835" max="13835" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="13836" max="13836" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13837" max="13837" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="13838" max="14080" width="9.140625" style="61"/>
+    <col min="14081" max="14081" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="14083" max="14083" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14084" max="14084" width="64.42578125" style="61" customWidth="1"/>
+    <col min="14085" max="14086" width="28.85546875" style="61" customWidth="1"/>
+    <col min="14087" max="14088" width="9.140625" style="61"/>
+    <col min="14089" max="14089" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14090" max="14090" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14091" max="14091" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="14092" max="14092" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14093" max="14093" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="14094" max="14336" width="9.140625" style="61"/>
+    <col min="14337" max="14337" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="14339" max="14339" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14340" max="14340" width="64.42578125" style="61" customWidth="1"/>
+    <col min="14341" max="14342" width="28.85546875" style="61" customWidth="1"/>
+    <col min="14343" max="14344" width="9.140625" style="61"/>
+    <col min="14345" max="14345" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14346" max="14346" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14347" max="14347" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="14348" max="14348" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14349" max="14349" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="14350" max="14592" width="9.140625" style="61"/>
+    <col min="14593" max="14593" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="14595" max="14595" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14596" max="14596" width="64.42578125" style="61" customWidth="1"/>
+    <col min="14597" max="14598" width="28.85546875" style="61" customWidth="1"/>
+    <col min="14599" max="14600" width="9.140625" style="61"/>
+    <col min="14601" max="14601" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14602" max="14602" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14603" max="14603" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="14604" max="14604" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14605" max="14605" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="14606" max="14848" width="9.140625" style="61"/>
+    <col min="14849" max="14849" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="14851" max="14851" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14852" max="14852" width="64.42578125" style="61" customWidth="1"/>
+    <col min="14853" max="14854" width="28.85546875" style="61" customWidth="1"/>
+    <col min="14855" max="14856" width="9.140625" style="61"/>
+    <col min="14857" max="14857" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14858" max="14858" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14859" max="14859" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="14860" max="14860" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14861" max="14861" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="14862" max="15104" width="9.140625" style="61"/>
+    <col min="15105" max="15105" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="15107" max="15107" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15108" max="15108" width="64.42578125" style="61" customWidth="1"/>
+    <col min="15109" max="15110" width="28.85546875" style="61" customWidth="1"/>
+    <col min="15111" max="15112" width="9.140625" style="61"/>
+    <col min="15113" max="15113" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15114" max="15114" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15115" max="15115" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="15116" max="15116" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15117" max="15117" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="15118" max="15360" width="9.140625" style="61"/>
+    <col min="15361" max="15361" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="15363" max="15363" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15364" max="15364" width="64.42578125" style="61" customWidth="1"/>
+    <col min="15365" max="15366" width="28.85546875" style="61" customWidth="1"/>
+    <col min="15367" max="15368" width="9.140625" style="61"/>
+    <col min="15369" max="15369" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15370" max="15370" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15371" max="15371" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="15372" max="15372" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15373" max="15373" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="15374" max="15616" width="9.140625" style="61"/>
+    <col min="15617" max="15617" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="15619" max="15619" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15620" max="15620" width="64.42578125" style="61" customWidth="1"/>
+    <col min="15621" max="15622" width="28.85546875" style="61" customWidth="1"/>
+    <col min="15623" max="15624" width="9.140625" style="61"/>
+    <col min="15625" max="15625" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15626" max="15626" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15627" max="15627" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="15628" max="15628" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15629" max="15629" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="15630" max="15872" width="9.140625" style="61"/>
+    <col min="15873" max="15873" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="15875" max="15875" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15876" max="15876" width="64.42578125" style="61" customWidth="1"/>
+    <col min="15877" max="15878" width="28.85546875" style="61" customWidth="1"/>
+    <col min="15879" max="15880" width="9.140625" style="61"/>
+    <col min="15881" max="15881" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15882" max="15882" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15883" max="15883" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="15884" max="15884" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15885" max="15885" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="15886" max="16128" width="9.140625" style="61"/>
+    <col min="16129" max="16129" width="22.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="16.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="16131" max="16131" width="64.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="16132" max="16132" width="64.42578125" style="61" customWidth="1"/>
+    <col min="16133" max="16134" width="28.85546875" style="61" customWidth="1"/>
+    <col min="16135" max="16136" width="9.140625" style="61"/>
+    <col min="16137" max="16137" width="11.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="16138" max="16138" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="16139" max="16139" width="9.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="16140" max="16140" width="10.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="16141" max="16141" width="34.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="16142" max="16384" width="9.140625" style="61"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" s="65" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>224</v>
+      </c>
+      <c r="G1" s="65" t="s">
+        <v>223</v>
+      </c>
+      <c r="H1" s="65" t="s">
+        <v>222</v>
+      </c>
+      <c r="I1" s="65" t="s">
+        <v>221</v>
+      </c>
+      <c r="J1" s="65" t="s">
+        <v>219</v>
+      </c>
+      <c r="K1" s="65" t="s">
+        <v>220</v>
+      </c>
+      <c r="L1" s="65" t="s">
+        <v>218</v>
+      </c>
+      <c r="M1" s="65" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="65" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="65" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="65" t="s">
+        <v>215</v>
+      </c>
+      <c r="B3" s="65" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="65" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" s="65" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="65" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="65" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="65" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" s="65" t="s">
+        <v>211</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="65" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="65" t="s">
+        <v>209</v>
+      </c>
+      <c r="C6" s="65" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>206</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>206</v>
+      </c>
+      <c r="G7" s="65" t="s">
+        <v>205</v>
+      </c>
+      <c r="M7" s="61" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="D8" s="65" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="65" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" s="65" t="s">
+        <v>200</v>
+      </c>
+      <c r="C10" s="65" t="s">
+        <v>199</v>
+      </c>
+      <c r="D10" s="65" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="65" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="C11" s="65" t="s">
+        <v>195</v>
+      </c>
+      <c r="D11" s="65" t="s">
+        <v>194</v>
+      </c>
+      <c r="M11" s="61" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="65" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="65" t="s">
+        <v>336</v>
+      </c>
+      <c r="H12" s="65" t="s">
+        <v>192</v>
+      </c>
+      <c r="M12" s="61" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="65" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="65" t="s">
+        <v>190</v>
+      </c>
+      <c r="I13" s="65" t="s">
+        <v>133</v>
+      </c>
+      <c r="K13" s="61" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" s="65" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="52" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="52" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" s="52" t="s">
+        <v>335</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>183</v>
+      </c>
+      <c r="F15" s="52" t="s">
+        <v>334</v>
+      </c>
+      <c r="G15" s="59"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="52" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="52" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="H16" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="L16" s="52" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="52" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="52" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>176</v>
+      </c>
+      <c r="D17" s="52" t="s">
+        <v>175</v>
+      </c>
+      <c r="H17" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+    </row>
+    <row r="18" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+    </row>
+    <row r="19" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="B19" s="65" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19" s="65" t="s">
+        <v>172</v>
+      </c>
+      <c r="D19" s="65" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+    </row>
+    <row r="20" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="D20" s="65" t="s">
+        <v>168</v>
+      </c>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+    </row>
+    <row r="21" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="65" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" s="65" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21" s="65" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" s="65" t="s">
+        <v>331</v>
+      </c>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="H21" s="65" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="65" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="65" t="s">
+        <v>314</v>
+      </c>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="H22" s="65" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+    </row>
+    <row r="24" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="B24" s="65" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24" s="65" t="s">
+        <v>330</v>
+      </c>
+      <c r="D24" s="65" t="s">
+        <v>329</v>
+      </c>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="H24" s="65" t="s">
+        <v>147</v>
+      </c>
+      <c r="M24" s="64" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="65" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C25" s="65" t="s">
+        <v>1390</v>
+      </c>
+      <c r="D25" s="65" t="s">
+        <v>1391</v>
+      </c>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="I25" s="65" t="s">
+        <v>133</v>
+      </c>
+      <c r="K25" s="64" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+    </row>
+    <row r="27" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="B27" s="65" t="s">
+        <v>150</v>
+      </c>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="J27" s="65" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="B28" s="65" t="s">
+        <v>327</v>
+      </c>
+      <c r="C28" s="65" t="s">
+        <v>1392</v>
+      </c>
+      <c r="D28" s="65" t="s">
+        <v>326</v>
+      </c>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="H28" s="65" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="65" t="s">
+        <v>325</v>
+      </c>
+      <c r="C29" s="65" t="s">
+        <v>324</v>
+      </c>
+      <c r="D29" s="65" t="s">
+        <v>323</v>
+      </c>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="K29" s="65" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="65" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="65" t="s">
+        <v>144</v>
+      </c>
+      <c r="D30" s="65" t="s">
+        <v>143</v>
+      </c>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+    </row>
+    <row r="31" spans="1:13" s="64" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="65" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="65" t="s">
+        <v>322</v>
+      </c>
+      <c r="E31" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="F31" s="58" t="s">
+        <v>321</v>
+      </c>
+      <c r="K31" s="65" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="65" t="s">
+        <v>137</v>
+      </c>
+      <c r="C32" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32" s="65" t="s">
+        <v>319</v>
+      </c>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="H32" s="65" t="s">
+        <v>134</v>
+      </c>
+      <c r="I32" s="65" t="s">
+        <v>133</v>
+      </c>
+      <c r="K32" s="65" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="E33" s="52"/>
+      <c r="F33" s="52"/>
+    </row>
+    <row r="34" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="B34" s="65" t="s">
+        <v>317</v>
+      </c>
+      <c r="C34" s="65" t="s">
+        <v>1393</v>
+      </c>
+      <c r="D34" s="65" t="s">
+        <v>1394</v>
+      </c>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="H34" s="65" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="65" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B35" s="65" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C35" s="65" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D35" s="65" t="s">
+        <v>1399</v>
+      </c>
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="M35" s="64" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="65" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C36" s="65" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D36" s="65" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="H36" s="65" t="s">
+        <v>1404</v>
+      </c>
+      <c r="I36" s="65" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="65" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B37" s="65" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C37" s="65" t="s">
+        <v>1407</v>
+      </c>
+      <c r="D37" s="65" t="s">
+        <v>1408</v>
+      </c>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="H37" s="65" t="s">
+        <v>1404</v>
+      </c>
+      <c r="M37" s="64" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="65" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B38" s="65" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C38" s="65" t="s">
+        <v>1412</v>
+      </c>
+      <c r="D38" s="65" t="s">
+        <v>1413</v>
+      </c>
+      <c r="E38" s="52"/>
+      <c r="F38" s="52"/>
+      <c r="H38" s="65" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="65" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C39" s="65" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D39" s="65" t="s">
+        <v>314</v>
+      </c>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="H39" s="65" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" s="52"/>
+      <c r="F40" s="52"/>
+    </row>
+    <row r="41" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41" s="65" t="s">
+        <v>316</v>
+      </c>
+      <c r="C41" s="65" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D41" s="65" t="s">
+        <v>1419</v>
+      </c>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+      <c r="H41" s="65" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="65" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B42" s="65" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C42" s="65" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D42" s="65" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="M42" s="64" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="65" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C43" s="65" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D43" s="65" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+      <c r="H43" s="65" t="s">
+        <v>1425</v>
+      </c>
+      <c r="I43" s="65" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="65" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B44" s="65" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C44" s="65" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D44" s="65" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+      <c r="H44" s="65" t="s">
+        <v>1425</v>
+      </c>
+      <c r="M44" s="64" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="65" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B45" s="65" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C45" s="65" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D45" s="65" t="s">
+        <v>1434</v>
+      </c>
+      <c r="E45" s="52"/>
+      <c r="F45" s="52"/>
+      <c r="H45" s="65" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="65" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C46" s="65" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D46" s="65" t="s">
+        <v>314</v>
+      </c>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+      <c r="H46" s="65" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="E47" s="52"/>
+      <c r="F47" s="52"/>
+    </row>
+    <row r="48" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="B48" s="65" t="s">
+        <v>315</v>
+      </c>
+      <c r="C48" s="65" t="s">
+        <v>1438</v>
+      </c>
+      <c r="D48" s="65" t="s">
+        <v>1439</v>
+      </c>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+      <c r="H48" s="65" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="65" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B49" s="65" t="s">
+        <v>1440</v>
+      </c>
+      <c r="C49" s="65" t="s">
+        <v>1441</v>
+      </c>
+      <c r="D49" s="65" t="s">
+        <v>1442</v>
+      </c>
+      <c r="E49" s="52"/>
+      <c r="F49" s="52"/>
+      <c r="M49" s="64" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="65" t="s">
+        <v>1444</v>
+      </c>
+      <c r="C50" s="65" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D50" s="65" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E50" s="52"/>
+      <c r="F50" s="52"/>
+      <c r="H50" s="65" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I50" s="65" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="65" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C51" s="65" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D51" s="65" t="s">
+        <v>1448</v>
+      </c>
+      <c r="E51" s="52"/>
+      <c r="F51" s="52"/>
+      <c r="H51" s="65" t="s">
+        <v>1445</v>
+      </c>
+      <c r="M51" s="64" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="65" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B52" s="65" t="s">
+        <v>1450</v>
+      </c>
+      <c r="C52" s="65" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D52" s="65" t="s">
+        <v>1452</v>
+      </c>
+      <c r="E52" s="52"/>
+      <c r="F52" s="52"/>
+      <c r="H52" s="65" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53" s="65" t="s">
+        <v>1454</v>
+      </c>
+      <c r="C53" s="65" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D53" s="65" t="s">
+        <v>314</v>
+      </c>
+      <c r="E53" s="52"/>
+      <c r="F53" s="52"/>
+      <c r="H53" s="65" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="E54" s="52"/>
+      <c r="F54" s="52"/>
+    </row>
+    <row r="55" spans="1:13" s="64" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A55" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="B55" s="65" t="s">
+        <v>313</v>
+      </c>
+      <c r="C55" s="65" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D55" s="58" t="s">
+        <v>1457</v>
+      </c>
+      <c r="E55" s="52"/>
+      <c r="F55" s="52"/>
+      <c r="H55" s="65" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="65" t="s">
+        <v>312</v>
+      </c>
+      <c r="B56" s="65" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C56" s="65" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D56" s="58" t="s">
+        <v>1460</v>
+      </c>
+      <c r="E56" s="52"/>
+      <c r="F56" s="52"/>
+      <c r="M56" s="64" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57" s="65" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C57" s="65" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D57" s="65" t="s">
+        <v>1464</v>
+      </c>
+      <c r="E57" s="52"/>
+      <c r="F57" s="52"/>
+      <c r="H57" s="65" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="E58" s="52"/>
+      <c r="F58" s="52"/>
+    </row>
+    <row r="59" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" s="52"/>
+      <c r="F59" s="52"/>
+    </row>
+    <row r="60" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="65"/>
+      <c r="B60" s="65"/>
+      <c r="E60" s="52"/>
+      <c r="F60" s="52"/>
+      <c r="L60" s="65"/>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;P</oddHeader>
+    <oddFooter>&amp;F</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:E76"/>
+  <sheetViews>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="K85" sqref="K85"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="4" max="256" width="9.140625" style="61"/>
+    <col min="257" max="257" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="260" max="512" width="9.140625" style="61"/>
+    <col min="513" max="513" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="515" max="515" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="516" max="768" width="9.140625" style="61"/>
+    <col min="769" max="769" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="771" max="771" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="772" max="1024" width="9.140625" style="61"/>
+    <col min="1025" max="1025" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1027" max="1027" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="1028" max="1280" width="9.140625" style="61"/>
+    <col min="1281" max="1281" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1283" max="1283" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="1284" max="1536" width="9.140625" style="61"/>
+    <col min="1537" max="1537" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1539" max="1539" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="1540" max="1792" width="9.140625" style="61"/>
+    <col min="1793" max="1793" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1795" max="1795" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="1796" max="2048" width="9.140625" style="61"/>
+    <col min="2049" max="2049" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2051" max="2051" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="2052" max="2304" width="9.140625" style="61"/>
+    <col min="2305" max="2305" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2307" max="2307" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="2308" max="2560" width="9.140625" style="61"/>
+    <col min="2561" max="2561" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2563" max="2563" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="2564" max="2816" width="9.140625" style="61"/>
+    <col min="2817" max="2817" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="2819" max="2819" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="2820" max="3072" width="9.140625" style="61"/>
+    <col min="3073" max="3073" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3075" max="3075" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="3076" max="3328" width="9.140625" style="61"/>
+    <col min="3329" max="3329" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3331" max="3331" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="3332" max="3584" width="9.140625" style="61"/>
+    <col min="3585" max="3585" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3587" max="3587" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="3588" max="3840" width="9.140625" style="61"/>
+    <col min="3841" max="3841" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3843" max="3843" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="3844" max="4096" width="9.140625" style="61"/>
+    <col min="4097" max="4097" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4099" max="4099" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="4100" max="4352" width="9.140625" style="61"/>
+    <col min="4353" max="4353" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4355" max="4355" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="4356" max="4608" width="9.140625" style="61"/>
+    <col min="4609" max="4609" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4611" max="4611" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="4612" max="4864" width="9.140625" style="61"/>
+    <col min="4865" max="4865" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4867" max="4867" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="4868" max="5120" width="9.140625" style="61"/>
+    <col min="5121" max="5121" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5123" max="5123" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="5124" max="5376" width="9.140625" style="61"/>
+    <col min="5377" max="5377" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5379" max="5379" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="5380" max="5632" width="9.140625" style="61"/>
+    <col min="5633" max="5633" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5635" max="5635" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="5636" max="5888" width="9.140625" style="61"/>
+    <col min="5889" max="5889" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="5891" max="5891" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="5892" max="6144" width="9.140625" style="61"/>
+    <col min="6145" max="6145" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6147" max="6147" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="6148" max="6400" width="9.140625" style="61"/>
+    <col min="6401" max="6401" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6403" max="6403" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="6404" max="6656" width="9.140625" style="61"/>
+    <col min="6657" max="6657" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6659" max="6659" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="6660" max="6912" width="9.140625" style="61"/>
+    <col min="6913" max="6913" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6915" max="6915" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="6916" max="7168" width="9.140625" style="61"/>
+    <col min="7169" max="7169" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7171" max="7171" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="7172" max="7424" width="9.140625" style="61"/>
+    <col min="7425" max="7425" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7427" max="7427" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="7428" max="7680" width="9.140625" style="61"/>
+    <col min="7681" max="7681" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7683" max="7683" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="7684" max="7936" width="9.140625" style="61"/>
+    <col min="7937" max="7937" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7939" max="7939" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="7940" max="8192" width="9.140625" style="61"/>
+    <col min="8193" max="8193" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8195" max="8195" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="8196" max="8448" width="9.140625" style="61"/>
+    <col min="8449" max="8449" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8451" max="8451" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="8452" max="8704" width="9.140625" style="61"/>
+    <col min="8705" max="8705" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8707" max="8707" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="8708" max="8960" width="9.140625" style="61"/>
+    <col min="8961" max="8961" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8963" max="8963" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="8964" max="9216" width="9.140625" style="61"/>
+    <col min="9217" max="9217" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9219" max="9219" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="9220" max="9472" width="9.140625" style="61"/>
+    <col min="9473" max="9473" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9475" max="9475" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="9476" max="9728" width="9.140625" style="61"/>
+    <col min="9729" max="9729" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9731" max="9731" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="9732" max="9984" width="9.140625" style="61"/>
+    <col min="9985" max="9985" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9987" max="9987" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="9988" max="10240" width="9.140625" style="61"/>
+    <col min="10241" max="10241" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10243" max="10243" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="10244" max="10496" width="9.140625" style="61"/>
+    <col min="10497" max="10497" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10499" max="10499" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="10500" max="10752" width="9.140625" style="61"/>
+    <col min="10753" max="10753" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10755" max="10755" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="10756" max="11008" width="9.140625" style="61"/>
+    <col min="11009" max="11009" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11011" max="11011" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="11012" max="11264" width="9.140625" style="61"/>
+    <col min="11265" max="11265" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11267" max="11267" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="11268" max="11520" width="9.140625" style="61"/>
+    <col min="11521" max="11521" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11523" max="11523" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="11524" max="11776" width="9.140625" style="61"/>
+    <col min="11777" max="11777" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11779" max="11779" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="11780" max="12032" width="9.140625" style="61"/>
+    <col min="12033" max="12033" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12035" max="12035" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="12036" max="12288" width="9.140625" style="61"/>
+    <col min="12289" max="12289" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12291" max="12291" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="12292" max="12544" width="9.140625" style="61"/>
+    <col min="12545" max="12545" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12547" max="12547" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="12548" max="12800" width="9.140625" style="61"/>
+    <col min="12801" max="12801" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12803" max="12803" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="12804" max="13056" width="9.140625" style="61"/>
+    <col min="13057" max="13057" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13059" max="13059" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="13060" max="13312" width="9.140625" style="61"/>
+    <col min="13313" max="13313" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13315" max="13315" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="13316" max="13568" width="9.140625" style="61"/>
+    <col min="13569" max="13569" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13571" max="13571" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="13572" max="13824" width="9.140625" style="61"/>
+    <col min="13825" max="13825" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="13827" max="13827" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="13828" max="14080" width="9.140625" style="61"/>
+    <col min="14081" max="14081" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14083" max="14083" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="14084" max="14336" width="9.140625" style="61"/>
+    <col min="14337" max="14337" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14339" max="14339" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="14340" max="14592" width="9.140625" style="61"/>
+    <col min="14593" max="14593" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14595" max="14595" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="14596" max="14848" width="9.140625" style="61"/>
+    <col min="14849" max="14849" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14851" max="14851" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="14852" max="15104" width="9.140625" style="61"/>
+    <col min="15105" max="15105" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15107" max="15107" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="15108" max="15360" width="9.140625" style="61"/>
+    <col min="15361" max="15361" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15363" max="15363" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="15364" max="15616" width="9.140625" style="61"/>
+    <col min="15617" max="15617" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15619" max="15619" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="15620" max="15872" width="9.140625" style="61"/>
+    <col min="15873" max="15873" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15875" max="15875" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="15876" max="16128" width="9.140625" style="61"/>
+    <col min="16129" max="16129" width="12.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="16.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="16131" max="16131" width="47" style="61" bestFit="1" customWidth="1"/>
+    <col min="16132" max="16384" width="9.140625" style="61"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="65" t="s">
+        <v>306</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" s="64" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>304</v>
+      </c>
+      <c r="D2" s="65" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="65" t="s">
+        <v>303</v>
+      </c>
+      <c r="C3" s="65" t="s">
+        <v>302</v>
+      </c>
+      <c r="D3" s="65" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="65" t="s">
+        <v>301</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>300</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="65" t="s">
+        <v>299</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>298</v>
+      </c>
+      <c r="D5" s="65" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="65" t="s">
+        <v>297</v>
+      </c>
+      <c r="C6" s="65" t="s">
+        <v>296</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="65" t="s">
+        <v>295</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="65" t="s">
+        <v>293</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>292</v>
+      </c>
+      <c r="D8" s="65" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="65" t="s">
+        <v>291</v>
+      </c>
+      <c r="C9" s="65" t="s">
+        <v>290</v>
+      </c>
+      <c r="D9" s="65" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="65" t="s">
+        <v>289</v>
+      </c>
+      <c r="C10" s="65" t="s">
+        <v>288</v>
+      </c>
+      <c r="D10" s="65" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="65" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="65" t="s">
+        <v>286</v>
+      </c>
+      <c r="D11" s="65" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="65" t="s">
+        <v>233</v>
+      </c>
+      <c r="C12" s="65" t="s">
+        <v>233</v>
+      </c>
+      <c r="D12" s="64" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="65"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="64"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="65" t="s">
+        <v>283</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>285</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="64" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="65" t="s">
+        <v>283</v>
+      </c>
+      <c r="B15" s="65" t="s">
+        <v>282</v>
+      </c>
+      <c r="C15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="64" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="65"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="64"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="65" t="s">
+        <v>271</v>
+      </c>
+      <c r="B17" s="65" t="s">
+        <v>280</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>279</v>
+      </c>
+      <c r="D17" s="64" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="65" t="s">
+        <v>271</v>
+      </c>
+      <c r="B18" s="65" t="s">
+        <v>277</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>276</v>
+      </c>
+      <c r="D18" s="64" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="65" t="s">
+        <v>271</v>
+      </c>
+      <c r="B19" s="65" t="s">
+        <v>274</v>
+      </c>
+      <c r="C19" s="65" t="s">
+        <v>273</v>
+      </c>
+      <c r="D19" s="61" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="65" t="s">
+        <v>271</v>
+      </c>
+      <c r="B20" s="65" t="s">
+        <v>233</v>
+      </c>
+      <c r="C20" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="64" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="65"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="64"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="65" t="s">
+        <v>270</v>
+      </c>
+      <c r="C22" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="64" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="65" t="s">
+        <v>268</v>
+      </c>
+      <c r="C23" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="64" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="65"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="64"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="65" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B25" s="65" t="s">
+        <v>282</v>
+      </c>
+      <c r="C25" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="64" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="65" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B26" s="65" t="s">
+        <v>1467</v>
+      </c>
+      <c r="C26" s="65" t="s">
+        <v>1468</v>
+      </c>
+      <c r="D26" s="64" t="s">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="65" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B27" s="65" t="s">
+        <v>1470</v>
+      </c>
+      <c r="C27" s="65" t="s">
+        <v>1471</v>
+      </c>
+      <c r="D27" s="64" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="65" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B28" s="65" t="s">
+        <v>245</v>
+      </c>
+      <c r="C28" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="64" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="65" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B29" s="65" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C29" s="65" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D29" s="64" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="65"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="64"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="65" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B31" s="65" t="s">
+        <v>1477</v>
+      </c>
+      <c r="C31" s="65" t="s">
+        <v>1478</v>
+      </c>
+      <c r="D31" s="64" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="65" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B32" s="65" t="s">
+        <v>365</v>
+      </c>
+      <c r="C32" s="65" t="s">
+        <v>1480</v>
+      </c>
+      <c r="D32" s="61" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="65" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B33" s="65" t="s">
+        <v>364</v>
+      </c>
+      <c r="C33" s="65" t="s">
+        <v>363</v>
+      </c>
+      <c r="D33" s="61" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="65" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B34" s="65" t="s">
+        <v>361</v>
+      </c>
+      <c r="C34" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="61" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="65" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B35" s="65" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C35" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="61" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="65" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B36" s="65" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C36" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="61" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="65" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B37" s="65" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C37" s="65" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D37" s="61" t="s">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="65" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B38" s="65" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C38" s="65" t="s">
+        <v>1488</v>
+      </c>
+      <c r="D38" s="64" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="65" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B39" s="65" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C39" s="65" t="s">
+        <v>1491</v>
+      </c>
+      <c r="D39" s="61" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="65" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B40" s="65" t="s">
+        <v>1493</v>
+      </c>
+      <c r="C40" s="65" t="s">
+        <v>1494</v>
+      </c>
+      <c r="D40" s="64" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="65"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="64"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="65" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B42" s="65" t="s">
+        <v>1497</v>
+      </c>
+      <c r="C42" s="65" t="s">
+        <v>357</v>
+      </c>
+      <c r="D42" s="61" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="65" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B43" s="65" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C43" s="65" t="s">
+        <v>1500</v>
+      </c>
+      <c r="D43" s="61" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="65" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B44" s="65" t="s">
+        <v>1502</v>
+      </c>
+      <c r="C44" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="61" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="65" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B45" s="65" t="s">
+        <v>1503</v>
+      </c>
+      <c r="C45" s="65" t="s">
+        <v>1504</v>
+      </c>
+      <c r="D45" s="61" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="65" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B46" s="65" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C46" s="65" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D46" s="61" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="65" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B47" s="65" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C47" s="65" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D47" s="61" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="65" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B48" s="65" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C48" s="65" t="s">
+        <v>1513</v>
+      </c>
+      <c r="D48" s="61" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="65" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B49" s="65" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C49" s="65" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D49" s="61" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="65" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B50" s="65" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C50" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="61" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="65" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B51" s="65" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C51" s="65" t="s">
+        <v>1494</v>
+      </c>
+      <c r="D51" s="64" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="65"/>
+      <c r="B52" s="65"/>
+      <c r="C52" s="65"/>
+      <c r="D52" s="64"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="65" t="s">
+        <v>354</v>
+      </c>
+      <c r="B53" s="65" t="s">
+        <v>282</v>
+      </c>
+      <c r="C53" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="64" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="65" t="s">
+        <v>354</v>
+      </c>
+      <c r="B54" s="65" t="s">
+        <v>285</v>
+      </c>
+      <c r="C54" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="64" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="65" t="s">
+        <v>354</v>
+      </c>
+      <c r="B55" s="65" t="s">
+        <v>245</v>
+      </c>
+      <c r="C55" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="D55" s="64" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="65" t="s">
+        <v>354</v>
+      </c>
+      <c r="B56" s="65" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C56" s="65" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D56" s="64" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="65"/>
+      <c r="B57" s="65"/>
+      <c r="C57" s="65"/>
+      <c r="D57" s="64"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="64"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="64" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B59" s="64" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C59" s="64" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D59" s="64" t="s">
+        <v>1522</v>
+      </c>
+      <c r="E59" s="64"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="64" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B60" s="64" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C60" s="64" t="s">
+        <v>1524</v>
+      </c>
+      <c r="D60" s="64" t="s">
+        <v>1524</v>
+      </c>
+      <c r="E60" s="64"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="64" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B61" s="64" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C61" s="64" t="s">
+        <v>1526</v>
+      </c>
+      <c r="D61" s="64" t="s">
+        <v>1526</v>
+      </c>
+      <c r="E61" s="64"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="64" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B62" s="64" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C62" s="64" t="s">
+        <v>1528</v>
+      </c>
+      <c r="D62" s="64" t="s">
+        <v>1528</v>
+      </c>
+      <c r="E62" s="64"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="64" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B63" s="64" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C63" s="64" t="s">
+        <v>1530</v>
+      </c>
+      <c r="D63" s="64" t="s">
+        <v>1530</v>
+      </c>
+      <c r="E63" s="64"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="64" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B64" s="64" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C64" s="64" t="s">
+        <v>1532</v>
+      </c>
+      <c r="D64" s="64" t="s">
+        <v>1532</v>
+      </c>
+      <c r="E64" s="64"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="64" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B65" s="64" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C65" s="64" t="s">
+        <v>1534</v>
+      </c>
+      <c r="D65" s="64" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E65" s="64"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="64" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B66" s="64" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C66" s="64" t="s">
+        <v>1536</v>
+      </c>
+      <c r="D66" s="64" t="s">
+        <v>1536</v>
+      </c>
+      <c r="E66" s="64"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="64" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B67" s="64" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C67" s="64" t="s">
+        <v>1538</v>
+      </c>
+      <c r="D67" s="64" t="s">
+        <v>1538</v>
+      </c>
+      <c r="E67" s="64"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="64"/>
+      <c r="B68" s="64"/>
+      <c r="C68" s="64"/>
+      <c r="D68" s="64"/>
+      <c r="E68" s="64"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="64" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B69" s="64" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C69" s="64" t="s">
+        <v>1541</v>
+      </c>
+      <c r="D69" s="64" t="s">
+        <v>1541</v>
+      </c>
+      <c r="E69" s="64"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="64" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B70" s="64" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C70" s="64" t="s">
+        <v>1543</v>
+      </c>
+      <c r="D70" s="64" t="s">
+        <v>1543</v>
+      </c>
+      <c r="E70" s="64"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="64" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B71" s="64" t="s">
+        <v>1544</v>
+      </c>
+      <c r="C71" s="64" t="s">
+        <v>1545</v>
+      </c>
+      <c r="D71" s="64" t="s">
+        <v>1545</v>
+      </c>
+      <c r="E71" s="64"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="64" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B72" s="64" t="s">
+        <v>1546</v>
+      </c>
+      <c r="C72" s="64" t="s">
+        <v>1547</v>
+      </c>
+      <c r="D72" s="64" t="s">
+        <v>1547</v>
+      </c>
+      <c r="E72" s="64"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="64" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B73" s="64" t="s">
+        <v>1548</v>
+      </c>
+      <c r="C73" s="64" t="s">
+        <v>1549</v>
+      </c>
+      <c r="D73" s="64" t="s">
+        <v>1549</v>
+      </c>
+      <c r="E73" s="64"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="64" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B74" s="64" t="s">
+        <v>1550</v>
+      </c>
+      <c r="C74" s="64" t="s">
+        <v>1551</v>
+      </c>
+      <c r="D74" s="64" t="s">
+        <v>1551</v>
+      </c>
+      <c r="E74" s="64"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="64" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B75" s="64" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C75" s="64" t="s">
+        <v>1553</v>
+      </c>
+      <c r="D75" s="64" t="s">
+        <v>1553</v>
+      </c>
+      <c r="E75" s="64"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="64" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B76" s="64" t="s">
+        <v>1554</v>
+      </c>
+      <c r="C76" s="64" t="s">
+        <v>1555</v>
+      </c>
+      <c r="D76" s="64" t="s">
+        <v>1555</v>
+      </c>
+      <c r="E76" s="64"/>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;P</oddHeader>
+    <oddFooter>&amp;F</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="61"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="65" t="s">
+        <v>999</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>310</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="65" t="s">
+        <v>374</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>373</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>372</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;P</oddHeader>
     <oddFooter>&amp;F</oddFooter>
@@ -16338,7 +19996,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P47" sqref="P47"/>
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Removed spaces and notes from EWAR tab
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-survey-dict.xlsx
+++ b/inst/extdata/MSF-survey-dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkeating\epidict\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4666BD-5EBA-41F5-BDDC-E5B61542D17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7538ED1-7850-4885-BB96-2EB54D301DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mortality" sheetId="11" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3564" uniqueCount="1855">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="1844">
   <si>
     <t>type</t>
   </si>
@@ -4951,18 +4951,6 @@
     <t>Ce signal doit-il être vérifié ?</t>
   </si>
   <si>
-    <t>discarded_note</t>
-  </si>
-  <si>
-    <t>You have triaged this signal and said it does not pose a public health threat and so no further action is required. Please explain this to the CHW</t>
-  </si>
-  <si>
-    <t>Vous avez trié ce signal et déclaré qu'il ne constitue pas une menace pour la santé publique et qu'aucune autre action n'est requise. Veuillez expliquer cela à l'ASC</t>
-  </si>
-  <si>
-    <t>${need_verif} = "0"</t>
-  </si>
-  <si>
     <t>Verificaton</t>
   </si>
   <si>
@@ -5026,18 +5014,6 @@
     <t>concat(${initials},"_", ${location_signal}, "_",${signal_type}, "_", ${date_signal})</t>
   </si>
   <si>
-    <t>event_id_show</t>
-  </si>
-  <si>
-    <t>Event ID is ${event_id}</t>
-  </si>
-  <si>
-    <t>ID de l'événement  ${event_id}</t>
-  </si>
-  <si>
-    <t>${event_status} = "1"</t>
-  </si>
-  <si>
     <t>date_assessment</t>
   </si>
   <si>
@@ -5099,15 +5075,6 @@
   </si>
   <si>
     <t>Événement en cours</t>
-  </si>
-  <si>
-    <t>case_finding</t>
-  </si>
-  <si>
-    <t>Visit around 10 households close to where the signal was identified to see if there are others affected by the same issue</t>
-  </si>
-  <si>
-    <t>Visitez une dizaine de foyers à proximité de l'endroit où le signal a été identifié pour voir s'il y a d'autres personnes touchées par le même problème</t>
   </si>
   <si>
     <t>acf_total</t>
@@ -14157,10 +14124,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF65934-6CFC-49E1-962F-A216D40F8DA6}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14445,325 +14412,344 @@
         <v>1608</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>178</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1609</v>
-      </c>
-      <c r="C20" s="67" t="s">
-        <v>1610</v>
-      </c>
-      <c r="D20" s="67" t="s">
-        <v>1611</v>
-      </c>
-      <c r="E20" t="s">
-        <v>1612</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>152</v>
-      </c>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
+        <v>160</v>
+      </c>
+      <c r="B21" t="s">
+        <v>200</v>
+      </c>
+      <c r="C21" s="67" t="s">
+        <v>1609</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1610</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1611</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C22" s="67"/>
+      <c r="A22" t="s">
+        <v>1612</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1613</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1614</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1615</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>160</v>
+        <v>1616</v>
       </c>
       <c r="B23" t="s">
-        <v>200</v>
-      </c>
-      <c r="C23" s="67" t="s">
-        <v>1613</v>
+        <v>1617</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1618</v>
       </c>
       <c r="D23" t="s">
-        <v>1614</v>
-      </c>
-      <c r="E23" t="s">
-        <v>1615</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>1616</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>1617</v>
+        <v>1620</v>
       </c>
       <c r="C24" t="s">
-        <v>1618</v>
+        <v>1621</v>
       </c>
       <c r="D24" t="s">
-        <v>1619</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>1620</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>1621</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1622</v>
+        <v>1623</v>
+      </c>
+      <c r="C25" s="67" t="s">
+        <v>1624</v>
       </c>
       <c r="D25" t="s">
-        <v>1623</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>138</v>
       </c>
       <c r="B26" t="s">
-        <v>1624</v>
+        <v>1626</v>
       </c>
       <c r="C26" t="s">
-        <v>1625</v>
+        <v>1627</v>
       </c>
       <c r="D26" t="s">
-        <v>1626</v>
+        <v>1628</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1629</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1627</v>
-      </c>
-      <c r="C27" s="67" t="s">
-        <v>1628</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1629</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>138</v>
+        <v>67</v>
       </c>
       <c r="B28" t="s">
         <v>1630</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="67" t="s">
         <v>1631</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="67" t="s">
         <v>1632</v>
       </c>
-      <c r="F28" t="s">
+    </row>
+    <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1626</v>
+      </c>
+      <c r="C29" s="67" t="s">
         <v>1633</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>178</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="D29" s="67" t="s">
         <v>1634</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1635</v>
-      </c>
-      <c r="D29" t="s">
-        <v>1636</v>
-      </c>
-      <c r="E29" t="s">
-        <v>1637</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>152</v>
+        <v>1635</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1636</v>
+      </c>
+      <c r="C30" s="67" t="s">
+        <v>1637</v>
+      </c>
+      <c r="D30" s="67" t="s">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1639</v>
+      </c>
+      <c r="C31" s="67" t="s">
+        <v>1640</v>
+      </c>
+      <c r="D31" s="67" t="s">
+        <v>1641</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1642</v>
+      </c>
+      <c r="C32" s="67" t="s">
+        <v>1643</v>
+      </c>
+      <c r="D32" s="67" t="s">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
         <v>67</v>
       </c>
-      <c r="B32" t="s">
-        <v>1638</v>
-      </c>
-      <c r="C32" s="67" t="s">
-        <v>1639</v>
-      </c>
-      <c r="D32" s="67" t="s">
-        <v>1640</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>39</v>
-      </c>
       <c r="B33" t="s">
-        <v>1630</v>
+        <v>1645</v>
       </c>
       <c r="C33" s="67" t="s">
-        <v>1641</v>
+        <v>1646</v>
       </c>
       <c r="D33" s="67" t="s">
-        <v>1642</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>1643</v>
+        <v>1596</v>
       </c>
       <c r="B34" t="s">
-        <v>1644</v>
+        <v>1648</v>
       </c>
       <c r="C34" s="67" t="s">
-        <v>1645</v>
+        <v>1649</v>
       </c>
       <c r="D34" s="67" t="s">
-        <v>1646</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>1647</v>
+        <v>1651</v>
       </c>
       <c r="C35" s="67" t="s">
-        <v>1648</v>
+        <v>1652</v>
       </c>
       <c r="D35" s="67" t="s">
-        <v>1649</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>1650</v>
+        <v>1654</v>
       </c>
       <c r="C36" s="67" t="s">
-        <v>1651</v>
+        <v>1655</v>
       </c>
       <c r="D36" s="67" t="s">
-        <v>1652</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>1656</v>
       </c>
       <c r="B37" t="s">
-        <v>1653</v>
+        <v>1657</v>
       </c>
       <c r="C37" s="67" t="s">
-        <v>1654</v>
+        <v>1658</v>
       </c>
       <c r="D37" s="67" t="s">
-        <v>1655</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1660</v>
+      </c>
+      <c r="C38" s="67" t="s">
+        <v>1661</v>
+      </c>
+      <c r="D38" s="67" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
         <v>1596</v>
       </c>
-      <c r="B38" t="s">
-        <v>1656</v>
-      </c>
-      <c r="C38" s="67" t="s">
-        <v>1657</v>
-      </c>
-      <c r="D38" s="67" t="s">
-        <v>1658</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>178</v>
-      </c>
       <c r="B39" t="s">
-        <v>1659</v>
+        <v>1663</v>
       </c>
       <c r="C39" s="67" t="s">
-        <v>1660</v>
+        <v>1664</v>
       </c>
       <c r="D39" s="67" t="s">
-        <v>1661</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>1596</v>
       </c>
       <c r="B40" t="s">
-        <v>1662</v>
+        <v>1666</v>
       </c>
       <c r="C40" s="67" t="s">
-        <v>1663</v>
+        <v>1667</v>
       </c>
       <c r="D40" s="67" t="s">
-        <v>1664</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>1596</v>
       </c>
       <c r="B41" t="s">
-        <v>1665</v>
+        <v>1669</v>
       </c>
       <c r="C41" s="67" t="s">
-        <v>1666</v>
+        <v>1670</v>
       </c>
       <c r="D41" s="67" t="s">
-        <v>1591</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>1667</v>
+        <v>1596</v>
       </c>
       <c r="B42" t="s">
-        <v>1668</v>
+        <v>1672</v>
       </c>
       <c r="C42" s="67" t="s">
-        <v>1669</v>
+        <v>1673</v>
       </c>
       <c r="D42" s="67" t="s">
-        <v>1670</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>1596</v>
       </c>
       <c r="B43" t="s">
-        <v>1671</v>
+        <v>1675</v>
       </c>
       <c r="C43" s="67" t="s">
-        <v>1672</v>
+        <v>1676</v>
       </c>
       <c r="D43" s="67" t="s">
-        <v>1673</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>1596</v>
+        <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>1674</v>
+        <v>1678</v>
       </c>
       <c r="C44" s="67" t="s">
-        <v>1675</v>
+        <v>1679</v>
       </c>
       <c r="D44" s="67" t="s">
-        <v>1676</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
@@ -14771,212 +14757,142 @@
         <v>1596</v>
       </c>
       <c r="B45" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="C45" s="67" t="s">
-        <v>1678</v>
+        <v>1682</v>
       </c>
       <c r="D45" s="67" t="s">
-        <v>1679</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>1596</v>
+        <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>1680</v>
+        <v>1684</v>
       </c>
       <c r="C46" s="67" t="s">
-        <v>1681</v>
+        <v>1685</v>
       </c>
       <c r="D46" s="67" t="s">
-        <v>1682</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>1596</v>
+        <v>1687</v>
       </c>
       <c r="B47" t="s">
-        <v>1683</v>
+        <v>1688</v>
       </c>
       <c r="C47" s="67" t="s">
-        <v>1684</v>
+        <v>1689</v>
       </c>
       <c r="D47" s="67" t="s">
-        <v>1685</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>1596</v>
+        <v>39</v>
       </c>
       <c r="B48" t="s">
-        <v>1686</v>
-      </c>
-      <c r="C48" s="67" t="s">
-        <v>1687</v>
+        <v>1626</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1691</v>
       </c>
       <c r="D48" s="67" t="s">
-        <v>1688</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>39</v>
+        <v>1596</v>
       </c>
       <c r="B49" t="s">
-        <v>1689</v>
-      </c>
-      <c r="C49" s="67" t="s">
-        <v>1690</v>
+        <v>1693</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1694</v>
       </c>
       <c r="D49" s="67" t="s">
-        <v>1691</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>1596</v>
+        <v>39</v>
       </c>
       <c r="B50" t="s">
-        <v>1692</v>
+        <v>1696</v>
       </c>
       <c r="C50" s="67" t="s">
-        <v>1693</v>
+        <v>1697</v>
       </c>
       <c r="D50" s="67" t="s">
-        <v>1694</v>
+        <v>1698</v>
+      </c>
+      <c r="E50" t="s">
+        <v>1699</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B51" t="s">
-        <v>1695</v>
-      </c>
-      <c r="C51" s="67" t="s">
-        <v>1696</v>
+        <v>1700</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1701</v>
       </c>
       <c r="D51" s="67" t="s">
-        <v>1697</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>1698</v>
+        <v>67</v>
       </c>
       <c r="B52" t="s">
-        <v>1699</v>
-      </c>
-      <c r="C52" s="67" t="s">
-        <v>1700</v>
+        <v>1703</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1704</v>
       </c>
       <c r="D52" s="67" t="s">
-        <v>1701</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1706</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1707</v>
+      </c>
+      <c r="D53" s="67" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>39</v>
       </c>
       <c r="B54" t="s">
-        <v>1630</v>
+        <v>1603</v>
       </c>
       <c r="C54" t="s">
-        <v>1702</v>
+        <v>1709</v>
       </c>
       <c r="D54" s="67" t="s">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
-        <v>1596</v>
-      </c>
-      <c r="B55" t="s">
-        <v>1704</v>
-      </c>
-      <c r="C55" t="s">
-        <v>1705</v>
-      </c>
-      <c r="D55" s="67" t="s">
-        <v>1706</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
-        <v>39</v>
-      </c>
-      <c r="B56" t="s">
-        <v>1707</v>
-      </c>
-      <c r="C56" s="67" t="s">
-        <v>1708</v>
-      </c>
-      <c r="D56" s="67" t="s">
-        <v>1709</v>
-      </c>
-      <c r="E56" t="s">
         <v>1710</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>39</v>
-      </c>
-      <c r="B57" t="s">
-        <v>1711</v>
-      </c>
-      <c r="C57" t="s">
-        <v>1712</v>
-      </c>
-      <c r="D57" s="67" t="s">
-        <v>1713</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>67</v>
-      </c>
-      <c r="B58" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C58" t="s">
-        <v>1715</v>
-      </c>
-      <c r="D58" s="67" t="s">
-        <v>1716</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>67</v>
-      </c>
-      <c r="B59" t="s">
-        <v>1717</v>
-      </c>
-      <c r="C59" t="s">
-        <v>1718</v>
-      </c>
-      <c r="D59" s="67" t="s">
-        <v>1719</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>39</v>
-      </c>
-      <c r="B60" t="s">
-        <v>1603</v>
-      </c>
-      <c r="C60" t="s">
-        <v>1720</v>
-      </c>
-      <c r="D60" s="67" t="s">
-        <v>1721</v>
       </c>
     </row>
   </sheetData>
@@ -15018,13 +14934,13 @@
         <v>887</v>
       </c>
       <c r="B2" t="s">
-        <v>1722</v>
+        <v>1711</v>
       </c>
       <c r="C2" t="s">
-        <v>1723</v>
+        <v>1712</v>
       </c>
       <c r="D2" t="s">
-        <v>1724</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -15071,10 +14987,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>1725</v>
+        <v>1714</v>
       </c>
       <c r="B6" t="s">
-        <v>1726</v>
+        <v>1715</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -15085,10 +15001,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>1725</v>
+        <v>1714</v>
       </c>
       <c r="B7" t="s">
-        <v>1727</v>
+        <v>1716</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -15099,13 +15015,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>1725</v>
+        <v>1714</v>
       </c>
       <c r="B8" t="s">
-        <v>1728</v>
+        <v>1717</v>
       </c>
       <c r="C8" t="s">
-        <v>1729</v>
+        <v>1718</v>
       </c>
       <c r="D8" t="s">
         <v>243</v>
@@ -15116,13 +15032,13 @@
         <v>954</v>
       </c>
       <c r="B9" t="s">
-        <v>1730</v>
+        <v>1719</v>
       </c>
       <c r="C9" t="s">
-        <v>1731</v>
+        <v>1720</v>
       </c>
       <c r="D9" t="s">
-        <v>1732</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
@@ -15130,13 +15046,13 @@
         <v>954</v>
       </c>
       <c r="B10" t="s">
-        <v>1733</v>
+        <v>1722</v>
       </c>
       <c r="C10" t="s">
-        <v>1734</v>
+        <v>1723</v>
       </c>
       <c r="D10" t="s">
-        <v>1735</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
@@ -15144,13 +15060,13 @@
         <v>954</v>
       </c>
       <c r="B11" t="s">
-        <v>1736</v>
+        <v>1725</v>
       </c>
       <c r="C11" t="s">
-        <v>1737</v>
+        <v>1726</v>
       </c>
       <c r="D11" t="s">
-        <v>1738</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
@@ -15158,13 +15074,13 @@
         <v>954</v>
       </c>
       <c r="B12" t="s">
-        <v>1739</v>
+        <v>1728</v>
       </c>
       <c r="C12" t="s">
-        <v>1740</v>
+        <v>1729</v>
       </c>
       <c r="D12" t="s">
-        <v>1741</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
@@ -15172,13 +15088,13 @@
         <v>954</v>
       </c>
       <c r="B13" t="s">
-        <v>1742</v>
+        <v>1731</v>
       </c>
       <c r="C13" t="s">
-        <v>1743</v>
+        <v>1732</v>
       </c>
       <c r="D13" t="s">
-        <v>1744</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
@@ -15186,97 +15102,97 @@
         <v>954</v>
       </c>
       <c r="B14" t="s">
-        <v>1745</v>
+        <v>1734</v>
       </c>
       <c r="C14" t="s">
-        <v>1746</v>
+        <v>1735</v>
       </c>
       <c r="D14" t="s">
-        <v>1747</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>1748</v>
+        <v>1737</v>
       </c>
       <c r="B15" t="s">
-        <v>1749</v>
+        <v>1738</v>
       </c>
       <c r="C15" t="s">
-        <v>1750</v>
+        <v>1739</v>
       </c>
       <c r="D15" t="s">
-        <v>1750</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>1748</v>
+        <v>1737</v>
       </c>
       <c r="B16" t="s">
-        <v>1751</v>
+        <v>1740</v>
       </c>
       <c r="C16" t="s">
-        <v>1752</v>
+        <v>1741</v>
       </c>
       <c r="D16" t="s">
-        <v>1752</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>1748</v>
+        <v>1737</v>
       </c>
       <c r="B17" t="s">
-        <v>1753</v>
+        <v>1742</v>
       </c>
       <c r="C17" t="s">
-        <v>1754</v>
+        <v>1743</v>
       </c>
       <c r="D17" t="s">
-        <v>1754</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>1748</v>
+        <v>1737</v>
       </c>
       <c r="B18" t="s">
-        <v>1755</v>
+        <v>1744</v>
       </c>
       <c r="C18" t="s">
-        <v>1756</v>
+        <v>1745</v>
       </c>
       <c r="D18" t="s">
-        <v>1756</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>1748</v>
+        <v>1737</v>
       </c>
       <c r="B19" t="s">
-        <v>1757</v>
+        <v>1746</v>
       </c>
       <c r="C19" t="s">
-        <v>1758</v>
+        <v>1747</v>
       </c>
       <c r="D19" t="s">
-        <v>1758</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
+        <v>1737</v>
+      </c>
+      <c r="B20" t="s">
         <v>1748</v>
       </c>
-      <c r="B20" t="s">
-        <v>1759</v>
-      </c>
       <c r="C20" t="s">
-        <v>1760</v>
+        <v>1749</v>
       </c>
       <c r="D20" t="s">
-        <v>1760</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
@@ -15284,13 +15200,13 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>1761</v>
+        <v>1750</v>
       </c>
       <c r="C21" t="s">
-        <v>1762</v>
+        <v>1751</v>
       </c>
       <c r="D21" t="s">
-        <v>1762</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
@@ -15298,13 +15214,13 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>1763</v>
+        <v>1752</v>
       </c>
       <c r="C22" t="s">
-        <v>1764</v>
+        <v>1753</v>
       </c>
       <c r="D22" t="s">
-        <v>1764</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
@@ -15312,13 +15228,13 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>1765</v>
+        <v>1754</v>
       </c>
       <c r="C23" t="s">
-        <v>1766</v>
+        <v>1755</v>
       </c>
       <c r="D23" t="s">
-        <v>1766</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
@@ -15326,13 +15242,13 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>1767</v>
+        <v>1756</v>
       </c>
       <c r="C24" t="s">
-        <v>1768</v>
+        <v>1757</v>
       </c>
       <c r="D24" t="s">
-        <v>1768</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
@@ -15340,13 +15256,13 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>1769</v>
+        <v>1758</v>
       </c>
       <c r="C25" t="s">
-        <v>1770</v>
+        <v>1759</v>
       </c>
       <c r="D25" t="s">
-        <v>1770</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -15354,66 +15270,66 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>1771</v>
+        <v>1760</v>
       </c>
       <c r="C26" t="s">
-        <v>1772</v>
+        <v>1761</v>
       </c>
       <c r="D26" t="s">
-        <v>1772</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>1773</v>
+        <v>1762</v>
       </c>
       <c r="B27" t="s">
-        <v>1774</v>
+        <v>1763</v>
       </c>
       <c r="C27" t="s">
-        <v>1775</v>
+        <v>1764</v>
       </c>
       <c r="D27" t="s">
-        <v>1776</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>1773</v>
+        <v>1762</v>
       </c>
       <c r="B28" t="s">
-        <v>1777</v>
+        <v>1766</v>
       </c>
       <c r="C28" t="s">
-        <v>1778</v>
+        <v>1767</v>
       </c>
       <c r="D28" t="s">
-        <v>1779</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>1773</v>
+        <v>1762</v>
       </c>
       <c r="B29" t="s">
-        <v>1780</v>
+        <v>1769</v>
       </c>
       <c r="C29" t="s">
-        <v>1781</v>
+        <v>1770</v>
       </c>
       <c r="D29" t="s">
-        <v>1782</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>1773</v>
+        <v>1762</v>
       </c>
       <c r="B30" t="s">
         <v>233</v>
       </c>
       <c r="C30" t="s">
-        <v>1783</v>
+        <v>1772</v>
       </c>
       <c r="D30" t="s">
         <v>232</v>
@@ -15421,338 +15337,338 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>1784</v>
+        <v>1773</v>
       </c>
       <c r="B31" t="s">
-        <v>1785</v>
+        <v>1774</v>
       </c>
       <c r="C31" t="s">
-        <v>1786</v>
+        <v>1775</v>
       </c>
       <c r="D31" t="s">
-        <v>1787</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>1784</v>
+        <v>1773</v>
       </c>
       <c r="B32" t="s">
-        <v>1788</v>
+        <v>1777</v>
       </c>
       <c r="C32" t="s">
-        <v>1789</v>
+        <v>1778</v>
       </c>
       <c r="D32" t="s">
-        <v>1790</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>1784</v>
+        <v>1773</v>
       </c>
       <c r="B33" t="s">
-        <v>1791</v>
+        <v>1780</v>
       </c>
       <c r="C33" t="s">
-        <v>1792</v>
+        <v>1781</v>
       </c>
       <c r="D33" t="s">
-        <v>1793</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1783</v>
+      </c>
+      <c r="C34" t="s">
         <v>1784</v>
       </c>
-      <c r="B34" t="s">
-        <v>1794</v>
-      </c>
-      <c r="C34" t="s">
-        <v>1795</v>
-      </c>
       <c r="D34" t="s">
-        <v>1796</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>1784</v>
+        <v>1773</v>
       </c>
       <c r="B35" t="s">
-        <v>1797</v>
+        <v>1786</v>
       </c>
       <c r="C35" t="s">
-        <v>1798</v>
+        <v>1787</v>
       </c>
       <c r="D35" t="s">
-        <v>1799</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>1784</v>
+        <v>1773</v>
       </c>
       <c r="B36" t="s">
-        <v>1800</v>
+        <v>1789</v>
       </c>
       <c r="C36" t="s">
-        <v>1801</v>
+        <v>1790</v>
       </c>
       <c r="D36" t="s">
-        <v>1802</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>1803</v>
+        <v>1792</v>
       </c>
       <c r="B37" t="s">
-        <v>1804</v>
+        <v>1793</v>
       </c>
       <c r="C37" t="s">
-        <v>1805</v>
+        <v>1794</v>
       </c>
       <c r="D37" t="s">
-        <v>1805</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>1803</v>
+        <v>1792</v>
       </c>
       <c r="B38" t="s">
-        <v>1806</v>
+        <v>1795</v>
       </c>
       <c r="C38" t="s">
-        <v>1807</v>
+        <v>1796</v>
       </c>
       <c r="D38" t="s">
-        <v>1807</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>1803</v>
+        <v>1792</v>
       </c>
       <c r="B39" t="s">
-        <v>1808</v>
+        <v>1797</v>
       </c>
       <c r="C39" t="s">
-        <v>1809</v>
+        <v>1798</v>
       </c>
       <c r="D39" t="s">
-        <v>1809</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>1803</v>
+        <v>1792</v>
       </c>
       <c r="B40" t="s">
-        <v>1810</v>
+        <v>1799</v>
       </c>
       <c r="C40" t="s">
-        <v>1811</v>
+        <v>1800</v>
       </c>
       <c r="D40" t="s">
-        <v>1811</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>1803</v>
+        <v>1792</v>
       </c>
       <c r="B41" t="s">
-        <v>1812</v>
+        <v>1801</v>
       </c>
       <c r="C41" t="s">
-        <v>1813</v>
+        <v>1802</v>
       </c>
       <c r="D41" t="s">
-        <v>1813</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B42" t="s">
         <v>1803</v>
       </c>
-      <c r="B42" t="s">
-        <v>1814</v>
-      </c>
       <c r="C42" t="s">
-        <v>1815</v>
+        <v>1804</v>
       </c>
       <c r="D42" t="s">
-        <v>1815</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>1816</v>
+        <v>1805</v>
       </c>
       <c r="B43" t="s">
-        <v>1817</v>
+        <v>1806</v>
       </c>
       <c r="C43" t="s">
-        <v>1818</v>
+        <v>1807</v>
       </c>
       <c r="D43" t="s">
-        <v>1819</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>1816</v>
+        <v>1805</v>
       </c>
       <c r="B44" t="s">
-        <v>1820</v>
+        <v>1809</v>
       </c>
       <c r="C44" t="s">
-        <v>1821</v>
+        <v>1810</v>
       </c>
       <c r="D44" t="s">
-        <v>1822</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>1816</v>
+        <v>1805</v>
       </c>
       <c r="B45" t="s">
-        <v>1823</v>
+        <v>1812</v>
       </c>
       <c r="C45" t="s">
-        <v>1824</v>
+        <v>1813</v>
       </c>
       <c r="D45" t="s">
-        <v>1825</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C46" t="s">
         <v>1816</v>
       </c>
-      <c r="B46" t="s">
-        <v>1826</v>
-      </c>
-      <c r="C46" t="s">
-        <v>1827</v>
-      </c>
       <c r="D46" t="s">
-        <v>1828</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>1816</v>
+        <v>1805</v>
       </c>
       <c r="B47" t="s">
-        <v>1829</v>
+        <v>1818</v>
       </c>
       <c r="C47" t="s">
-        <v>1830</v>
+        <v>1819</v>
       </c>
       <c r="D47" t="s">
-        <v>1831</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>1816</v>
+        <v>1805</v>
       </c>
       <c r="B48" t="s">
-        <v>1832</v>
+        <v>1821</v>
       </c>
       <c r="C48" t="s">
-        <v>1833</v>
+        <v>1822</v>
       </c>
       <c r="D48" t="s">
-        <v>1834</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>1835</v>
+        <v>1824</v>
       </c>
       <c r="B49" t="s">
-        <v>1836</v>
+        <v>1825</v>
       </c>
       <c r="C49" t="s">
-        <v>1837</v>
+        <v>1826</v>
       </c>
       <c r="D49" t="s">
-        <v>1838</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>1835</v>
+        <v>1824</v>
       </c>
       <c r="B50" t="s">
-        <v>1839</v>
+        <v>1828</v>
       </c>
       <c r="C50" t="s">
-        <v>1840</v>
+        <v>1829</v>
       </c>
       <c r="D50" t="s">
-        <v>1841</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>1835</v>
+        <v>1824</v>
       </c>
       <c r="B51" t="s">
-        <v>1842</v>
+        <v>1831</v>
       </c>
       <c r="C51" t="s">
-        <v>1843</v>
+        <v>1832</v>
       </c>
       <c r="D51" t="s">
-        <v>1844</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1834</v>
+      </c>
+      <c r="C52" t="s">
         <v>1835</v>
       </c>
-      <c r="B52" t="s">
-        <v>1845</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1846</v>
-      </c>
       <c r="D52" t="s">
-        <v>1847</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>1835</v>
+        <v>1824</v>
       </c>
       <c r="B53" t="s">
-        <v>1848</v>
+        <v>1837</v>
       </c>
       <c r="C53" t="s">
-        <v>1849</v>
+        <v>1838</v>
       </c>
       <c r="D53" t="s">
-        <v>1850</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>1835</v>
+        <v>1824</v>
       </c>
       <c r="B54" t="s">
-        <v>1851</v>
+        <v>1840</v>
       </c>
       <c r="C54" t="s">
-        <v>1852</v>
+        <v>1841</v>
       </c>
       <c r="D54" t="s">
-        <v>1853</v>
+        <v>1842</v>
       </c>
     </row>
   </sheetData>
@@ -15764,7 +15680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD90C4A9-D4E0-4E63-9235-92D70EC4C6A5}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -15777,7 +15693,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="68" t="s">
-        <v>1854</v>
+        <v>1843</v>
       </c>
     </row>
   </sheetData>
@@ -20169,7 +20085,7 @@
       </c>
       <c r="I49" s="57"/>
     </row>
-    <row r="50" spans="1:12" s="3" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:12" s="3" customFormat="1" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A50" s="57" t="s">
         <v>312</v>
       </c>

</xml_diff>

<commit_message>
Updated variable names to make all unique e.g. comments becames comments_signal and comments_response
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-survey-dict.xlsx
+++ b/inst/extdata/MSF-survey-dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkeating\epidict\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7538ED1-7850-4885-BB96-2EB54D301DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B69E0A-7D3F-41CD-A8ED-3F01DB708865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="1844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="1846">
   <si>
     <t>type</t>
   </si>
@@ -4933,9 +4933,6 @@
     <t>Signal signalé précédemment</t>
   </si>
   <si>
-    <t>comments</t>
-  </si>
-  <si>
     <t>Any additional information?</t>
   </si>
   <si>
@@ -5654,6 +5651,15 @@
   </si>
   <si>
     <t>ewar</t>
+  </si>
+  <si>
+    <t>comments_signal</t>
+  </si>
+  <si>
+    <t>comments_response</t>
+  </si>
+  <si>
+    <t>event_id_res</t>
   </si>
 </sst>
 </file>
@@ -14126,8 +14132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF65934-6CFC-49E1-962F-A216D40F8DA6}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14389,13 +14395,13 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C18" t="s">
         <v>1603</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>1604</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1605</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
@@ -14403,13 +14409,13 @@
         <v>53</v>
       </c>
       <c r="B19" t="s">
+        <v>1605</v>
+      </c>
+      <c r="C19" s="67" t="s">
         <v>1606</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="D19" t="s">
         <v>1607</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1608</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -14427,41 +14433,41 @@
         <v>200</v>
       </c>
       <c r="C21" s="67" t="s">
+        <v>1608</v>
+      </c>
+      <c r="D21" t="s">
         <v>1609</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>1610</v>
-      </c>
-      <c r="E21" t="s">
-        <v>1611</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
+        <v>1611</v>
+      </c>
+      <c r="B22" t="s">
         <v>1612</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>1613</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>1614</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1615</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
+        <v>1615</v>
+      </c>
+      <c r="B23" t="s">
         <v>1616</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>1617</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>1618</v>
-      </c>
-      <c r="D23" t="s">
-        <v>1619</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -14469,13 +14475,13 @@
         <v>67</v>
       </c>
       <c r="B24" t="s">
+        <v>1619</v>
+      </c>
+      <c r="C24" t="s">
         <v>1620</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>1621</v>
-      </c>
-      <c r="D24" t="s">
-        <v>1622</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
@@ -14483,13 +14489,13 @@
         <v>53</v>
       </c>
       <c r="B25" t="s">
+        <v>1622</v>
+      </c>
+      <c r="C25" s="67" t="s">
         <v>1623</v>
       </c>
-      <c r="C25" s="67" t="s">
+      <c r="D25" t="s">
         <v>1624</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1625</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -14497,16 +14503,16 @@
         <v>138</v>
       </c>
       <c r="B26" t="s">
+        <v>1625</v>
+      </c>
+      <c r="C26" t="s">
         <v>1626</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>1627</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>1628</v>
-      </c>
-      <c r="F26" t="s">
-        <v>1629</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
@@ -14519,13 +14525,13 @@
         <v>67</v>
       </c>
       <c r="B28" t="s">
+        <v>1629</v>
+      </c>
+      <c r="C28" s="67" t="s">
         <v>1630</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="D28" s="67" t="s">
         <v>1631</v>
-      </c>
-      <c r="D28" s="67" t="s">
-        <v>1632</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
@@ -14533,27 +14539,27 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="C29" s="67" t="s">
+        <v>1632</v>
+      </c>
+      <c r="D29" s="67" t="s">
         <v>1633</v>
-      </c>
-      <c r="D29" s="67" t="s">
-        <v>1634</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
+        <v>1634</v>
+      </c>
+      <c r="B30" t="s">
         <v>1635</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" s="67" t="s">
         <v>1636</v>
       </c>
-      <c r="C30" s="67" t="s">
+      <c r="D30" s="67" t="s">
         <v>1637</v>
-      </c>
-      <c r="D30" s="67" t="s">
-        <v>1638</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -14561,13 +14567,13 @@
         <v>39</v>
       </c>
       <c r="B31" t="s">
+        <v>1638</v>
+      </c>
+      <c r="C31" s="67" t="s">
         <v>1639</v>
       </c>
-      <c r="C31" s="67" t="s">
+      <c r="D31" s="67" t="s">
         <v>1640</v>
-      </c>
-      <c r="D31" s="67" t="s">
-        <v>1641</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -14575,13 +14581,13 @@
         <v>39</v>
       </c>
       <c r="B32" t="s">
+        <v>1641</v>
+      </c>
+      <c r="C32" s="67" t="s">
         <v>1642</v>
       </c>
-      <c r="C32" s="67" t="s">
+      <c r="D32" s="67" t="s">
         <v>1643</v>
-      </c>
-      <c r="D32" s="67" t="s">
-        <v>1644</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
@@ -14589,13 +14595,13 @@
         <v>67</v>
       </c>
       <c r="B33" t="s">
+        <v>1644</v>
+      </c>
+      <c r="C33" s="67" t="s">
         <v>1645</v>
       </c>
-      <c r="C33" s="67" t="s">
+      <c r="D33" s="67" t="s">
         <v>1646</v>
-      </c>
-      <c r="D33" s="67" t="s">
-        <v>1647</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
@@ -14603,13 +14609,13 @@
         <v>1596</v>
       </c>
       <c r="B34" t="s">
+        <v>1647</v>
+      </c>
+      <c r="C34" s="67" t="s">
         <v>1648</v>
       </c>
-      <c r="C34" s="67" t="s">
+      <c r="D34" s="67" t="s">
         <v>1649</v>
-      </c>
-      <c r="D34" s="67" t="s">
-        <v>1650</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
@@ -14617,13 +14623,13 @@
         <v>49</v>
       </c>
       <c r="B35" t="s">
+        <v>1650</v>
+      </c>
+      <c r="C35" s="67" t="s">
         <v>1651</v>
       </c>
-      <c r="C35" s="67" t="s">
+      <c r="D35" s="67" t="s">
         <v>1652</v>
-      </c>
-      <c r="D35" s="67" t="s">
-        <v>1653</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
@@ -14631,10 +14637,10 @@
         <v>49</v>
       </c>
       <c r="B36" t="s">
+        <v>1653</v>
+      </c>
+      <c r="C36" s="67" t="s">
         <v>1654</v>
-      </c>
-      <c r="C36" s="67" t="s">
-        <v>1655</v>
       </c>
       <c r="D36" s="67" t="s">
         <v>1591</v>
@@ -14642,16 +14648,16 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
+        <v>1655</v>
+      </c>
+      <c r="B37" t="s">
         <v>1656</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" s="67" t="s">
         <v>1657</v>
       </c>
-      <c r="C37" s="67" t="s">
+      <c r="D37" s="67" t="s">
         <v>1658</v>
-      </c>
-      <c r="D37" s="67" t="s">
-        <v>1659</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
@@ -14659,13 +14665,13 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
+        <v>1659</v>
+      </c>
+      <c r="C38" s="67" t="s">
         <v>1660</v>
       </c>
-      <c r="C38" s="67" t="s">
+      <c r="D38" s="67" t="s">
         <v>1661</v>
-      </c>
-      <c r="D38" s="67" t="s">
-        <v>1662</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
@@ -14673,13 +14679,13 @@
         <v>1596</v>
       </c>
       <c r="B39" t="s">
+        <v>1662</v>
+      </c>
+      <c r="C39" s="67" t="s">
         <v>1663</v>
       </c>
-      <c r="C39" s="67" t="s">
+      <c r="D39" s="67" t="s">
         <v>1664</v>
-      </c>
-      <c r="D39" s="67" t="s">
-        <v>1665</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
@@ -14687,13 +14693,13 @@
         <v>1596</v>
       </c>
       <c r="B40" t="s">
+        <v>1665</v>
+      </c>
+      <c r="C40" s="67" t="s">
         <v>1666</v>
       </c>
-      <c r="C40" s="67" t="s">
+      <c r="D40" s="67" t="s">
         <v>1667</v>
-      </c>
-      <c r="D40" s="67" t="s">
-        <v>1668</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
@@ -14701,13 +14707,13 @@
         <v>1596</v>
       </c>
       <c r="B41" t="s">
+        <v>1668</v>
+      </c>
+      <c r="C41" s="67" t="s">
         <v>1669</v>
       </c>
-      <c r="C41" s="67" t="s">
+      <c r="D41" s="67" t="s">
         <v>1670</v>
-      </c>
-      <c r="D41" s="67" t="s">
-        <v>1671</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
@@ -14715,13 +14721,13 @@
         <v>1596</v>
       </c>
       <c r="B42" t="s">
+        <v>1671</v>
+      </c>
+      <c r="C42" s="67" t="s">
         <v>1672</v>
       </c>
-      <c r="C42" s="67" t="s">
+      <c r="D42" s="67" t="s">
         <v>1673</v>
-      </c>
-      <c r="D42" s="67" t="s">
-        <v>1674</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
@@ -14729,13 +14735,13 @@
         <v>1596</v>
       </c>
       <c r="B43" t="s">
+        <v>1674</v>
+      </c>
+      <c r="C43" s="67" t="s">
         <v>1675</v>
       </c>
-      <c r="C43" s="67" t="s">
+      <c r="D43" s="67" t="s">
         <v>1676</v>
-      </c>
-      <c r="D43" s="67" t="s">
-        <v>1677</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
@@ -14743,13 +14749,13 @@
         <v>39</v>
       </c>
       <c r="B44" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C44" s="67" t="s">
         <v>1678</v>
       </c>
-      <c r="C44" s="67" t="s">
+      <c r="D44" s="67" t="s">
         <v>1679</v>
-      </c>
-      <c r="D44" s="67" t="s">
-        <v>1680</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
@@ -14757,13 +14763,13 @@
         <v>1596</v>
       </c>
       <c r="B45" t="s">
+        <v>1680</v>
+      </c>
+      <c r="C45" s="67" t="s">
         <v>1681</v>
       </c>
-      <c r="C45" s="67" t="s">
+      <c r="D45" s="67" t="s">
         <v>1682</v>
-      </c>
-      <c r="D45" s="67" t="s">
-        <v>1683</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
@@ -14771,27 +14777,27 @@
         <v>53</v>
       </c>
       <c r="B46" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C46" s="67" t="s">
         <v>1684</v>
       </c>
-      <c r="C46" s="67" t="s">
+      <c r="D46" s="67" t="s">
         <v>1685</v>
-      </c>
-      <c r="D46" s="67" t="s">
-        <v>1686</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B47" t="s">
         <v>1687</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" s="67" t="s">
         <v>1688</v>
       </c>
-      <c r="C47" s="67" t="s">
+      <c r="D47" s="67" t="s">
         <v>1689</v>
-      </c>
-      <c r="D47" s="67" t="s">
-        <v>1690</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
@@ -14799,13 +14805,13 @@
         <v>39</v>
       </c>
       <c r="B48" t="s">
-        <v>1626</v>
+        <v>1845</v>
       </c>
       <c r="C48" t="s">
+        <v>1690</v>
+      </c>
+      <c r="D48" s="67" t="s">
         <v>1691</v>
-      </c>
-      <c r="D48" s="67" t="s">
-        <v>1692</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
@@ -14813,13 +14819,13 @@
         <v>1596</v>
       </c>
       <c r="B49" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C49" t="s">
         <v>1693</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" s="67" t="s">
         <v>1694</v>
-      </c>
-      <c r="D49" s="67" t="s">
-        <v>1695</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.45">
@@ -14827,16 +14833,16 @@
         <v>39</v>
       </c>
       <c r="B50" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C50" s="67" t="s">
         <v>1696</v>
       </c>
-      <c r="C50" s="67" t="s">
+      <c r="D50" s="67" t="s">
         <v>1697</v>
       </c>
-      <c r="D50" s="67" t="s">
+      <c r="E50" t="s">
         <v>1698</v>
-      </c>
-      <c r="E50" t="s">
-        <v>1699</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
@@ -14844,13 +14850,13 @@
         <v>39</v>
       </c>
       <c r="B51" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C51" t="s">
         <v>1700</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" s="67" t="s">
         <v>1701</v>
-      </c>
-      <c r="D51" s="67" t="s">
-        <v>1702</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
@@ -14858,13 +14864,13 @@
         <v>67</v>
       </c>
       <c r="B52" t="s">
+        <v>1702</v>
+      </c>
+      <c r="C52" t="s">
         <v>1703</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" s="67" t="s">
         <v>1704</v>
-      </c>
-      <c r="D52" s="67" t="s">
-        <v>1705</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
@@ -14872,13 +14878,13 @@
         <v>67</v>
       </c>
       <c r="B53" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C53" t="s">
         <v>1706</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" s="67" t="s">
         <v>1707</v>
-      </c>
-      <c r="D53" s="67" t="s">
-        <v>1708</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
@@ -14886,13 +14892,13 @@
         <v>39</v>
       </c>
       <c r="B54" t="s">
-        <v>1603</v>
+        <v>1844</v>
       </c>
       <c r="C54" t="s">
+        <v>1708</v>
+      </c>
+      <c r="D54" s="67" t="s">
         <v>1709</v>
-      </c>
-      <c r="D54" s="67" t="s">
-        <v>1710</v>
       </c>
     </row>
   </sheetData>
@@ -14934,13 +14940,13 @@
         <v>887</v>
       </c>
       <c r="B2" t="s">
+        <v>1710</v>
+      </c>
+      <c r="C2" t="s">
         <v>1711</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>1712</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1713</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -14987,10 +14993,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B6" t="s">
         <v>1714</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1715</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -15001,10 +15007,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="B7" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -15015,13 +15021,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="B8" t="s">
+        <v>1716</v>
+      </c>
+      <c r="C8" t="s">
         <v>1717</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1718</v>
       </c>
       <c r="D8" t="s">
         <v>243</v>
@@ -15032,13 +15038,13 @@
         <v>954</v>
       </c>
       <c r="B9" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C9" t="s">
         <v>1719</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>1720</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1721</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
@@ -15046,13 +15052,13 @@
         <v>954</v>
       </c>
       <c r="B10" t="s">
+        <v>1721</v>
+      </c>
+      <c r="C10" t="s">
         <v>1722</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>1723</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1724</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
@@ -15060,13 +15066,13 @@
         <v>954</v>
       </c>
       <c r="B11" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C11" t="s">
         <v>1725</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>1726</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1727</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
@@ -15074,13 +15080,13 @@
         <v>954</v>
       </c>
       <c r="B12" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C12" t="s">
         <v>1728</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>1729</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1730</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
@@ -15088,13 +15094,13 @@
         <v>954</v>
       </c>
       <c r="B13" t="s">
+        <v>1730</v>
+      </c>
+      <c r="C13" t="s">
         <v>1731</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>1732</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1733</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
@@ -15102,97 +15108,97 @@
         <v>954</v>
       </c>
       <c r="B14" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C14" t="s">
         <v>1734</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>1735</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1736</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
+        <v>1736</v>
+      </c>
+      <c r="B15" t="s">
         <v>1737</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>1738</v>
       </c>
-      <c r="C15" t="s">
-        <v>1739</v>
-      </c>
       <c r="D15" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="B16" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C16" t="s">
         <v>1740</v>
       </c>
-      <c r="C16" t="s">
-        <v>1741</v>
-      </c>
       <c r="D16" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="B17" t="s">
+        <v>1741</v>
+      </c>
+      <c r="C17" t="s">
         <v>1742</v>
       </c>
-      <c r="C17" t="s">
-        <v>1743</v>
-      </c>
       <c r="D17" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="B18" t="s">
+        <v>1743</v>
+      </c>
+      <c r="C18" t="s">
         <v>1744</v>
       </c>
-      <c r="C18" t="s">
-        <v>1745</v>
-      </c>
       <c r="D18" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="B19" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C19" t="s">
         <v>1746</v>
       </c>
-      <c r="C19" t="s">
-        <v>1747</v>
-      </c>
       <c r="D19" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="B20" t="s">
+        <v>1747</v>
+      </c>
+      <c r="C20" t="s">
         <v>1748</v>
       </c>
-      <c r="C20" t="s">
-        <v>1749</v>
-      </c>
       <c r="D20" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
@@ -15200,13 +15206,13 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C21" t="s">
         <v>1750</v>
       </c>
-      <c r="C21" t="s">
-        <v>1751</v>
-      </c>
       <c r="D21" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
@@ -15214,13 +15220,13 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
+        <v>1751</v>
+      </c>
+      <c r="C22" t="s">
         <v>1752</v>
       </c>
-      <c r="C22" t="s">
-        <v>1753</v>
-      </c>
       <c r="D22" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
@@ -15228,13 +15234,13 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
+        <v>1753</v>
+      </c>
+      <c r="C23" t="s">
         <v>1754</v>
       </c>
-      <c r="C23" t="s">
-        <v>1755</v>
-      </c>
       <c r="D23" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
@@ -15242,13 +15248,13 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
+        <v>1755</v>
+      </c>
+      <c r="C24" t="s">
         <v>1756</v>
       </c>
-      <c r="C24" t="s">
-        <v>1757</v>
-      </c>
       <c r="D24" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
@@ -15256,13 +15262,13 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
+        <v>1757</v>
+      </c>
+      <c r="C25" t="s">
         <v>1758</v>
       </c>
-      <c r="C25" t="s">
-        <v>1759</v>
-      </c>
       <c r="D25" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -15270,66 +15276,66 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
+        <v>1759</v>
+      </c>
+      <c r="C26" t="s">
         <v>1760</v>
       </c>
-      <c r="C26" t="s">
-        <v>1761</v>
-      </c>
       <c r="D26" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B27" t="s">
         <v>1762</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>1763</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>1764</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1765</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="B28" t="s">
+        <v>1765</v>
+      </c>
+      <c r="C28" t="s">
         <v>1766</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>1767</v>
-      </c>
-      <c r="D28" t="s">
-        <v>1768</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="B29" t="s">
+        <v>1768</v>
+      </c>
+      <c r="C29" t="s">
         <v>1769</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>1770</v>
-      </c>
-      <c r="D29" t="s">
-        <v>1771</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="B30" t="s">
         <v>233</v>
       </c>
       <c r="C30" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D30" t="s">
         <v>232</v>
@@ -15337,338 +15343,338 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B31" t="s">
         <v>1773</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>1774</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>1775</v>
-      </c>
-      <c r="D31" t="s">
-        <v>1776</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="B32" t="s">
+        <v>1776</v>
+      </c>
+      <c r="C32" t="s">
         <v>1777</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>1778</v>
-      </c>
-      <c r="D32" t="s">
-        <v>1779</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="B33" t="s">
+        <v>1779</v>
+      </c>
+      <c r="C33" t="s">
         <v>1780</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>1781</v>
-      </c>
-      <c r="D33" t="s">
-        <v>1782</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="B34" t="s">
+        <v>1782</v>
+      </c>
+      <c r="C34" t="s">
         <v>1783</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>1784</v>
-      </c>
-      <c r="D34" t="s">
-        <v>1785</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="B35" t="s">
+        <v>1785</v>
+      </c>
+      <c r="C35" t="s">
         <v>1786</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>1787</v>
-      </c>
-      <c r="D35" t="s">
-        <v>1788</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="B36" t="s">
+        <v>1788</v>
+      </c>
+      <c r="C36" t="s">
         <v>1789</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>1790</v>
-      </c>
-      <c r="D36" t="s">
-        <v>1791</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B37" t="s">
         <v>1792</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>1793</v>
       </c>
-      <c r="C37" t="s">
-        <v>1794</v>
-      </c>
       <c r="D37" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="B38" t="s">
+        <v>1794</v>
+      </c>
+      <c r="C38" t="s">
         <v>1795</v>
       </c>
-      <c r="C38" t="s">
-        <v>1796</v>
-      </c>
       <c r="D38" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="B39" t="s">
+        <v>1796</v>
+      </c>
+      <c r="C39" t="s">
         <v>1797</v>
       </c>
-      <c r="C39" t="s">
-        <v>1798</v>
-      </c>
       <c r="D39" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="B40" t="s">
+        <v>1798</v>
+      </c>
+      <c r="C40" t="s">
         <v>1799</v>
       </c>
-      <c r="C40" t="s">
-        <v>1800</v>
-      </c>
       <c r="D40" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="B41" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C41" t="s">
         <v>1801</v>
       </c>
-      <c r="C41" t="s">
-        <v>1802</v>
-      </c>
       <c r="D41" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="B42" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C42" t="s">
         <v>1803</v>
       </c>
-      <c r="C42" t="s">
-        <v>1804</v>
-      </c>
       <c r="D42" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B43" t="s">
         <v>1805</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>1806</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>1807</v>
-      </c>
-      <c r="D43" t="s">
-        <v>1808</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="B44" t="s">
+        <v>1808</v>
+      </c>
+      <c r="C44" t="s">
         <v>1809</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>1810</v>
-      </c>
-      <c r="D44" t="s">
-        <v>1811</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="B45" t="s">
+        <v>1811</v>
+      </c>
+      <c r="C45" t="s">
         <v>1812</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>1813</v>
-      </c>
-      <c r="D45" t="s">
-        <v>1814</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="B46" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C46" t="s">
         <v>1815</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>1816</v>
-      </c>
-      <c r="D46" t="s">
-        <v>1817</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="B47" t="s">
+        <v>1817</v>
+      </c>
+      <c r="C47" t="s">
         <v>1818</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>1819</v>
-      </c>
-      <c r="D47" t="s">
-        <v>1820</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="B48" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C48" t="s">
         <v>1821</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>1822</v>
-      </c>
-      <c r="D48" t="s">
-        <v>1823</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B49" t="s">
         <v>1824</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>1825</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>1826</v>
-      </c>
-      <c r="D49" t="s">
-        <v>1827</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="B50" t="s">
+        <v>1827</v>
+      </c>
+      <c r="C50" t="s">
         <v>1828</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>1829</v>
-      </c>
-      <c r="D50" t="s">
-        <v>1830</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="B51" t="s">
+        <v>1830</v>
+      </c>
+      <c r="C51" t="s">
         <v>1831</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>1832</v>
-      </c>
-      <c r="D51" t="s">
-        <v>1833</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="B52" t="s">
+        <v>1833</v>
+      </c>
+      <c r="C52" t="s">
         <v>1834</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>1835</v>
-      </c>
-      <c r="D52" t="s">
-        <v>1836</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="B53" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C53" t="s">
         <v>1837</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>1838</v>
-      </c>
-      <c r="D53" t="s">
-        <v>1839</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="B54" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C54" t="s">
         <v>1840</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>1841</v>
-      </c>
-      <c r="D54" t="s">
-        <v>1842</v>
       </c>
     </row>
   </sheetData>
@@ -15693,7 +15699,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="68" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made each variable name of event_id unique
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-survey-dict.xlsx
+++ b/inst/extdata/MSF-survey-dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkeating\epidict\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B69E0A-7D3F-41CD-A8ED-3F01DB708865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C613B50-CC2E-47D0-9A3E-1B4310AA7F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="1846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="1847">
   <si>
     <t>type</t>
   </si>
@@ -4999,9 +4999,6 @@
     <t>Statut de l'événement</t>
   </si>
   <si>
-    <t>event_id</t>
-  </si>
-  <si>
     <t>Event ID</t>
   </si>
   <si>
@@ -5660,6 +5657,12 @@
   </si>
   <si>
     <t>event_id_res</t>
+  </si>
+  <si>
+    <t>event_id_sig</t>
+  </si>
+  <si>
+    <t>event_id_assess</t>
   </si>
 </sst>
 </file>
@@ -14132,8 +14135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF65934-6CFC-49E1-962F-A216D40F8DA6}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14395,7 +14398,7 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="C18" t="s">
         <v>1603</v>
@@ -14503,16 +14506,16 @@
         <v>138</v>
       </c>
       <c r="B26" t="s">
+        <v>1845</v>
+      </c>
+      <c r="C26" t="s">
         <v>1625</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>1626</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>1627</v>
-      </c>
-      <c r="F26" t="s">
-        <v>1628</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
@@ -14525,13 +14528,13 @@
         <v>67</v>
       </c>
       <c r="B28" t="s">
+        <v>1628</v>
+      </c>
+      <c r="C28" s="67" t="s">
         <v>1629</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="D28" s="67" t="s">
         <v>1630</v>
-      </c>
-      <c r="D28" s="67" t="s">
-        <v>1631</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
@@ -14539,27 +14542,27 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>1625</v>
+        <v>1846</v>
       </c>
       <c r="C29" s="67" t="s">
+        <v>1631</v>
+      </c>
+      <c r="D29" s="67" t="s">
         <v>1632</v>
-      </c>
-      <c r="D29" s="67" t="s">
-        <v>1633</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B30" t="s">
         <v>1634</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" s="67" t="s">
         <v>1635</v>
       </c>
-      <c r="C30" s="67" t="s">
+      <c r="D30" s="67" t="s">
         <v>1636</v>
-      </c>
-      <c r="D30" s="67" t="s">
-        <v>1637</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -14567,13 +14570,13 @@
         <v>39</v>
       </c>
       <c r="B31" t="s">
+        <v>1637</v>
+      </c>
+      <c r="C31" s="67" t="s">
         <v>1638</v>
       </c>
-      <c r="C31" s="67" t="s">
+      <c r="D31" s="67" t="s">
         <v>1639</v>
-      </c>
-      <c r="D31" s="67" t="s">
-        <v>1640</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -14581,13 +14584,13 @@
         <v>39</v>
       </c>
       <c r="B32" t="s">
+        <v>1640</v>
+      </c>
+      <c r="C32" s="67" t="s">
         <v>1641</v>
       </c>
-      <c r="C32" s="67" t="s">
+      <c r="D32" s="67" t="s">
         <v>1642</v>
-      </c>
-      <c r="D32" s="67" t="s">
-        <v>1643</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
@@ -14595,13 +14598,13 @@
         <v>67</v>
       </c>
       <c r="B33" t="s">
+        <v>1643</v>
+      </c>
+      <c r="C33" s="67" t="s">
         <v>1644</v>
       </c>
-      <c r="C33" s="67" t="s">
+      <c r="D33" s="67" t="s">
         <v>1645</v>
-      </c>
-      <c r="D33" s="67" t="s">
-        <v>1646</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
@@ -14609,13 +14612,13 @@
         <v>1596</v>
       </c>
       <c r="B34" t="s">
+        <v>1646</v>
+      </c>
+      <c r="C34" s="67" t="s">
         <v>1647</v>
       </c>
-      <c r="C34" s="67" t="s">
+      <c r="D34" s="67" t="s">
         <v>1648</v>
-      </c>
-      <c r="D34" s="67" t="s">
-        <v>1649</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
@@ -14623,13 +14626,13 @@
         <v>49</v>
       </c>
       <c r="B35" t="s">
+        <v>1649</v>
+      </c>
+      <c r="C35" s="67" t="s">
         <v>1650</v>
       </c>
-      <c r="C35" s="67" t="s">
+      <c r="D35" s="67" t="s">
         <v>1651</v>
-      </c>
-      <c r="D35" s="67" t="s">
-        <v>1652</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
@@ -14637,10 +14640,10 @@
         <v>49</v>
       </c>
       <c r="B36" t="s">
+        <v>1652</v>
+      </c>
+      <c r="C36" s="67" t="s">
         <v>1653</v>
-      </c>
-      <c r="C36" s="67" t="s">
-        <v>1654</v>
       </c>
       <c r="D36" s="67" t="s">
         <v>1591</v>
@@ -14648,16 +14651,16 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
+        <v>1654</v>
+      </c>
+      <c r="B37" t="s">
         <v>1655</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" s="67" t="s">
         <v>1656</v>
       </c>
-      <c r="C37" s="67" t="s">
+      <c r="D37" s="67" t="s">
         <v>1657</v>
-      </c>
-      <c r="D37" s="67" t="s">
-        <v>1658</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
@@ -14665,13 +14668,13 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
+        <v>1658</v>
+      </c>
+      <c r="C38" s="67" t="s">
         <v>1659</v>
       </c>
-      <c r="C38" s="67" t="s">
+      <c r="D38" s="67" t="s">
         <v>1660</v>
-      </c>
-      <c r="D38" s="67" t="s">
-        <v>1661</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
@@ -14679,13 +14682,13 @@
         <v>1596</v>
       </c>
       <c r="B39" t="s">
+        <v>1661</v>
+      </c>
+      <c r="C39" s="67" t="s">
         <v>1662</v>
       </c>
-      <c r="C39" s="67" t="s">
+      <c r="D39" s="67" t="s">
         <v>1663</v>
-      </c>
-      <c r="D39" s="67" t="s">
-        <v>1664</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
@@ -14693,13 +14696,13 @@
         <v>1596</v>
       </c>
       <c r="B40" t="s">
+        <v>1664</v>
+      </c>
+      <c r="C40" s="67" t="s">
         <v>1665</v>
       </c>
-      <c r="C40" s="67" t="s">
+      <c r="D40" s="67" t="s">
         <v>1666</v>
-      </c>
-      <c r="D40" s="67" t="s">
-        <v>1667</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
@@ -14707,13 +14710,13 @@
         <v>1596</v>
       </c>
       <c r="B41" t="s">
+        <v>1667</v>
+      </c>
+      <c r="C41" s="67" t="s">
         <v>1668</v>
       </c>
-      <c r="C41" s="67" t="s">
+      <c r="D41" s="67" t="s">
         <v>1669</v>
-      </c>
-      <c r="D41" s="67" t="s">
-        <v>1670</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
@@ -14721,13 +14724,13 @@
         <v>1596</v>
       </c>
       <c r="B42" t="s">
+        <v>1670</v>
+      </c>
+      <c r="C42" s="67" t="s">
         <v>1671</v>
       </c>
-      <c r="C42" s="67" t="s">
+      <c r="D42" s="67" t="s">
         <v>1672</v>
-      </c>
-      <c r="D42" s="67" t="s">
-        <v>1673</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
@@ -14735,13 +14738,13 @@
         <v>1596</v>
       </c>
       <c r="B43" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C43" s="67" t="s">
         <v>1674</v>
       </c>
-      <c r="C43" s="67" t="s">
+      <c r="D43" s="67" t="s">
         <v>1675</v>
-      </c>
-      <c r="D43" s="67" t="s">
-        <v>1676</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
@@ -14749,13 +14752,13 @@
         <v>39</v>
       </c>
       <c r="B44" t="s">
+        <v>1676</v>
+      </c>
+      <c r="C44" s="67" t="s">
         <v>1677</v>
       </c>
-      <c r="C44" s="67" t="s">
+      <c r="D44" s="67" t="s">
         <v>1678</v>
-      </c>
-      <c r="D44" s="67" t="s">
-        <v>1679</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
@@ -14763,13 +14766,13 @@
         <v>1596</v>
       </c>
       <c r="B45" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C45" s="67" t="s">
         <v>1680</v>
       </c>
-      <c r="C45" s="67" t="s">
+      <c r="D45" s="67" t="s">
         <v>1681</v>
-      </c>
-      <c r="D45" s="67" t="s">
-        <v>1682</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
@@ -14777,27 +14780,27 @@
         <v>53</v>
       </c>
       <c r="B46" t="s">
+        <v>1682</v>
+      </c>
+      <c r="C46" s="67" t="s">
         <v>1683</v>
       </c>
-      <c r="C46" s="67" t="s">
+      <c r="D46" s="67" t="s">
         <v>1684</v>
-      </c>
-      <c r="D46" s="67" t="s">
-        <v>1685</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B47" t="s">
         <v>1686</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" s="67" t="s">
         <v>1687</v>
       </c>
-      <c r="C47" s="67" t="s">
+      <c r="D47" s="67" t="s">
         <v>1688</v>
-      </c>
-      <c r="D47" s="67" t="s">
-        <v>1689</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
@@ -14805,13 +14808,13 @@
         <v>39</v>
       </c>
       <c r="B48" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="C48" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D48" s="67" t="s">
         <v>1690</v>
-      </c>
-      <c r="D48" s="67" t="s">
-        <v>1691</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
@@ -14819,13 +14822,13 @@
         <v>1596</v>
       </c>
       <c r="B49" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C49" t="s">
         <v>1692</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" s="67" t="s">
         <v>1693</v>
-      </c>
-      <c r="D49" s="67" t="s">
-        <v>1694</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.45">
@@ -14833,16 +14836,16 @@
         <v>39</v>
       </c>
       <c r="B50" t="s">
+        <v>1694</v>
+      </c>
+      <c r="C50" s="67" t="s">
         <v>1695</v>
       </c>
-      <c r="C50" s="67" t="s">
+      <c r="D50" s="67" t="s">
         <v>1696</v>
       </c>
-      <c r="D50" s="67" t="s">
+      <c r="E50" t="s">
         <v>1697</v>
-      </c>
-      <c r="E50" t="s">
-        <v>1698</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
@@ -14850,13 +14853,13 @@
         <v>39</v>
       </c>
       <c r="B51" t="s">
+        <v>1698</v>
+      </c>
+      <c r="C51" t="s">
         <v>1699</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" s="67" t="s">
         <v>1700</v>
-      </c>
-      <c r="D51" s="67" t="s">
-        <v>1701</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
@@ -14864,13 +14867,13 @@
         <v>67</v>
       </c>
       <c r="B52" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C52" t="s">
         <v>1702</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" s="67" t="s">
         <v>1703</v>
-      </c>
-      <c r="D52" s="67" t="s">
-        <v>1704</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
@@ -14878,13 +14881,13 @@
         <v>67</v>
       </c>
       <c r="B53" t="s">
+        <v>1704</v>
+      </c>
+      <c r="C53" t="s">
         <v>1705</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" s="67" t="s">
         <v>1706</v>
-      </c>
-      <c r="D53" s="67" t="s">
-        <v>1707</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
@@ -14892,13 +14895,13 @@
         <v>39</v>
       </c>
       <c r="B54" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="C54" t="s">
+        <v>1707</v>
+      </c>
+      <c r="D54" s="67" t="s">
         <v>1708</v>
-      </c>
-      <c r="D54" s="67" t="s">
-        <v>1709</v>
       </c>
     </row>
   </sheetData>
@@ -14940,13 +14943,13 @@
         <v>887</v>
       </c>
       <c r="B2" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C2" t="s">
         <v>1710</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>1711</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1712</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -14993,10 +14996,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B6" t="s">
         <v>1713</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1714</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -15007,10 +15010,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="B7" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -15021,13 +15024,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="B8" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C8" t="s">
         <v>1716</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1717</v>
       </c>
       <c r="D8" t="s">
         <v>243</v>
@@ -15038,13 +15041,13 @@
         <v>954</v>
       </c>
       <c r="B9" t="s">
+        <v>1717</v>
+      </c>
+      <c r="C9" t="s">
         <v>1718</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>1719</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1720</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
@@ -15052,13 +15055,13 @@
         <v>954</v>
       </c>
       <c r="B10" t="s">
+        <v>1720</v>
+      </c>
+      <c r="C10" t="s">
         <v>1721</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>1722</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1723</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
@@ -15066,13 +15069,13 @@
         <v>954</v>
       </c>
       <c r="B11" t="s">
+        <v>1723</v>
+      </c>
+      <c r="C11" t="s">
         <v>1724</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>1725</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1726</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
@@ -15080,13 +15083,13 @@
         <v>954</v>
       </c>
       <c r="B12" t="s">
+        <v>1726</v>
+      </c>
+      <c r="C12" t="s">
         <v>1727</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>1728</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1729</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
@@ -15094,13 +15097,13 @@
         <v>954</v>
       </c>
       <c r="B13" t="s">
+        <v>1729</v>
+      </c>
+      <c r="C13" t="s">
         <v>1730</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>1731</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1732</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
@@ -15108,97 +15111,97 @@
         <v>954</v>
       </c>
       <c r="B14" t="s">
+        <v>1732</v>
+      </c>
+      <c r="C14" t="s">
         <v>1733</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>1734</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1735</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B15" t="s">
         <v>1736</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>1737</v>
       </c>
-      <c r="C15" t="s">
-        <v>1738</v>
-      </c>
       <c r="D15" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="B16" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C16" t="s">
         <v>1739</v>
       </c>
-      <c r="C16" t="s">
-        <v>1740</v>
-      </c>
       <c r="D16" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="B17" t="s">
+        <v>1740</v>
+      </c>
+      <c r="C17" t="s">
         <v>1741</v>
       </c>
-      <c r="C17" t="s">
-        <v>1742</v>
-      </c>
       <c r="D17" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="B18" t="s">
+        <v>1742</v>
+      </c>
+      <c r="C18" t="s">
         <v>1743</v>
       </c>
-      <c r="C18" t="s">
-        <v>1744</v>
-      </c>
       <c r="D18" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="B19" t="s">
+        <v>1744</v>
+      </c>
+      <c r="C19" t="s">
         <v>1745</v>
       </c>
-      <c r="C19" t="s">
-        <v>1746</v>
-      </c>
       <c r="D19" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="B20" t="s">
+        <v>1746</v>
+      </c>
+      <c r="C20" t="s">
         <v>1747</v>
       </c>
-      <c r="C20" t="s">
-        <v>1748</v>
-      </c>
       <c r="D20" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
@@ -15206,13 +15209,13 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C21" t="s">
         <v>1749</v>
       </c>
-      <c r="C21" t="s">
-        <v>1750</v>
-      </c>
       <c r="D21" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
@@ -15220,13 +15223,13 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
+        <v>1750</v>
+      </c>
+      <c r="C22" t="s">
         <v>1751</v>
       </c>
-      <c r="C22" t="s">
-        <v>1752</v>
-      </c>
       <c r="D22" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
@@ -15234,13 +15237,13 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
+        <v>1752</v>
+      </c>
+      <c r="C23" t="s">
         <v>1753</v>
       </c>
-      <c r="C23" t="s">
-        <v>1754</v>
-      </c>
       <c r="D23" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
@@ -15248,13 +15251,13 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
+        <v>1754</v>
+      </c>
+      <c r="C24" t="s">
         <v>1755</v>
       </c>
-      <c r="C24" t="s">
-        <v>1756</v>
-      </c>
       <c r="D24" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
@@ -15262,13 +15265,13 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
+        <v>1756</v>
+      </c>
+      <c r="C25" t="s">
         <v>1757</v>
       </c>
-      <c r="C25" t="s">
-        <v>1758</v>
-      </c>
       <c r="D25" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -15276,66 +15279,66 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
+        <v>1758</v>
+      </c>
+      <c r="C26" t="s">
         <v>1759</v>
       </c>
-      <c r="C26" t="s">
-        <v>1760</v>
-      </c>
       <c r="D26" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B27" t="s">
         <v>1761</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>1762</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>1763</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1764</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="B28" t="s">
+        <v>1764</v>
+      </c>
+      <c r="C28" t="s">
         <v>1765</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>1766</v>
-      </c>
-      <c r="D28" t="s">
-        <v>1767</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="B29" t="s">
+        <v>1767</v>
+      </c>
+      <c r="C29" t="s">
         <v>1768</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>1769</v>
-      </c>
-      <c r="D29" t="s">
-        <v>1770</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="B30" t="s">
         <v>233</v>
       </c>
       <c r="C30" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D30" t="s">
         <v>232</v>
@@ -15343,338 +15346,338 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B31" t="s">
         <v>1772</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>1773</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>1774</v>
-      </c>
-      <c r="D31" t="s">
-        <v>1775</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="B32" t="s">
+        <v>1775</v>
+      </c>
+      <c r="C32" t="s">
         <v>1776</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>1777</v>
-      </c>
-      <c r="D32" t="s">
-        <v>1778</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="B33" t="s">
+        <v>1778</v>
+      </c>
+      <c r="C33" t="s">
         <v>1779</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>1780</v>
-      </c>
-      <c r="D33" t="s">
-        <v>1781</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="B34" t="s">
+        <v>1781</v>
+      </c>
+      <c r="C34" t="s">
         <v>1782</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>1783</v>
-      </c>
-      <c r="D34" t="s">
-        <v>1784</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="B35" t="s">
+        <v>1784</v>
+      </c>
+      <c r="C35" t="s">
         <v>1785</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>1786</v>
-      </c>
-      <c r="D35" t="s">
-        <v>1787</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="B36" t="s">
+        <v>1787</v>
+      </c>
+      <c r="C36" t="s">
         <v>1788</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>1789</v>
-      </c>
-      <c r="D36" t="s">
-        <v>1790</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B37" t="s">
         <v>1791</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>1792</v>
       </c>
-      <c r="C37" t="s">
-        <v>1793</v>
-      </c>
       <c r="D37" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="B38" t="s">
+        <v>1793</v>
+      </c>
+      <c r="C38" t="s">
         <v>1794</v>
       </c>
-      <c r="C38" t="s">
-        <v>1795</v>
-      </c>
       <c r="D38" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="B39" t="s">
+        <v>1795</v>
+      </c>
+      <c r="C39" t="s">
         <v>1796</v>
       </c>
-      <c r="C39" t="s">
-        <v>1797</v>
-      </c>
       <c r="D39" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="B40" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C40" t="s">
         <v>1798</v>
       </c>
-      <c r="C40" t="s">
-        <v>1799</v>
-      </c>
       <c r="D40" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="B41" t="s">
+        <v>1799</v>
+      </c>
+      <c r="C41" t="s">
         <v>1800</v>
       </c>
-      <c r="C41" t="s">
-        <v>1801</v>
-      </c>
       <c r="D41" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="B42" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C42" t="s">
         <v>1802</v>
       </c>
-      <c r="C42" t="s">
-        <v>1803</v>
-      </c>
       <c r="D42" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
+        <v>1803</v>
+      </c>
+      <c r="B43" t="s">
         <v>1804</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>1805</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>1806</v>
-      </c>
-      <c r="D43" t="s">
-        <v>1807</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="B44" t="s">
+        <v>1807</v>
+      </c>
+      <c r="C44" t="s">
         <v>1808</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>1809</v>
-      </c>
-      <c r="D44" t="s">
-        <v>1810</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="B45" t="s">
+        <v>1810</v>
+      </c>
+      <c r="C45" t="s">
         <v>1811</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>1812</v>
-      </c>
-      <c r="D45" t="s">
-        <v>1813</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="B46" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C46" t="s">
         <v>1814</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>1815</v>
-      </c>
-      <c r="D46" t="s">
-        <v>1816</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="B47" t="s">
+        <v>1816</v>
+      </c>
+      <c r="C47" t="s">
         <v>1817</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>1818</v>
-      </c>
-      <c r="D47" t="s">
-        <v>1819</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="B48" t="s">
+        <v>1819</v>
+      </c>
+      <c r="C48" t="s">
         <v>1820</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>1821</v>
-      </c>
-      <c r="D48" t="s">
-        <v>1822</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B49" t="s">
         <v>1823</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>1824</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>1825</v>
-      </c>
-      <c r="D49" t="s">
-        <v>1826</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="B50" t="s">
+        <v>1826</v>
+      </c>
+      <c r="C50" t="s">
         <v>1827</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>1828</v>
-      </c>
-      <c r="D50" t="s">
-        <v>1829</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="B51" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C51" t="s">
         <v>1830</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>1831</v>
-      </c>
-      <c r="D51" t="s">
-        <v>1832</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="B52" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C52" t="s">
         <v>1833</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>1834</v>
-      </c>
-      <c r="D52" t="s">
-        <v>1835</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="B53" t="s">
+        <v>1835</v>
+      </c>
+      <c r="C53" t="s">
         <v>1836</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>1837</v>
-      </c>
-      <c r="D53" t="s">
-        <v>1838</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="B54" t="s">
+        <v>1838</v>
+      </c>
+      <c r="C54" t="s">
         <v>1839</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>1840</v>
-      </c>
-      <c r="D54" t="s">
-        <v>1841</v>
       </c>
     </row>
   </sheetData>
@@ -15699,7 +15702,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="68" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix village options nutrition
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-survey-dict.xlsx
+++ b/inst/extdata/MSF-survey-dict.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Mortality" sheetId="11" r:id="rId1"/>
@@ -11192,7 +11192,7 @@
   </sheetPr>
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
     </sheetView>
@@ -17484,8 +17484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17652,7 +17652,7 @@
         <v>233</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>233</v>
+        <v>3</v>
       </c>
       <c r="D12" s="48" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
Add extra questions to the risk assessment forms
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-survey-dict.xlsx
+++ b/inst/extdata/MSF-survey-dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkeating\epidict\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C613B50-CC2E-47D0-9A3E-1B4310AA7F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D30502D-E414-49BB-AB3A-22FA8820FE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1837" yWindow="1837" windowWidth="15391" windowHeight="9443" firstSheet="12" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mortality" sheetId="11" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="1847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3590" uniqueCount="1873">
   <si>
     <t>type</t>
   </si>
@@ -5663,6 +5663,84 @@
   </si>
   <si>
     <t>event_id_assess</t>
+  </si>
+  <si>
+    <t>select_one hml</t>
+  </si>
+  <si>
+    <t>maximum_size</t>
+  </si>
+  <si>
+    <t>Likely maximum size of an outbreak linked with this event</t>
+  </si>
+  <si>
+    <t>Taille maximale probable d'une épidémie liée à cet événement</t>
+  </si>
+  <si>
+    <t>maximum_impact</t>
+  </si>
+  <si>
+    <t>Likely maximum impact of an outbreak linked with this event</t>
+  </si>
+  <si>
+    <t>Impact maximal probable d'une épidémie liée à cet événement</t>
+  </si>
+  <si>
+    <t>duration_outbreak</t>
+  </si>
+  <si>
+    <t>Likely duration of an outbreak linked with this event</t>
+  </si>
+  <si>
+    <t>Durée probable d'une épidémie liée à cet événement</t>
+  </si>
+  <si>
+    <t>eprep</t>
+  </si>
+  <si>
+    <t>Event included among EPREP scenarios</t>
+  </si>
+  <si>
+    <t>Événement inclus dans les scénarios EPREP</t>
+  </si>
+  <si>
+    <t>hml</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Haut</t>
+  </si>
+  <si>
+    <t>Moyen</t>
+  </si>
+  <si>
+    <t>Bas</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Années</t>
   </si>
 </sst>
 </file>
@@ -14133,10 +14211,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF65934-6CFC-49E1-962F-A216D40F8DA6}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14733,88 +14811,88 @@
         <v>1672</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>1596</v>
+        <v>1847</v>
       </c>
       <c r="B43" t="s">
-        <v>1673</v>
+        <v>1848</v>
       </c>
       <c r="C43" s="67" t="s">
-        <v>1674</v>
+        <v>1849</v>
       </c>
       <c r="D43" s="67" t="s">
-        <v>1675</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>39</v>
+        <v>1847</v>
       </c>
       <c r="B44" t="s">
-        <v>1676</v>
+        <v>1851</v>
       </c>
       <c r="C44" s="67" t="s">
-        <v>1677</v>
+        <v>1852</v>
       </c>
       <c r="D44" s="67" t="s">
-        <v>1678</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>1596</v>
+        <v>653</v>
       </c>
       <c r="B45" t="s">
-        <v>1679</v>
+        <v>1854</v>
       </c>
       <c r="C45" s="67" t="s">
-        <v>1680</v>
+        <v>1855</v>
       </c>
       <c r="D45" s="67" t="s">
-        <v>1681</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>1596</v>
       </c>
       <c r="B46" t="s">
-        <v>1682</v>
+        <v>1857</v>
       </c>
       <c r="C46" s="67" t="s">
-        <v>1683</v>
+        <v>1858</v>
       </c>
       <c r="D46" s="67" t="s">
-        <v>1684</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>1685</v>
+        <v>1596</v>
       </c>
       <c r="B47" t="s">
-        <v>1686</v>
+        <v>1673</v>
       </c>
       <c r="C47" s="67" t="s">
-        <v>1687</v>
+        <v>1674</v>
       </c>
       <c r="D47" s="67" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>39</v>
       </c>
       <c r="B48" t="s">
-        <v>1844</v>
-      </c>
-      <c r="C48" t="s">
-        <v>1689</v>
+        <v>1676</v>
+      </c>
+      <c r="C48" s="67" t="s">
+        <v>1677</v>
       </c>
       <c r="D48" s="67" t="s">
-        <v>1690</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
@@ -14822,72 +14900,69 @@
         <v>1596</v>
       </c>
       <c r="B49" t="s">
-        <v>1691</v>
-      </c>
-      <c r="C49" t="s">
-        <v>1692</v>
+        <v>1679</v>
+      </c>
+      <c r="C49" s="67" t="s">
+        <v>1680</v>
       </c>
       <c r="D49" s="67" t="s">
-        <v>1693</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>1694</v>
+        <v>1682</v>
       </c>
       <c r="C50" s="67" t="s">
-        <v>1695</v>
+        <v>1683</v>
       </c>
       <c r="D50" s="67" t="s">
-        <v>1696</v>
-      </c>
-      <c r="E50" t="s">
-        <v>1697</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1686</v>
+      </c>
+      <c r="C51" s="67" t="s">
+        <v>1687</v>
+      </c>
+      <c r="D51" s="67" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
         <v>39</v>
       </c>
-      <c r="B51" t="s">
-        <v>1698</v>
-      </c>
-      <c r="C51" t="s">
-        <v>1699</v>
-      </c>
-      <c r="D51" s="67" t="s">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
-        <v>67</v>
-      </c>
       <c r="B52" t="s">
-        <v>1701</v>
+        <v>1844</v>
       </c>
       <c r="C52" t="s">
-        <v>1702</v>
+        <v>1689</v>
       </c>
       <c r="D52" s="67" t="s">
-        <v>1703</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>1596</v>
       </c>
       <c r="B53" t="s">
-        <v>1704</v>
+        <v>1691</v>
       </c>
       <c r="C53" t="s">
-        <v>1705</v>
+        <v>1692</v>
       </c>
       <c r="D53" s="67" t="s">
-        <v>1706</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
@@ -14895,12 +14970,71 @@
         <v>39</v>
       </c>
       <c r="B54" t="s">
+        <v>1694</v>
+      </c>
+      <c r="C54" s="67" t="s">
+        <v>1695</v>
+      </c>
+      <c r="D54" s="67" t="s">
+        <v>1696</v>
+      </c>
+      <c r="E54" t="s">
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>39</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1698</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1699</v>
+      </c>
+      <c r="D55" s="67" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D56" s="67" t="s">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>67</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1704</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1705</v>
+      </c>
+      <c r="D57" s="67" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>39</v>
+      </c>
+      <c r="B58" t="s">
         <v>1843</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C58" t="s">
         <v>1707</v>
       </c>
-      <c r="D54" s="67" t="s">
+      <c r="D58" s="67" t="s">
         <v>1708</v>
       </c>
     </row>
@@ -14911,10 +15045,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04301A27-7367-4AE0-8969-ABBCAA198EF2}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -15678,6 +15812,90 @@
       </c>
       <c r="D54" t="s">
         <v>1840</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1861</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1864</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1862</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1865</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1866</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>933</v>
+      </c>
+      <c r="B58" t="s">
+        <v>901</v>
+      </c>
+      <c r="C58" t="s">
+        <v>902</v>
+      </c>
+      <c r="D58" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>933</v>
+      </c>
+      <c r="B59" t="s">
+        <v>904</v>
+      </c>
+      <c r="C59" t="s">
+        <v>905</v>
+      </c>
+      <c r="D59" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>933</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1870</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1871</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1872</v>
       </c>
     </row>
   </sheetData>
@@ -20459,7 +20677,7 @@
       <c r="K66" s="57"/>
       <c r="L66" s="57"/>
     </row>
-    <row r="67" spans="1:12" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="57" t="s">
         <v>312</v>
       </c>

</xml_diff>

<commit_message>
Changed c_signal_id to c_signal_id as cannot have a duplicate variable name
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-survey-dict.xlsx
+++ b/inst/extdata/MSF-survey-dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkeating\epidict\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82D5427-7F0A-4A23-958C-B5C75B555D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D98E4AD-1870-4543-A610-E5DFFDD38499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-195" yWindow="-195" windowWidth="29190" windowHeight="15870" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20617" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mortality" sheetId="11" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3590" uniqueCount="1872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3590" uniqueCount="1873">
   <si>
     <t>type</t>
   </si>
@@ -5738,6 +5738,9 @@
   </si>
   <si>
     <t>int(round(now() *10000)) + 1</t>
+  </si>
+  <si>
+    <t>c_signal_id2</t>
   </si>
 </sst>
 </file>
@@ -13894,8 +13897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF65934-6CFC-49E1-962F-A216D40F8DA6}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14623,7 +14626,7 @@
         <v>39</v>
       </c>
       <c r="B52" t="s">
-        <v>1869</v>
+        <v>1872</v>
       </c>
       <c r="C52" t="s">
         <v>1688</v>
@@ -20090,7 +20093,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>39</v>
       </c>

</xml_diff>